<commit_message>
Generate joinWith with appearance column of the Generator
Change the scss, to have a small padding space between each joinWith question.
Update the Generator Excel with an example of joinWith.
Make some Tests inside test_generate_widgets. Make sure to put TODOs for all remaining testing.
</commit_message>
<xml_diff>
--- a/example/demo_generator/references/Household_Travel_Generate_Survey.xlsx
+++ b/example/demo_generator/references/Household_Travel_Generate_Survey.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28922"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="493" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F12F502B-FFBC-43CF-9C06-8D61C0A4F3F7}"/>
+  <xr:revisionPtr revIDLastSave="514" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{869A8025-255C-48B7-B4C3-461505204C6E}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Widgets" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="158">
   <si>
     <t>questionName</t>
   </si>
@@ -50,13 +50,16 @@
     <t>section</t>
   </si>
   <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
     <t>parameters</t>
   </si>
   <si>
-    <t>group</t>
-  </si>
-  <si>
-    <t>path</t>
+    <t>appareance</t>
   </si>
   <si>
     <t>fr</t>
@@ -147,6 +150,9 @@
     <t>Please enter the email **or** phone number to get in contact.</t>
   </si>
   <si>
+    <t>joi</t>
+  </si>
+  <si>
     <t>contactEmail</t>
   </si>
   <si>
@@ -160,6 +166,9 @@
   </si>
   <si>
     <t>phoneNumber</t>
+  </si>
+  <si>
+    <t>join_with=${contactEmail}</t>
   </si>
   <si>
     <t>**Numéro de téléphone**
@@ -653,7 +662,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -719,7 +728,19 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1127,11 +1148,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U20"/>
+  <dimension ref="A1:V20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="G1" sqref="G1:G1048576"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -1141,27 +1162,29 @@
     <col min="1" max="1" width="19.85546875" style="9" customWidth="1"/>
     <col min="2" max="2" width="10.140625" style="9" customWidth="1"/>
     <col min="3" max="3" width="6.42578125" style="9" customWidth="1"/>
-    <col min="4" max="5" width="10.5703125" style="9" customWidth="1"/>
-    <col min="6" max="6" width="5.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17" style="9" customWidth="1"/>
-    <col min="8" max="8" width="31.28515625" style="9" customWidth="1"/>
-    <col min="9" max="9" width="31.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.7109375" style="9" customWidth="1"/>
-    <col min="11" max="11" width="13.5703125" style="9" customWidth="1"/>
-    <col min="12" max="12" width="13" style="9" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" style="9" customWidth="1"/>
-    <col min="14" max="14" width="10" style="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.42578125" style="9" customWidth="1"/>
-    <col min="17" max="17" width="14.140625" style="9" customWidth="1"/>
-    <col min="18" max="18" width="10.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.42578125" style="9" customWidth="1"/>
-    <col min="20" max="20" width="11.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.5703125" style="9" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="9"/>
+    <col min="4" max="4" width="10.5703125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17" style="9" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" style="9" customWidth="1"/>
+    <col min="8" max="8" width="21.140625" style="27" customWidth="1"/>
+    <col min="9" max="9" width="31.28515625" style="9" customWidth="1"/>
+    <col min="10" max="10" width="31.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.7109375" style="9" customWidth="1"/>
+    <col min="12" max="12" width="13.5703125" style="9" customWidth="1"/>
+    <col min="13" max="13" width="13" style="9" customWidth="1"/>
+    <col min="14" max="14" width="13.42578125" style="9" customWidth="1"/>
+    <col min="15" max="15" width="10" style="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.42578125" style="9" customWidth="1"/>
+    <col min="18" max="18" width="14.140625" style="9" customWidth="1"/>
+    <col min="19" max="19" width="10.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.42578125" style="9" customWidth="1"/>
+    <col min="21" max="21" width="11.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.5703125" style="9" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="17.25" customHeight="1">
+    <row r="1" spans="1:22" ht="17.25" customHeight="1">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1183,7 +1206,7 @@
       <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="23" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="8" t="s">
@@ -1207,7 +1230,7 @@
       <c r="O1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="P1" s="8" t="s">
         <v>15</v>
       </c>
       <c r="Q1" s="7" t="s">
@@ -1225,774 +1248,799 @@
       <c r="U1" s="7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" ht="27">
+      <c r="V1" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" ht="27">
       <c r="A2" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>24</v>
-      </c>
+      <c r="G2" s="10"/>
+      <c r="H2" s="24"/>
       <c r="I2" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="J2" s="10"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="10"/>
+      <c r="J2" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" s="10"/>
+      <c r="L2" s="13"/>
       <c r="M2" s="10"/>
       <c r="N2" s="10"/>
       <c r="O2" s="10"/>
       <c r="P2" s="10"/>
-      <c r="Q2" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="R2" s="10"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="S2" s="10"/>
       <c r="T2" s="10"/>
       <c r="U2" s="10"/>
-    </row>
-    <row r="3" spans="1:21" ht="81">
+      <c r="V2" s="10"/>
+    </row>
+    <row r="3" spans="1:22" ht="81">
       <c r="A3" s="10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B3" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>28</v>
-      </c>
+      <c r="G3" s="10"/>
       <c r="I3" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="J3" s="13"/>
+      <c r="J3" s="10" t="s">
+        <v>30</v>
+      </c>
       <c r="K3" s="13"/>
-      <c r="L3" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="M3" s="10"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="N3" s="10"/>
       <c r="O3" s="10"/>
       <c r="P3" s="10"/>
-      <c r="Q3" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="R3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="S3" s="10"/>
       <c r="T3" s="10"/>
       <c r="U3" s="10"/>
-    </row>
-    <row r="4" spans="1:21" ht="40.5">
+      <c r="V3" s="10"/>
+    </row>
+    <row r="4" spans="1:22" ht="40.5">
       <c r="A4" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B4" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" s="10" t="s">
-        <v>33</v>
-      </c>
+      <c r="G4" s="10"/>
+      <c r="H4" s="24"/>
       <c r="I4" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="13"/>
-      <c r="K4" s="10"/>
+      <c r="J4" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="K4" s="13"/>
       <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
+      <c r="M4" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="N4" s="10"/>
       <c r="O4" s="10"/>
       <c r="P4" s="10"/>
-      <c r="Q4" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="R4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="S4" s="10"/>
       <c r="T4" s="10"/>
       <c r="U4" s="10"/>
-    </row>
-    <row r="5" spans="1:21">
+      <c r="V4" s="10"/>
+    </row>
+    <row r="5" spans="1:22">
       <c r="A5" s="10" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C5" s="10" t="b">
         <v>1</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>36</v>
-      </c>
+      <c r="F5" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="10"/>
+      <c r="H5" s="24"/>
       <c r="I5" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="L5" s="10"/>
+      <c r="J5" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5" s="13"/>
+      <c r="L5" s="24" t="s">
+        <v>40</v>
+      </c>
       <c r="M5" s="10"/>
       <c r="N5" s="10"/>
       <c r="O5" s="10"/>
       <c r="P5" s="10"/>
-      <c r="Q5" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="R5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="S5" s="10"/>
       <c r="T5" s="10"/>
       <c r="U5" s="10"/>
-    </row>
-    <row r="6" spans="1:21" ht="27">
+      <c r="V5" s="10"/>
+    </row>
+    <row r="6" spans="1:22" ht="27">
       <c r="A6" s="10" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6" s="10" t="b">
         <v>1</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>40</v>
+      <c r="F6" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="10"/>
+      <c r="H6" s="24" t="s">
+        <v>42</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="L6" s="10"/>
+        <v>43</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="K6" s="13"/>
+      <c r="L6" s="24" t="s">
+        <v>45</v>
+      </c>
       <c r="M6" s="10"/>
       <c r="N6" s="10"/>
       <c r="O6" s="10"/>
       <c r="P6" s="10"/>
-      <c r="Q6" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="R6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="S6" s="10"/>
       <c r="T6" s="10"/>
       <c r="U6" s="10"/>
-    </row>
-    <row r="7" spans="1:21">
+      <c r="V6" s="10"/>
+    </row>
+    <row r="7" spans="1:22">
       <c r="A7" s="10" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C7" s="10" t="b">
         <v>1</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10" t="str">
-        <f t="shared" ref="G7:G19" si="0">REPLACE(A7, FIND("_", A7), 1, ".")</f>
+      <c r="F7" s="10" t="str">
+        <f t="shared" ref="F7:F19" si="0">REPLACE(A7, FIND("_", A7), 1, ".")</f>
         <v>home.address</v>
       </c>
-      <c r="H7" s="10" t="s">
-        <v>44</v>
-      </c>
+      <c r="G7" s="10"/>
+      <c r="H7" s="24"/>
       <c r="I7" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="J7" s="10"/>
+        <v>47</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>48</v>
+      </c>
       <c r="K7" s="10"/>
       <c r="L7" s="10"/>
       <c r="M7" s="10"/>
       <c r="N7" s="10"/>
       <c r="O7" s="10"/>
       <c r="P7" s="10"/>
-      <c r="Q7" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="R7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="S7" s="10"/>
       <c r="T7" s="10"/>
       <c r="U7" s="10"/>
-    </row>
-    <row r="8" spans="1:21">
+      <c r="V7" s="10"/>
+    </row>
+    <row r="8" spans="1:22">
       <c r="A8" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C8" s="10" t="b">
         <v>1</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10" t="str">
+      <c r="F8" s="10" t="str">
         <f t="shared" si="0"/>
         <v>home.city</v>
       </c>
-      <c r="H8" s="10" t="s">
-        <v>47</v>
-      </c>
+      <c r="G8" s="10"/>
+      <c r="H8" s="24"/>
       <c r="I8" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="J8" s="10"/>
+        <v>50</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>51</v>
+      </c>
       <c r="K8" s="10"/>
       <c r="L8" s="10"/>
-      <c r="M8" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="N8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10" t="s">
+        <v>52</v>
+      </c>
       <c r="O8" s="10"/>
       <c r="P8" s="10"/>
-      <c r="Q8" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="R8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="S8" s="10"/>
       <c r="T8" s="10"/>
       <c r="U8" s="10"/>
-    </row>
-    <row r="9" spans="1:21" ht="40.5">
+      <c r="V8" s="10"/>
+    </row>
+    <row r="9" spans="1:22" ht="40.5">
       <c r="A9" s="10" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C9" s="10" t="b">
         <v>1</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10" t="str">
+      <c r="F9" s="10" t="str">
         <f t="shared" si="0"/>
         <v>home.region</v>
       </c>
-      <c r="H9" s="10" t="s">
-        <v>51</v>
-      </c>
+      <c r="G9" s="10"/>
+      <c r="H9" s="24"/>
       <c r="I9" s="10" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="K9" s="10"/>
+        <v>54</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>55</v>
+      </c>
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>
       <c r="N9" s="10"/>
       <c r="O9" s="10"/>
       <c r="P9" s="10"/>
-      <c r="Q9" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="R9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="S9" s="10"/>
-      <c r="T9" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="U9" s="10"/>
-    </row>
-    <row r="10" spans="1:21" ht="40.5">
+      <c r="T9" s="10"/>
+      <c r="U9" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="V9" s="10"/>
+    </row>
+    <row r="10" spans="1:22" ht="40.5">
       <c r="A10" s="10" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C10" s="10" t="b">
         <v>1</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10" t="str">
+      <c r="F10" s="10" t="str">
         <f>REPLACE(A10, FIND("_", A10), 1, ".")</f>
         <v>home.country</v>
       </c>
-      <c r="H10" s="10" t="s">
-        <v>55</v>
-      </c>
+      <c r="G10" s="10"/>
+      <c r="H10" s="24"/>
       <c r="I10" s="10" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="K10" s="10"/>
+        <v>59</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>60</v>
+      </c>
       <c r="L10" s="10"/>
       <c r="M10" s="10"/>
       <c r="N10" s="10"/>
       <c r="O10" s="10"/>
       <c r="P10" s="10"/>
-      <c r="Q10" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="R10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="S10" s="10"/>
-      <c r="T10" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="U10" s="10"/>
-    </row>
-    <row r="11" spans="1:21" ht="27">
+      <c r="T10" s="10"/>
+      <c r="U10" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="V10" s="10"/>
+    </row>
+    <row r="11" spans="1:22" ht="27">
       <c r="A11" s="10" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C11" s="10" t="b">
         <v>1</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10" t="str">
+      <c r="F11" s="10" t="str">
         <f t="shared" si="0"/>
         <v>home.postalCode</v>
       </c>
-      <c r="H11" s="10" t="s">
-        <v>60</v>
-      </c>
+      <c r="G11" s="10"/>
+      <c r="H11" s="24"/>
       <c r="I11" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="L11" s="10"/>
+        <v>63</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10" t="s">
+        <v>65</v>
+      </c>
       <c r="M11" s="10"/>
       <c r="N11" s="10"/>
       <c r="O11" s="10"/>
       <c r="P11" s="10"/>
-      <c r="Q11" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="R11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="S11" s="10"/>
       <c r="T11" s="10"/>
       <c r="U11" s="10"/>
-    </row>
-    <row r="12" spans="1:21" ht="117.75" customHeight="1">
+      <c r="V11" s="10"/>
+    </row>
+    <row r="12" spans="1:22" ht="117.75" customHeight="1">
       <c r="A12" s="15" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C12" s="10" t="b">
         <v>1</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10" t="str">
+      <c r="F12" s="10" t="str">
         <f t="shared" si="0"/>
         <v>home.geography</v>
       </c>
-      <c r="H12" s="10" t="s">
-        <v>65</v>
-      </c>
+      <c r="G12" s="10"/>
+      <c r="H12" s="24"/>
       <c r="I12" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="J12" s="15"/>
-      <c r="K12" s="10"/>
+        <v>68</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="K12" s="15"/>
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
       <c r="N12" s="10"/>
       <c r="O12" s="10"/>
       <c r="P12" s="10"/>
-      <c r="Q12" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="R12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="S12" s="10"/>
       <c r="T12" s="10"/>
       <c r="U12" s="10"/>
-    </row>
-    <row r="13" spans="1:21" ht="48" customHeight="1">
+      <c r="V12" s="10"/>
+    </row>
+    <row r="13" spans="1:22" ht="48" customHeight="1">
       <c r="A13" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="B13" s="10" t="s">
-        <v>64</v>
-      </c>
       <c r="C13" s="10" t="b">
         <v>1</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10" t="str">
+      <c r="F13" s="10" t="str">
         <f t="shared" si="0"/>
         <v>household.size</v>
       </c>
-      <c r="H13" s="10" t="s">
-        <v>68</v>
-      </c>
+      <c r="G13" s="10"/>
+      <c r="H13" s="24"/>
       <c r="I13" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="J13" s="10"/>
+        <v>71</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>72</v>
+      </c>
       <c r="K13" s="10"/>
       <c r="L13" s="10"/>
       <c r="M13" s="10"/>
       <c r="N13" s="10"/>
       <c r="O13" s="10"/>
       <c r="P13" s="10"/>
-      <c r="Q13" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="R13" s="10"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="S13" s="10"/>
       <c r="T13" s="10"/>
       <c r="U13" s="10"/>
-    </row>
-    <row r="14" spans="1:21" ht="56.25" customHeight="1">
+      <c r="V13" s="10"/>
+    </row>
+    <row r="14" spans="1:22" ht="56.25" customHeight="1">
       <c r="A14" s="10" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C14" s="10" t="b">
         <v>1</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10" t="str">
+      <c r="F14" s="10" t="str">
         <f t="shared" si="0"/>
         <v>household.carNumber</v>
       </c>
-      <c r="H14" s="10" t="s">
-        <v>71</v>
-      </c>
+      <c r="G14" s="10"/>
+      <c r="H14" s="24"/>
       <c r="I14" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="N14" s="10"/>
+      <c r="J14" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10" t="s">
+        <v>77</v>
+      </c>
       <c r="O14" s="10"/>
       <c r="P14" s="10"/>
-      <c r="Q14" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="R14" s="10"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="S14" s="10"/>
       <c r="T14" s="10"/>
       <c r="U14" s="10"/>
-    </row>
-    <row r="15" spans="1:21" ht="76.5" customHeight="1">
+      <c r="V14" s="10"/>
+    </row>
+    <row r="15" spans="1:22" ht="76.5" customHeight="1">
       <c r="A15" s="10" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C15" s="10" t="b">
         <v>1</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10" t="str">
+      <c r="F15" s="10" t="str">
         <f t="shared" si="0"/>
         <v>household.bicycleNumber</v>
       </c>
-      <c r="H15" s="10" t="s">
-        <v>76</v>
-      </c>
+      <c r="G15" s="10"/>
+      <c r="H15" s="24"/>
       <c r="I15" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="L15" s="10"/>
+        <v>79</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10" t="s">
+        <v>81</v>
+      </c>
       <c r="M15" s="10"/>
       <c r="N15" s="10"/>
       <c r="O15" s="10"/>
       <c r="P15" s="10"/>
-      <c r="Q15" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="R15" s="10"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="S15" s="10"/>
       <c r="T15" s="10"/>
       <c r="U15" s="10"/>
-    </row>
-    <row r="16" spans="1:21" ht="40.5">
+      <c r="V15" s="10"/>
+    </row>
+    <row r="16" spans="1:22" ht="40.5">
       <c r="A16" s="10" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C16" s="10" t="b">
         <v>1</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10" t="str">
+      <c r="F16" s="10" t="str">
         <f t="shared" si="0"/>
         <v>household.electricBicycleNumber</v>
       </c>
-      <c r="H16" s="23" t="s">
-        <v>80</v>
-      </c>
+      <c r="G16" s="10"/>
+      <c r="H16" s="24"/>
       <c r="I16" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="J16" s="10"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="10"/>
+        <v>83</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="K16" s="10"/>
+      <c r="L16" s="13"/>
       <c r="M16" s="10"/>
       <c r="N16" s="10"/>
       <c r="O16" s="10"/>
       <c r="P16" s="10"/>
-      <c r="Q16" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="R16" s="10"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="S16" s="10"/>
       <c r="T16" s="10"/>
       <c r="U16" s="10"/>
-    </row>
-    <row r="17" spans="1:21" ht="76.5" customHeight="1">
+      <c r="V16" s="10"/>
+    </row>
+    <row r="17" spans="1:22" ht="76.5" customHeight="1">
       <c r="A17" s="10" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C17" s="10" t="b">
         <v>1</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10" t="str">
+      <c r="F17" s="10" t="str">
         <f>REPLACE(A17, FIND("_", A17), 1, ".")</f>
         <v>household.atLeastOnePersonWithDisability</v>
       </c>
-      <c r="H17" s="10" t="s">
-        <v>83</v>
-      </c>
+      <c r="G17" s="10"/>
+      <c r="H17" s="24"/>
       <c r="I17" s="10" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="M17" s="10"/>
+        <v>87</v>
+      </c>
+      <c r="K17" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10" t="s">
+        <v>89</v>
+      </c>
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
       <c r="P17" s="10"/>
-      <c r="Q17" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="R17" s="10"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="S17" s="10"/>
       <c r="T17" s="10"/>
       <c r="U17" s="10"/>
-    </row>
-    <row r="18" spans="1:21">
+      <c r="V17" s="10"/>
+    </row>
+    <row r="18" spans="1:22">
       <c r="A18" s="11" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C18" s="11" t="b">
         <v>1</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E18" s="11"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="20" t="str">
+        <v>24</v>
+      </c>
+      <c r="E18" s="12"/>
+      <c r="F18" s="20" t="str">
         <f t="shared" si="0"/>
         <v>home.save</v>
       </c>
-      <c r="H18" s="11" t="s">
-        <v>89</v>
-      </c>
+      <c r="G18" s="11"/>
+      <c r="H18" s="25"/>
       <c r="I18" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="J18" s="12"/>
+        <v>92</v>
+      </c>
+      <c r="J18" s="11" t="s">
+        <v>93</v>
+      </c>
       <c r="K18" s="12"/>
       <c r="L18" s="12"/>
       <c r="M18" s="12"/>
       <c r="N18" s="12"/>
       <c r="O18" s="12"/>
       <c r="P18" s="12"/>
-      <c r="Q18" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="R18" s="12"/>
+      <c r="Q18" s="12"/>
+      <c r="R18" s="11" t="b">
+        <v>1</v>
+      </c>
       <c r="S18" s="12"/>
       <c r="T18" s="12"/>
       <c r="U18" s="12"/>
-    </row>
-    <row r="19" spans="1:21">
+      <c r="V18" s="12"/>
+    </row>
+    <row r="19" spans="1:22">
       <c r="A19" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B19" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="B19" s="11" t="s">
-        <v>88</v>
-      </c>
       <c r="C19" s="11" t="b">
         <v>1</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="E19" s="11"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="20" t="str">
+        <v>95</v>
+      </c>
+      <c r="E19" s="12"/>
+      <c r="F19" s="20" t="str">
         <f t="shared" si="0"/>
         <v>household.save</v>
       </c>
-      <c r="H19" s="11" t="s">
-        <v>89</v>
-      </c>
+      <c r="G19" s="11"/>
+      <c r="H19" s="25"/>
       <c r="I19" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="J19" s="12"/>
+        <v>92</v>
+      </c>
+      <c r="J19" s="11" t="s">
+        <v>93</v>
+      </c>
       <c r="K19" s="12"/>
       <c r="L19" s="12"/>
       <c r="M19" s="12"/>
       <c r="N19" s="12"/>
       <c r="O19" s="12"/>
       <c r="P19" s="12"/>
-      <c r="Q19" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="R19" s="12"/>
+      <c r="Q19" s="12"/>
+      <c r="R19" s="11" t="b">
+        <v>1</v>
+      </c>
       <c r="S19" s="12"/>
       <c r="T19" s="12"/>
       <c r="U19" s="12"/>
-    </row>
-    <row r="20" spans="1:21" ht="130.5">
+      <c r="V19" s="12"/>
+    </row>
+    <row r="20" spans="1:22" ht="130.5">
       <c r="A20" s="9" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C20" s="9" t="b">
         <v>1</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>95</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="H20" s="26"/>
       <c r="I20" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="J20" s="22"/>
-      <c r="Q20" s="9" t="b">
+        <v>98</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="K20" s="22"/>
+      <c r="R20" s="9" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2015,19 +2063,19 @@
       <formula>NOT(ISERROR(SEARCH("TRUE",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K20:N20">
+  <conditionalFormatting sqref="L20:O20">
     <cfRule type="expression" dxfId="2" priority="1">
-      <formula>AND($B1048348="Custom",  $B1048348&lt;&gt;"", ROW(K1048348)&lt;&gt;1)</formula>
+      <formula>AND($B1048348="Custom",  $B1048348&lt;&gt;"", ROW(L1048348)&lt;&gt;1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L20:M20">
+  <conditionalFormatting sqref="M20:N20">
     <cfRule type="expression" dxfId="1" priority="5">
-      <formula>AND($B20&lt;&gt;"Select", $B20&lt;&gt;"Checkbox", $B20&lt;&gt;"Radio",  $B20&lt;&gt;"", ROW(L20)&lt;&gt;1)</formula>
+      <formula>AND($B20&lt;&gt;"Select", $B20&lt;&gt;"Checkbox", $B20&lt;&gt;"Radio",  $B20&lt;&gt;"", ROW(M20)&lt;&gt;1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N20">
+  <conditionalFormatting sqref="O20">
     <cfRule type="expression" dxfId="0" priority="2">
-      <formula>AND($B20&lt;&gt;"Range", $B20&lt;&gt;"", ROW(N20)&lt;&gt;1)</formula>
+      <formula>AND($B20&lt;&gt;"Range", $B20&lt;&gt;"", ROW(O20)&lt;&gt;1)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2054,34 +2102,34 @@
   <sheetData>
     <row r="1" spans="1:6" s="6" customFormat="1">
       <c r="A1" s="16" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="29.25">
       <c r="A2" s="14" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B2" s="14"/>
       <c r="C2" s="14" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E2" s="14">
         <v>1</v>
@@ -2090,14 +2138,14 @@
     </row>
     <row r="3" spans="1:6" ht="29.25">
       <c r="A3" s="14" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B3" s="14"/>
       <c r="C3" s="14" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="E3" s="14">
         <v>2</v>
@@ -2113,7 +2161,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{154E0277-C785-47D8-A3E6-B2B8778DC36B}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
@@ -2134,39 +2182,39 @@
         <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="E2" s="14" t="b">
         <v>1</v>
@@ -2180,16 +2228,16 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="14" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="E3" s="14" t="b">
         <v>1</v>
@@ -2203,16 +2251,16 @@
     </row>
     <row r="4" spans="1:8" ht="29.25">
       <c r="A4" s="14" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="E4" s="14" t="b">
         <v>0</v>
@@ -2234,7 +2282,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2249,148 +2297,148 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="3" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B2" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C2" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="D2" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B3" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C3" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D3" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B4" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C4" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="D4" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C5" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="D5" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B6" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="C6" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D6" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E7" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E8" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="E10" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="E11" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="E12" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="E13" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -2403,7 +2451,7 @@
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2420,42 +2468,42 @@
     <col min="12" max="12" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="5" customFormat="1" ht="30.75">
+    <row r="1" spans="1:12" s="5" customFormat="1">
       <c r="A1" s="4" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -2475,19 +2523,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Generate radio number widget with Generator
Test simple and complex cases for Radio and RadioNumber.
Remove RadioNumber custom inside the demo_generator, because we can generate it with Generator now.
</commit_message>
<xml_diff>
--- a/example/demo_generator/references/Household_Travel_Generate_Survey.xlsx
+++ b/example/demo_generator/references/Household_Travel_Generate_Survey.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28922"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="514" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{869A8025-255C-48B7-B4C3-461505204C6E}"/>
+  <xr:revisionPtr revIDLastSave="552" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5204B30E-6338-475F-9908-FF13A30C759E}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="164">
   <si>
     <t>questionName</t>
   </si>
@@ -56,16 +56,16 @@
     <t>path</t>
   </si>
   <si>
+    <t>fr</t>
+  </si>
+  <si>
+    <t>en</t>
+  </si>
+  <si>
     <t>parameters</t>
   </si>
   <si>
-    <t>appareance</t>
-  </si>
-  <si>
-    <t>fr</t>
-  </si>
-  <si>
-    <t>en</t>
+    <t>appearance</t>
   </si>
   <si>
     <t>conditional</t>
@@ -168,9 +168,6 @@
     <t>phoneNumber</t>
   </si>
   <si>
-    <t>join_with=${contactEmail}</t>
-  </si>
-  <si>
     <t>**Numéro de téléphone**
 __Format: 123-456-7890__</t>
   </si>
@@ -179,6 +176,9 @@
 __Format: 123-456-7890__</t>
   </si>
   <si>
+    <t>join_with=${contactEmail}</t>
+  </si>
+  <si>
     <t>phoneValidation</t>
   </si>
   <si>
@@ -259,6 +259,9 @@
     <t>household_size</t>
   </si>
   <si>
+    <t>RadioNumber</t>
+  </si>
+  <si>
     <t>**Personnes habitant votre domicile** ou logement.
 __Y compris vous-même.__</t>
   </si>
@@ -267,6 +270,19 @@
 __Including yourself.__</t>
   </si>
   <si>
+    <t>min=1
+max=6</t>
+  </si>
+  <si>
+    <t>overMaxAllowed</t>
+  </si>
+  <si>
+    <t>householdSizeValidation</t>
+  </si>
+  <si>
+    <t>householdSizeHelpPopup</t>
+  </si>
+  <si>
     <t>household_carNumber</t>
   </si>
   <si>
@@ -276,6 +292,10 @@
   <si>
     <t>**Cars**, SUVs, light-duty trucks or vans, etc.
 __Available to one or more members of your household.__</t>
+  </si>
+  <si>
+    <t>min=0
+max=5</t>
   </si>
   <si>
     <t>carNumberValidation</t>
@@ -1151,8 +1171,8 @@
   <dimension ref="A1:V20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="G1" sqref="G1:G1048576"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="K16" sqref="K16"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -1160,15 +1180,15 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.85546875" style="9" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="9" customWidth="1"/>
     <col min="3" max="3" width="6.42578125" style="9" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" style="9" customWidth="1"/>
     <col min="5" max="5" width="5.7109375" style="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" style="9" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" style="9" customWidth="1"/>
-    <col min="8" max="8" width="21.140625" style="27" customWidth="1"/>
-    <col min="9" max="9" width="31.28515625" style="9" customWidth="1"/>
-    <col min="10" max="10" width="31.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.28515625" style="9" customWidth="1"/>
+    <col min="8" max="8" width="31.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" style="9" customWidth="1"/>
+    <col min="10" max="10" width="22.7109375" style="27" customWidth="1"/>
     <col min="11" max="11" width="19.7109375" style="9" customWidth="1"/>
     <col min="12" max="12" width="13.5703125" style="9" customWidth="1"/>
     <col min="13" max="13" width="13" style="9" customWidth="1"/>
@@ -1203,16 +1223,16 @@
       <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="23" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="8" t="s">
@@ -1269,14 +1289,14 @@
       <c r="F2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="10"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="10" t="s">
+      <c r="G2" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="H2" s="10" t="s">
         <v>26</v>
       </c>
+      <c r="I2" s="10"/>
+      <c r="J2" s="24"/>
       <c r="K2" s="10"/>
       <c r="L2" s="13"/>
       <c r="M2" s="10"/>
@@ -1309,13 +1329,13 @@
       <c r="F3" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="10"/>
-      <c r="I3" s="10" t="s">
+      <c r="G3" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="H3" s="10" t="s">
         <v>30</v>
       </c>
+      <c r="I3" s="10"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="10" t="s">
@@ -1350,14 +1370,14 @@
       <c r="F4" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="10" t="s">
+      <c r="G4" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="H4" s="10" t="s">
         <v>35</v>
       </c>
+      <c r="I4" s="10"/>
+      <c r="J4" s="24"/>
       <c r="K4" s="13"/>
       <c r="L4" s="10"/>
       <c r="M4" s="10" t="s">
@@ -1392,14 +1412,14 @@
       <c r="F5" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="G5" s="10"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="10" t="s">
+      <c r="G5" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="H5" s="10" t="s">
         <v>39</v>
       </c>
+      <c r="I5" s="10"/>
+      <c r="J5" s="24"/>
       <c r="K5" s="13"/>
       <c r="L5" s="24" t="s">
         <v>40</v>
@@ -1434,14 +1454,14 @@
       <c r="F6" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="24" t="s">
+      <c r="G6" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="H6" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="I6" s="10"/>
+      <c r="J6" s="24" t="s">
         <v>44</v>
       </c>
       <c r="K6" s="13"/>
@@ -1479,14 +1499,14 @@
         <f t="shared" ref="F7:F19" si="0">REPLACE(A7, FIND("_", A7), 1, ".")</f>
         <v>home.address</v>
       </c>
-      <c r="G7" s="10"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="10" t="s">
+      <c r="G7" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="H7" s="10" t="s">
         <v>48</v>
       </c>
+      <c r="I7" s="10"/>
+      <c r="J7" s="24"/>
       <c r="K7" s="10"/>
       <c r="L7" s="10"/>
       <c r="M7" s="10"/>
@@ -1520,14 +1540,14 @@
         <f t="shared" si="0"/>
         <v>home.city</v>
       </c>
-      <c r="G8" s="10"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="10" t="s">
+      <c r="G8" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="H8" s="10" t="s">
         <v>51</v>
       </c>
+      <c r="I8" s="10"/>
+      <c r="J8" s="24"/>
       <c r="K8" s="10"/>
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
@@ -1563,14 +1583,14 @@
         <f t="shared" si="0"/>
         <v>home.region</v>
       </c>
-      <c r="G9" s="10"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="10" t="s">
+      <c r="G9" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="J9" s="10" t="s">
+      <c r="H9" s="10" t="s">
         <v>54</v>
       </c>
+      <c r="I9" s="10"/>
+      <c r="J9" s="24"/>
       <c r="K9" s="10" t="s">
         <v>55</v>
       </c>
@@ -1608,14 +1628,14 @@
         <f>REPLACE(A10, FIND("_", A10), 1, ".")</f>
         <v>home.country</v>
       </c>
-      <c r="G10" s="10"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="10" t="s">
+      <c r="G10" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J10" s="10" t="s">
+      <c r="H10" s="10" t="s">
         <v>59</v>
       </c>
+      <c r="I10" s="10"/>
+      <c r="J10" s="24"/>
       <c r="K10" s="10" t="s">
         <v>60</v>
       </c>
@@ -1653,14 +1673,14 @@
         <f t="shared" si="0"/>
         <v>home.postalCode</v>
       </c>
-      <c r="G11" s="10"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="10" t="s">
+      <c r="G11" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="J11" s="10" t="s">
+      <c r="H11" s="10" t="s">
         <v>64</v>
       </c>
+      <c r="I11" s="10"/>
+      <c r="J11" s="24"/>
       <c r="K11" s="10"/>
       <c r="L11" s="10" t="s">
         <v>65</v>
@@ -1696,14 +1716,14 @@
         <f t="shared" si="0"/>
         <v>home.geography</v>
       </c>
-      <c r="G12" s="10"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="10" t="s">
+      <c r="G12" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="J12" s="10" t="s">
+      <c r="H12" s="10" t="s">
         <v>69</v>
       </c>
+      <c r="I12" s="10"/>
+      <c r="J12" s="24"/>
       <c r="K12" s="15"/>
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
@@ -1724,7 +1744,7 @@
         <v>70</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C13" s="10" t="b">
         <v>1</v>
@@ -1737,18 +1757,26 @@
         <f t="shared" si="0"/>
         <v>household.size</v>
       </c>
-      <c r="G13" s="10"/>
-      <c r="H13" s="24"/>
+      <c r="G13" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>73</v>
+      </c>
       <c r="I13" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="J13" s="10" t="s">
-        <v>72</v>
+        <v>74</v>
+      </c>
+      <c r="J13" s="24" t="s">
+        <v>75</v>
       </c>
       <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
+      <c r="L13" s="10" t="s">
+        <v>76</v>
+      </c>
       <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
+      <c r="N13" s="10" t="s">
+        <v>77</v>
+      </c>
       <c r="O13" s="10"/>
       <c r="P13" s="10"/>
       <c r="Q13" s="10"/>
@@ -1762,10 +1790,10 @@
     </row>
     <row r="14" spans="1:22" ht="56.25" customHeight="1">
       <c r="A14" s="10" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C14" s="10" t="b">
         <v>1</v>
@@ -1778,21 +1806,25 @@
         <f t="shared" si="0"/>
         <v>household.carNumber</v>
       </c>
-      <c r="G14" s="10"/>
-      <c r="H14" s="24"/>
+      <c r="G14" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>80</v>
+      </c>
       <c r="I14" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="J14" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="J14" s="24" t="s">
         <v>75</v>
       </c>
       <c r="K14" s="10"/>
       <c r="L14" s="10" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="M14" s="10"/>
       <c r="N14" s="10" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="O14" s="10"/>
       <c r="P14" s="10"/>
@@ -1807,10 +1839,10 @@
     </row>
     <row r="15" spans="1:22" ht="76.5" customHeight="1">
       <c r="A15" s="10" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C15" s="10" t="b">
         <v>1</v>
@@ -1823,17 +1855,21 @@
         <f t="shared" si="0"/>
         <v>household.bicycleNumber</v>
       </c>
-      <c r="G15" s="10"/>
-      <c r="H15" s="24"/>
+      <c r="G15" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>86</v>
+      </c>
       <c r="I15" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="J15" s="10" t="s">
-        <v>80</v>
+        <v>81</v>
+      </c>
+      <c r="J15" s="24" t="s">
+        <v>75</v>
       </c>
       <c r="K15" s="10"/>
       <c r="L15" s="10" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="M15" s="10"/>
       <c r="N15" s="10"/>
@@ -1850,10 +1886,10 @@
     </row>
     <row r="16" spans="1:22" ht="40.5">
       <c r="A16" s="10" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C16" s="10" t="b">
         <v>1</v>
@@ -1866,15 +1902,19 @@
         <f t="shared" si="0"/>
         <v>household.electricBicycleNumber</v>
       </c>
-      <c r="G16" s="10"/>
-      <c r="H16" s="24"/>
+      <c r="G16" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>90</v>
+      </c>
       <c r="I16" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="J16" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="K16" s="10"/>
+        <v>81</v>
+      </c>
+      <c r="J16" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="K16" s="13"/>
       <c r="L16" s="13"/>
       <c r="M16" s="10"/>
       <c r="N16" s="10"/>
@@ -1891,7 +1931,7 @@
     </row>
     <row r="17" spans="1:22" ht="76.5" customHeight="1">
       <c r="A17" s="10" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>28</v>
@@ -1907,20 +1947,20 @@
         <f>REPLACE(A17, FIND("_", A17), 1, ".")</f>
         <v>household.atLeastOnePersonWithDisability</v>
       </c>
-      <c r="G17" s="10"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="J17" s="10" t="s">
-        <v>87</v>
-      </c>
+      <c r="G17" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="I17" s="10"/>
+      <c r="J17" s="24"/>
       <c r="K17" s="10" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="L17" s="10"/>
       <c r="M17" s="10" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
@@ -1936,10 +1976,10 @@
     </row>
     <row r="18" spans="1:22">
       <c r="A18" s="11" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="C18" s="11" t="b">
         <v>1</v>
@@ -1952,14 +1992,14 @@
         <f t="shared" si="0"/>
         <v>home.save</v>
       </c>
-      <c r="G18" s="11"/>
-      <c r="H18" s="25"/>
-      <c r="I18" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="J18" s="11" t="s">
-        <v>93</v>
-      </c>
+      <c r="G18" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="I18" s="11"/>
+      <c r="J18" s="25"/>
       <c r="K18" s="12"/>
       <c r="L18" s="12"/>
       <c r="M18" s="12"/>
@@ -1977,30 +2017,30 @@
     </row>
     <row r="19" spans="1:22">
       <c r="A19" s="11" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="C19" s="11" t="b">
         <v>1</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="E19" s="12"/>
       <c r="F19" s="20" t="str">
         <f t="shared" si="0"/>
         <v>household.save</v>
       </c>
-      <c r="G19" s="11"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="J19" s="11" t="s">
-        <v>93</v>
-      </c>
+      <c r="G19" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="I19" s="11"/>
+      <c r="J19" s="25"/>
       <c r="K19" s="12"/>
       <c r="L19" s="12"/>
       <c r="M19" s="12"/>
@@ -2018,7 +2058,7 @@
     </row>
     <row r="20" spans="1:22" ht="130.5">
       <c r="A20" s="9" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>33</v>
@@ -2027,30 +2067,30 @@
         <v>1</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="H20" s="26"/>
-      <c r="I20" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="J20" s="9" t="s">
-        <v>99</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="J20" s="26"/>
       <c r="K20" s="22"/>
       <c r="R20" s="9" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C19 C21:C1048576">
+  <conditionalFormatting sqref="C21:C1048576 C1:C19">
     <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C19 C21:C1048576">
+  <conditionalFormatting sqref="C21:C1048576 C1:C19">
     <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C1)))</formula>
     </cfRule>
@@ -2102,34 +2142,34 @@
   <sheetData>
     <row r="1" spans="1:6" s="6" customFormat="1">
       <c r="A1" s="16" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="C1" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="29.25">
       <c r="A2" s="14" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B2" s="14"/>
       <c r="C2" s="14" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="E2" s="14">
         <v>1</v>
@@ -2138,14 +2178,14 @@
     </row>
     <row r="3" spans="1:6" ht="29.25">
       <c r="A3" s="14" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B3" s="14"/>
       <c r="C3" s="14" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="E3" s="14">
         <v>2</v>
@@ -2182,25 +2222,25 @@
         <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -2208,13 +2248,13 @@
         <v>24</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="E2" s="14" t="b">
         <v>1</v>
@@ -2228,16 +2268,16 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="14" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="E3" s="14" t="b">
         <v>1</v>
@@ -2251,16 +2291,16 @@
     </row>
     <row r="4" spans="1:8" ht="29.25">
       <c r="A4" s="14" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="E4" s="14" t="b">
         <v>0</v>
@@ -2297,19 +2337,19 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="3" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>10</v>
@@ -2317,72 +2357,72 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="B2" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="C2" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="D2" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B3" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="C3" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="D3" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="B4" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="C4" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="D4" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="C5" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="D5" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="B6" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="C6" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="D6" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2390,7 +2430,7 @@
         <v>31</v>
       </c>
       <c r="E7" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2398,12 +2438,12 @@
         <v>31</v>
       </c>
       <c r="E8" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="E9" t="s">
         <v>31</v>
@@ -2411,34 +2451,34 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
+        <v>148</v>
+      </c>
+      <c r="E10" t="s">
         <v>142</v>
-      </c>
-      <c r="E10" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="E11" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="E12" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="E13" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -2470,40 +2510,40 @@
   <sheetData>
     <row r="1" spans="1:12" s="5" customFormat="1">
       <c r="A1" s="4" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -2523,19 +2563,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Generate radio number widget with generator (#1005)
* Test generate_radio_widget with minimal required fields.

* Generate radio number widget with Generator

Test simple and complex cases for Radio and RadioNumber.
Remove RadioNumber custom inside the demo_generator, because we can generate it with the Generator now.

* Add get_parameters_values function.

Test that get_parameters_values() can split parameters on newlines, semicolons, or spaces.
Update the README with a parameters column.
</commit_message>
<xml_diff>
--- a/example/demo_generator/references/Household_Travel_Generate_Survey.xlsx
+++ b/example/demo_generator/references/Household_Travel_Generate_Survey.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28922"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="514" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{869A8025-255C-48B7-B4C3-461505204C6E}"/>
+  <xr:revisionPtr revIDLastSave="567" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5483AD5-6D98-4611-80B2-E389FD18E1E7}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Widgets" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="163">
   <si>
     <t>questionName</t>
   </si>
@@ -56,16 +56,16 @@
     <t>path</t>
   </si>
   <si>
+    <t>fr</t>
+  </si>
+  <si>
+    <t>en</t>
+  </si>
+  <si>
     <t>parameters</t>
   </si>
   <si>
-    <t>appareance</t>
-  </si>
-  <si>
-    <t>fr</t>
-  </si>
-  <si>
-    <t>en</t>
+    <t>appearance</t>
   </si>
   <si>
     <t>conditional</t>
@@ -168,9 +168,6 @@
     <t>phoneNumber</t>
   </si>
   <si>
-    <t>join_with=${contactEmail}</t>
-  </si>
-  <si>
     <t>**Numéro de téléphone**
 __Format: 123-456-7890__</t>
   </si>
@@ -179,6 +176,9 @@
 __Format: 123-456-7890__</t>
   </si>
   <si>
+    <t>join_with=${contactEmail}</t>
+  </si>
+  <si>
     <t>phoneValidation</t>
   </si>
   <si>
@@ -259,6 +259,9 @@
     <t>household_size</t>
   </si>
   <si>
+    <t>RadioNumber</t>
+  </si>
+  <si>
     <t>**Personnes habitant votre domicile** ou logement.
 __Y compris vous-même.__</t>
   </si>
@@ -267,6 +270,17 @@
 __Including yourself.__</t>
   </si>
   <si>
+    <t>min=0
+max=6
+overMaxAllowed</t>
+  </si>
+  <si>
+    <t>householdSizeValidation</t>
+  </si>
+  <si>
+    <t>householdSizeHelpPopup</t>
+  </si>
+  <si>
     <t>household_carNumber</t>
   </si>
   <si>
@@ -276,6 +290,11 @@
   <si>
     <t>**Cars**, SUVs, light-duty trucks or vans, etc.
 __Available to one or more members of your household.__</t>
+  </si>
+  <si>
+    <t>min=0
+max=5
+overMaxAllowed</t>
   </si>
   <si>
     <t>carNumberValidation</t>
@@ -662,7 +681,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -728,20 +747,11 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1151,8 +1161,8 @@
   <dimension ref="A1:V20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="G1" sqref="G1:G1048576"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="J16" sqref="J16"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -1160,15 +1170,15 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.85546875" style="9" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="9" customWidth="1"/>
     <col min="3" max="3" width="6.42578125" style="9" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" style="9" customWidth="1"/>
     <col min="5" max="5" width="5.7109375" style="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" style="9" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" style="9" customWidth="1"/>
-    <col min="8" max="8" width="21.140625" style="27" customWidth="1"/>
-    <col min="9" max="9" width="31.28515625" style="9" customWidth="1"/>
-    <col min="10" max="10" width="31.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.28515625" style="9" customWidth="1"/>
+    <col min="8" max="8" width="31.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" style="9" customWidth="1"/>
+    <col min="10" max="10" width="22.7109375" style="9" customWidth="1"/>
     <col min="11" max="11" width="19.7109375" style="9" customWidth="1"/>
     <col min="12" max="12" width="13.5703125" style="9" customWidth="1"/>
     <col min="13" max="13" width="13" style="9" customWidth="1"/>
@@ -1203,16 +1213,16 @@
       <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="23" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="8" t="s">
@@ -1269,14 +1279,14 @@
       <c r="F2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="10"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="10" t="s">
+      <c r="G2" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="H2" s="10" t="s">
         <v>26</v>
       </c>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
       <c r="K2" s="10"/>
       <c r="L2" s="13"/>
       <c r="M2" s="10"/>
@@ -1309,13 +1319,13 @@
       <c r="F3" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="10"/>
-      <c r="I3" s="10" t="s">
+      <c r="G3" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="H3" s="10" t="s">
         <v>30</v>
       </c>
+      <c r="I3" s="10"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="10" t="s">
@@ -1350,14 +1360,14 @@
       <c r="F4" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="10" t="s">
+      <c r="G4" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="H4" s="10" t="s">
         <v>35</v>
       </c>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
       <c r="K4" s="13"/>
       <c r="L4" s="10"/>
       <c r="M4" s="10" t="s">
@@ -1392,16 +1402,16 @@
       <c r="F5" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="G5" s="10"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="10" t="s">
+      <c r="G5" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="H5" s="10" t="s">
         <v>39</v>
       </c>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
       <c r="K5" s="13"/>
-      <c r="L5" s="24" t="s">
+      <c r="L5" s="10" t="s">
         <v>40</v>
       </c>
       <c r="M5" s="10"/>
@@ -1434,18 +1444,18 @@
       <c r="F6" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="24" t="s">
+      <c r="G6" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="H6" s="10" t="s">
         <v>43</v>
       </c>
+      <c r="I6" s="10"/>
       <c r="J6" s="10" t="s">
         <v>44</v>
       </c>
       <c r="K6" s="13"/>
-      <c r="L6" s="24" t="s">
+      <c r="L6" s="10" t="s">
         <v>45</v>
       </c>
       <c r="M6" s="10"/>
@@ -1479,14 +1489,14 @@
         <f t="shared" ref="F7:F19" si="0">REPLACE(A7, FIND("_", A7), 1, ".")</f>
         <v>home.address</v>
       </c>
-      <c r="G7" s="10"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="10" t="s">
+      <c r="G7" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="H7" s="10" t="s">
         <v>48</v>
       </c>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
       <c r="K7" s="10"/>
       <c r="L7" s="10"/>
       <c r="M7" s="10"/>
@@ -1520,14 +1530,14 @@
         <f t="shared" si="0"/>
         <v>home.city</v>
       </c>
-      <c r="G8" s="10"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="10" t="s">
+      <c r="G8" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="H8" s="10" t="s">
         <v>51</v>
       </c>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
       <c r="K8" s="10"/>
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
@@ -1563,14 +1573,14 @@
         <f t="shared" si="0"/>
         <v>home.region</v>
       </c>
-      <c r="G9" s="10"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="10" t="s">
+      <c r="G9" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="J9" s="10" t="s">
+      <c r="H9" s="10" t="s">
         <v>54</v>
       </c>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
       <c r="K9" s="10" t="s">
         <v>55</v>
       </c>
@@ -1608,14 +1618,14 @@
         <f>REPLACE(A10, FIND("_", A10), 1, ".")</f>
         <v>home.country</v>
       </c>
-      <c r="G10" s="10"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="10" t="s">
+      <c r="G10" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J10" s="10" t="s">
+      <c r="H10" s="10" t="s">
         <v>59</v>
       </c>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
       <c r="K10" s="10" t="s">
         <v>60</v>
       </c>
@@ -1653,14 +1663,14 @@
         <f t="shared" si="0"/>
         <v>home.postalCode</v>
       </c>
-      <c r="G11" s="10"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="10" t="s">
+      <c r="G11" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="J11" s="10" t="s">
+      <c r="H11" s="10" t="s">
         <v>64</v>
       </c>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
       <c r="K11" s="10"/>
       <c r="L11" s="10" t="s">
         <v>65</v>
@@ -1696,14 +1706,14 @@
         <f t="shared" si="0"/>
         <v>home.geography</v>
       </c>
-      <c r="G12" s="10"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="10" t="s">
+      <c r="G12" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="J12" s="10" t="s">
+      <c r="H12" s="10" t="s">
         <v>69</v>
       </c>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
       <c r="K12" s="15"/>
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
@@ -1724,7 +1734,7 @@
         <v>70</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C13" s="10" t="b">
         <v>1</v>
@@ -1737,18 +1747,24 @@
         <f t="shared" si="0"/>
         <v>household.size</v>
       </c>
-      <c r="G13" s="10"/>
-      <c r="H13" s="24"/>
+      <c r="G13" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>73</v>
+      </c>
       <c r="I13" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="J13" s="10" t="s">
-        <v>72</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="J13" s="10"/>
       <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
+      <c r="L13" s="10" t="s">
+        <v>75</v>
+      </c>
       <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
+      <c r="N13" s="10" t="s">
+        <v>76</v>
+      </c>
       <c r="O13" s="10"/>
       <c r="P13" s="10"/>
       <c r="Q13" s="10"/>
@@ -1762,10 +1778,10 @@
     </row>
     <row r="14" spans="1:22" ht="56.25" customHeight="1">
       <c r="A14" s="10" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C14" s="10" t="b">
         <v>1</v>
@@ -1778,21 +1794,23 @@
         <f t="shared" si="0"/>
         <v>household.carNumber</v>
       </c>
-      <c r="G14" s="10"/>
-      <c r="H14" s="24"/>
+      <c r="G14" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>79</v>
+      </c>
       <c r="I14" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="J14" s="10" t="s">
-        <v>75</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="J14" s="10"/>
       <c r="K14" s="10"/>
       <c r="L14" s="10" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="M14" s="10"/>
       <c r="N14" s="10" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="O14" s="10"/>
       <c r="P14" s="10"/>
@@ -1807,10 +1825,10 @@
     </row>
     <row r="15" spans="1:22" ht="76.5" customHeight="1">
       <c r="A15" s="10" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C15" s="10" t="b">
         <v>1</v>
@@ -1823,17 +1841,19 @@
         <f t="shared" si="0"/>
         <v>household.bicycleNumber</v>
       </c>
-      <c r="G15" s="10"/>
-      <c r="H15" s="24"/>
+      <c r="G15" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>85</v>
+      </c>
       <c r="I15" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="J15" s="10" t="s">
         <v>80</v>
       </c>
+      <c r="J15" s="10"/>
       <c r="K15" s="10"/>
       <c r="L15" s="10" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="M15" s="10"/>
       <c r="N15" s="10"/>
@@ -1850,10 +1870,10 @@
     </row>
     <row r="16" spans="1:22" ht="40.5">
       <c r="A16" s="10" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C16" s="10" t="b">
         <v>1</v>
@@ -1866,15 +1886,17 @@
         <f t="shared" si="0"/>
         <v>household.electricBicycleNumber</v>
       </c>
-      <c r="G16" s="10"/>
-      <c r="H16" s="24"/>
+      <c r="G16" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>89</v>
+      </c>
       <c r="I16" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="J16" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="K16" s="10"/>
+        <v>80</v>
+      </c>
+      <c r="J16" s="10"/>
+      <c r="K16" s="13"/>
       <c r="L16" s="13"/>
       <c r="M16" s="10"/>
       <c r="N16" s="10"/>
@@ -1891,7 +1913,7 @@
     </row>
     <row r="17" spans="1:22" ht="76.5" customHeight="1">
       <c r="A17" s="10" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>28</v>
@@ -1907,20 +1929,20 @@
         <f>REPLACE(A17, FIND("_", A17), 1, ".")</f>
         <v>household.atLeastOnePersonWithDisability</v>
       </c>
-      <c r="G17" s="10"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="J17" s="10" t="s">
-        <v>87</v>
-      </c>
+      <c r="G17" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
       <c r="K17" s="10" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="L17" s="10"/>
       <c r="M17" s="10" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
@@ -1936,10 +1958,10 @@
     </row>
     <row r="18" spans="1:22">
       <c r="A18" s="11" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="C18" s="11" t="b">
         <v>1</v>
@@ -1952,14 +1974,14 @@
         <f t="shared" si="0"/>
         <v>home.save</v>
       </c>
-      <c r="G18" s="11"/>
-      <c r="H18" s="25"/>
-      <c r="I18" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="J18" s="11" t="s">
-        <v>93</v>
-      </c>
+      <c r="G18" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="I18" s="11"/>
+      <c r="J18" s="12"/>
       <c r="K18" s="12"/>
       <c r="L18" s="12"/>
       <c r="M18" s="12"/>
@@ -1977,30 +1999,30 @@
     </row>
     <row r="19" spans="1:22">
       <c r="A19" s="11" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="C19" s="11" t="b">
         <v>1</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="E19" s="12"/>
       <c r="F19" s="20" t="str">
         <f t="shared" si="0"/>
         <v>household.save</v>
       </c>
-      <c r="G19" s="11"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="J19" s="11" t="s">
-        <v>93</v>
-      </c>
+      <c r="G19" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="I19" s="11"/>
+      <c r="J19" s="12"/>
       <c r="K19" s="12"/>
       <c r="L19" s="12"/>
       <c r="M19" s="12"/>
@@ -2018,7 +2040,7 @@
     </row>
     <row r="20" spans="1:22" ht="130.5">
       <c r="A20" s="9" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>33</v>
@@ -2027,30 +2049,30 @@
         <v>1</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="H20" s="26"/>
-      <c r="I20" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="J20" s="9" t="s">
-        <v>99</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="J20" s="24"/>
       <c r="K20" s="22"/>
       <c r="R20" s="9" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C19 C21:C1048576">
+  <conditionalFormatting sqref="C21:C1048576 C1:C19">
     <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C19 C21:C1048576">
+  <conditionalFormatting sqref="C21:C1048576 C1:C19">
     <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C1)))</formula>
     </cfRule>
@@ -2102,34 +2124,34 @@
   <sheetData>
     <row r="1" spans="1:6" s="6" customFormat="1">
       <c r="A1" s="16" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="C1" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="29.25">
       <c r="A2" s="14" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B2" s="14"/>
       <c r="C2" s="14" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E2" s="14">
         <v>1</v>
@@ -2138,14 +2160,14 @@
     </row>
     <row r="3" spans="1:6" ht="29.25">
       <c r="A3" s="14" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="B3" s="14"/>
       <c r="C3" s="14" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="E3" s="14">
         <v>2</v>
@@ -2182,25 +2204,25 @@
         <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -2208,13 +2230,13 @@
         <v>24</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="E2" s="14" t="b">
         <v>1</v>
@@ -2228,16 +2250,16 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="14" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="E3" s="14" t="b">
         <v>1</v>
@@ -2251,16 +2273,16 @@
     </row>
     <row r="4" spans="1:8" ht="29.25">
       <c r="A4" s="14" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="E4" s="14" t="b">
         <v>0</v>
@@ -2297,19 +2319,19 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="3" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>10</v>
@@ -2317,72 +2339,72 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="B2" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="C2" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="D2" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="C3" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="D3" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="B4" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="C4" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="D4" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="C5" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D5" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="B6" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="C6" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="D6" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2390,7 +2412,7 @@
         <v>31</v>
       </c>
       <c r="E7" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2398,12 +2420,12 @@
         <v>31</v>
       </c>
       <c r="E8" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="E9" t="s">
         <v>31</v>
@@ -2411,34 +2433,34 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="E10" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="E11" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="E12" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="E13" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -2470,40 +2492,40 @@
   <sheetData>
     <row r="1" spans="1:12" s="5" customFormat="1">
       <c r="A1" s="4" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -2523,19 +2545,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Household section in Demo_Generator
Test the household section with 1 and 2 persons.
</commit_message>
<xml_diff>
--- a/example/demo_generator/references/Household_Travel_Generate_Survey.xlsx
+++ b/example/demo_generator/references/Household_Travel_Generate_Survey.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28922"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="567" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5483AD5-6D98-4611-80B2-E389FD18E1E7}"/>
+  <xr:revisionPtr revIDLastSave="681" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB5A37E8-8767-4056-91CD-F7CE27EF0031}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="188">
   <si>
     <t>questionName</t>
   </si>
@@ -355,10 +355,89 @@
     <t>Save and continue</t>
   </si>
   <si>
+    <t>householdMembers</t>
+  </si>
+  <si>
+    <t>household</t>
+  </si>
+  <si>
+    <t>personNickname</t>
+  </si>
+  <si>
+    <t>nickname</t>
+  </si>
+  <si>
+    <t>**Nom ou surnom** pour identifier cette personne pour la suite de l'entrevue.
+__Peut être un surnom, des initiales, ou encore ce que cette personne est pour vous (ex: 'Moi', 'Toto', 'Maman', 'PN').
+Ce nom est seulement utilisé pour faciliter l'enquête et sera ensuite supprimé.__</t>
+  </si>
+  <si>
+    <t>**Name or nickname** that will allow you to identify this person for the remainder of the interview.
+__Can be a nickname, initials, or who this person represents to you (ex: 'Me','Kiddo','Mum','JT').
+The name is only used to simplify the response process and will be removed from the final dataset.__</t>
+  </si>
+  <si>
+    <t>personAge</t>
+  </si>
+  <si>
+    <t>personGender</t>
+  </si>
+  <si>
+    <t>personWorkerType</t>
+  </si>
+  <si>
+    <t>personSchoolType</t>
+  </si>
+  <si>
+    <t>personStudentType</t>
+  </si>
+  <si>
+    <t>personOccupation</t>
+  </si>
+  <si>
+    <t>personDrivingLicenseOwner</t>
+  </si>
+  <si>
+    <t>personCarSharingMember</t>
+  </si>
+  <si>
+    <t>personTransitFares</t>
+  </si>
+  <si>
+    <t>personHasDisability</t>
+  </si>
+  <si>
+    <t>personWorkLocationType</t>
+  </si>
+  <si>
+    <t>personSchoolLocationType</t>
+  </si>
+  <si>
+    <t>personUsualWorkPlaceName</t>
+  </si>
+  <si>
+    <t>personUsualWorkPlaceGeography</t>
+  </si>
+  <si>
+    <t>personUsualSchoolPlaceName</t>
+  </si>
+  <si>
+    <t>personUsualSchoolPlaceGeography</t>
+  </si>
+  <si>
+    <t>personTravelToWorkDays</t>
+  </si>
+  <si>
+    <t>personRemoteWorkDays</t>
+  </si>
+  <si>
+    <t>personTravelToStudyDays</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personRemoteStudyDays   </t>
+  </si>
+  <si>
     <t>household_save</t>
-  </si>
-  <si>
-    <t>household</t>
   </si>
   <si>
     <t>completedText</t>
@@ -553,7 +632,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -618,6 +697,17 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -645,7 +735,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -677,11 +767,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -752,6 +851,48 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1158,11 +1299,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V20"/>
+  <dimension ref="A1:V42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="J16" sqref="J16"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="I20" sqref="I20"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -1173,7 +1314,7 @@
     <col min="2" max="2" width="12.85546875" style="9" customWidth="1"/>
     <col min="3" max="3" width="6.42578125" style="9" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" style="9" customWidth="1"/>
-    <col min="5" max="5" width="5.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" style="9" customWidth="1"/>
     <col min="6" max="6" width="17" style="9" customWidth="1"/>
     <col min="7" max="7" width="31.28515625" style="9" customWidth="1"/>
     <col min="8" max="8" width="31.5703125" style="9" bestFit="1" customWidth="1"/>
@@ -1486,7 +1627,7 @@
       </c>
       <c r="E7" s="10"/>
       <c r="F7" s="10" t="str">
-        <f t="shared" ref="F7:F19" si="0">REPLACE(A7, FIND("_", A7), 1, ".")</f>
+        <f t="shared" ref="F7:F41" si="0">REPLACE(A7, FIND("_", A7), 1, ".")</f>
         <v>home.address</v>
       </c>
       <c r="G7" s="10" t="s">
@@ -1957,147 +2098,905 @@
       <c r="V17" s="10"/>
     </row>
     <row r="18" spans="1:22">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="C18" s="11" t="b">
+      <c r="C18" s="26" t="b">
         <v>1</v>
       </c>
       <c r="D18" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="12"/>
-      <c r="F18" s="20" t="str">
+      <c r="E18" s="27"/>
+      <c r="F18" s="28" t="str">
         <f t="shared" si="0"/>
         <v>home.save</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="G18" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="H18" s="11" t="s">
+      <c r="H18" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="I18" s="11"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="12"/>
-      <c r="M18" s="12"/>
-      <c r="N18" s="12"/>
-      <c r="O18" s="12"/>
-      <c r="P18" s="12"/>
-      <c r="Q18" s="12"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
+      <c r="L18" s="27"/>
+      <c r="M18" s="27"/>
+      <c r="N18" s="27"/>
+      <c r="O18" s="27"/>
+      <c r="P18" s="27"/>
+      <c r="Q18" s="27"/>
       <c r="R18" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="S18" s="12"/>
-      <c r="T18" s="12"/>
-      <c r="U18" s="12"/>
-      <c r="V18" s="12"/>
-    </row>
-    <row r="19" spans="1:22">
-      <c r="A19" s="11" t="s">
+      <c r="S18" s="27"/>
+      <c r="T18" s="27"/>
+      <c r="U18" s="27"/>
+      <c r="V18" s="27"/>
+    </row>
+    <row r="19" spans="1:22" s="25" customFormat="1">
+      <c r="A19" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="33" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="E19" s="31"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="31"/>
+      <c r="L19" s="31"/>
+      <c r="M19" s="31"/>
+      <c r="N19" s="31"/>
+      <c r="O19" s="31"/>
+      <c r="P19" s="31"/>
+      <c r="Q19" s="31"/>
+      <c r="R19" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="S19" s="31"/>
+      <c r="T19" s="31"/>
+      <c r="U19" s="31"/>
+      <c r="V19" s="31"/>
+    </row>
+    <row r="20" spans="1:22" s="29" customFormat="1" ht="144" customHeight="1">
+      <c r="A20" s="37" t="s">
+        <v>101</v>
+      </c>
+      <c r="B20" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="E20" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="F20" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="G20" s="34" t="s">
+        <v>103</v>
+      </c>
+      <c r="H20" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="I20" s="26"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="L20" s="35"/>
+      <c r="M20" s="27"/>
+      <c r="N20" s="27"/>
+      <c r="O20" s="27"/>
+      <c r="P20" s="27"/>
+      <c r="Q20" s="27"/>
+      <c r="R20" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="S20" s="27"/>
+      <c r="T20" s="27"/>
+      <c r="U20" s="27"/>
+      <c r="V20" s="27"/>
+    </row>
+    <row r="21" spans="1:22" s="29" customFormat="1" ht="27">
+      <c r="A21" s="36" t="s">
+        <v>105</v>
+      </c>
+      <c r="B21" s="26"/>
+      <c r="C21" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D21" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="E21" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="F21" s="28"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="27"/>
+      <c r="M21" s="27"/>
+      <c r="N21" s="27"/>
+      <c r="O21" s="27"/>
+      <c r="P21" s="27"/>
+      <c r="Q21" s="27"/>
+      <c r="R21" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="S21" s="27"/>
+      <c r="T21" s="27"/>
+      <c r="U21" s="27"/>
+      <c r="V21" s="27"/>
+    </row>
+    <row r="22" spans="1:22" s="29" customFormat="1" ht="27">
+      <c r="A22" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="B22" s="26"/>
+      <c r="C22" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D22" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="E22" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="F22" s="28"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="27"/>
+      <c r="M22" s="27"/>
+      <c r="N22" s="27"/>
+      <c r="O22" s="27"/>
+      <c r="P22" s="27"/>
+      <c r="Q22" s="27"/>
+      <c r="R22" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="S22" s="27"/>
+      <c r="T22" s="27"/>
+      <c r="U22" s="27"/>
+      <c r="V22" s="27"/>
+    </row>
+    <row r="23" spans="1:22" s="29" customFormat="1" ht="27">
+      <c r="A23" s="36" t="s">
+        <v>107</v>
+      </c>
+      <c r="B23" s="26"/>
+      <c r="C23" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D23" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="E23" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="F23" s="28"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="27"/>
+      <c r="L23" s="27"/>
+      <c r="M23" s="27"/>
+      <c r="N23" s="27"/>
+      <c r="O23" s="27"/>
+      <c r="P23" s="27"/>
+      <c r="Q23" s="27"/>
+      <c r="R23" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="S23" s="27"/>
+      <c r="T23" s="27"/>
+      <c r="U23" s="27"/>
+      <c r="V23" s="27"/>
+    </row>
+    <row r="24" spans="1:22" s="29" customFormat="1" ht="27">
+      <c r="A24" s="36" t="s">
+        <v>108</v>
+      </c>
+      <c r="B24" s="26"/>
+      <c r="C24" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D24" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="E24" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="F24" s="28"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="27"/>
+      <c r="L24" s="27"/>
+      <c r="M24" s="27"/>
+      <c r="N24" s="27"/>
+      <c r="O24" s="27"/>
+      <c r="P24" s="27"/>
+      <c r="Q24" s="27"/>
+      <c r="R24" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="S24" s="27"/>
+      <c r="T24" s="27"/>
+      <c r="U24" s="27"/>
+      <c r="V24" s="27"/>
+    </row>
+    <row r="25" spans="1:22" s="29" customFormat="1" ht="27">
+      <c r="A25" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="B25" s="26"/>
+      <c r="C25" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D25" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="E25" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="F25" s="28"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="27"/>
+      <c r="L25" s="27"/>
+      <c r="M25" s="27"/>
+      <c r="N25" s="27"/>
+      <c r="O25" s="27"/>
+      <c r="P25" s="27"/>
+      <c r="Q25" s="27"/>
+      <c r="R25" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="S25" s="27"/>
+      <c r="T25" s="27"/>
+      <c r="U25" s="27"/>
+      <c r="V25" s="27"/>
+    </row>
+    <row r="26" spans="1:22" s="29" customFormat="1" ht="27">
+      <c r="A26" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="B26" s="26"/>
+      <c r="C26" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D26" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="E26" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="F26" s="28"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="26"/>
+      <c r="J26" s="27"/>
+      <c r="K26" s="27"/>
+      <c r="L26" s="27"/>
+      <c r="M26" s="27"/>
+      <c r="N26" s="27"/>
+      <c r="O26" s="27"/>
+      <c r="P26" s="27"/>
+      <c r="Q26" s="27"/>
+      <c r="R26" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="S26" s="27"/>
+      <c r="T26" s="27"/>
+      <c r="U26" s="27"/>
+      <c r="V26" s="27"/>
+    </row>
+    <row r="27" spans="1:22" s="29" customFormat="1" ht="27">
+      <c r="A27" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="B27" s="26"/>
+      <c r="C27" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D27" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="E27" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="F27" s="28"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="26"/>
+      <c r="J27" s="27"/>
+      <c r="K27" s="27"/>
+      <c r="L27" s="27"/>
+      <c r="M27" s="27"/>
+      <c r="N27" s="27"/>
+      <c r="O27" s="27"/>
+      <c r="P27" s="27"/>
+      <c r="Q27" s="27"/>
+      <c r="R27" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="S27" s="27"/>
+      <c r="T27" s="27"/>
+      <c r="U27" s="27"/>
+      <c r="V27" s="27"/>
+    </row>
+    <row r="28" spans="1:22" s="29" customFormat="1" ht="27">
+      <c r="A28" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="B28" s="26"/>
+      <c r="C28" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D28" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="E28" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="F28" s="28"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="27"/>
+      <c r="K28" s="27"/>
+      <c r="L28" s="27"/>
+      <c r="M28" s="27"/>
+      <c r="N28" s="27"/>
+      <c r="O28" s="27"/>
+      <c r="P28" s="27"/>
+      <c r="Q28" s="27"/>
+      <c r="R28" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="S28" s="27"/>
+      <c r="T28" s="27"/>
+      <c r="U28" s="27"/>
+      <c r="V28" s="27"/>
+    </row>
+    <row r="29" spans="1:22" s="29" customFormat="1" ht="27">
+      <c r="A29" s="36" t="s">
+        <v>113</v>
+      </c>
+      <c r="B29" s="26"/>
+      <c r="C29" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D29" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="E29" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="F29" s="28"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="27"/>
+      <c r="K29" s="27"/>
+      <c r="L29" s="27"/>
+      <c r="M29" s="27"/>
+      <c r="N29" s="27"/>
+      <c r="O29" s="27"/>
+      <c r="P29" s="27"/>
+      <c r="Q29" s="27"/>
+      <c r="R29" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="S29" s="27"/>
+      <c r="T29" s="27"/>
+      <c r="U29" s="27"/>
+      <c r="V29" s="27"/>
+    </row>
+    <row r="30" spans="1:22" s="29" customFormat="1" ht="27">
+      <c r="A30" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="B30" s="26"/>
+      <c r="C30" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D30" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="E30" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="F30" s="28"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="27"/>
+      <c r="K30" s="27"/>
+      <c r="L30" s="27"/>
+      <c r="M30" s="27"/>
+      <c r="N30" s="27"/>
+      <c r="O30" s="27"/>
+      <c r="P30" s="27"/>
+      <c r="Q30" s="27"/>
+      <c r="R30" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="S30" s="27"/>
+      <c r="T30" s="27"/>
+      <c r="U30" s="27"/>
+      <c r="V30" s="27"/>
+    </row>
+    <row r="31" spans="1:22" s="29" customFormat="1" ht="27">
+      <c r="A31" s="36" t="s">
+        <v>115</v>
+      </c>
+      <c r="B31" s="26"/>
+      <c r="C31" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D31" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="E31" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="F31" s="28"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="27"/>
+      <c r="K31" s="27"/>
+      <c r="L31" s="27"/>
+      <c r="M31" s="27"/>
+      <c r="N31" s="27"/>
+      <c r="O31" s="27"/>
+      <c r="P31" s="27"/>
+      <c r="Q31" s="27"/>
+      <c r="R31" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="S31" s="27"/>
+      <c r="T31" s="27"/>
+      <c r="U31" s="27"/>
+      <c r="V31" s="27"/>
+    </row>
+    <row r="32" spans="1:22" s="29" customFormat="1" ht="27">
+      <c r="A32" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="B32" s="26"/>
+      <c r="C32" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D32" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="E32" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="F32" s="28"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="26"/>
+      <c r="I32" s="26"/>
+      <c r="J32" s="27"/>
+      <c r="K32" s="27"/>
+      <c r="L32" s="27"/>
+      <c r="M32" s="27"/>
+      <c r="N32" s="27"/>
+      <c r="O32" s="27"/>
+      <c r="P32" s="27"/>
+      <c r="Q32" s="27"/>
+      <c r="R32" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="S32" s="27"/>
+      <c r="T32" s="27"/>
+      <c r="U32" s="27"/>
+      <c r="V32" s="27"/>
+    </row>
+    <row r="33" spans="1:22" s="29" customFormat="1" ht="27">
+      <c r="A33" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="B33" s="26"/>
+      <c r="C33" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D33" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="E33" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="F33" s="28"/>
+      <c r="G33" s="26"/>
+      <c r="H33" s="26"/>
+      <c r="I33" s="26"/>
+      <c r="J33" s="27"/>
+      <c r="K33" s="27"/>
+      <c r="L33" s="27"/>
+      <c r="M33" s="27"/>
+      <c r="N33" s="27"/>
+      <c r="O33" s="27"/>
+      <c r="P33" s="27"/>
+      <c r="Q33" s="27"/>
+      <c r="R33" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="S33" s="27"/>
+      <c r="T33" s="27"/>
+      <c r="U33" s="27"/>
+      <c r="V33" s="27"/>
+    </row>
+    <row r="34" spans="1:22" s="29" customFormat="1" ht="27">
+      <c r="A34" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="B34" s="26"/>
+      <c r="C34" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D34" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="E34" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="F34" s="28"/>
+      <c r="G34" s="26"/>
+      <c r="H34" s="26"/>
+      <c r="I34" s="26"/>
+      <c r="J34" s="27"/>
+      <c r="K34" s="27"/>
+      <c r="L34" s="27"/>
+      <c r="M34" s="27"/>
+      <c r="N34" s="27"/>
+      <c r="O34" s="27"/>
+      <c r="P34" s="27"/>
+      <c r="Q34" s="27"/>
+      <c r="R34" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="S34" s="27"/>
+      <c r="T34" s="27"/>
+      <c r="U34" s="27"/>
+      <c r="V34" s="27"/>
+    </row>
+    <row r="35" spans="1:22" s="29" customFormat="1" ht="27">
+      <c r="A35" s="36" t="s">
+        <v>119</v>
+      </c>
+      <c r="B35" s="26"/>
+      <c r="C35" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D35" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="E35" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="F35" s="28"/>
+      <c r="G35" s="26"/>
+      <c r="H35" s="26"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="27"/>
+      <c r="K35" s="27"/>
+      <c r="L35" s="27"/>
+      <c r="M35" s="27"/>
+      <c r="N35" s="27"/>
+      <c r="O35" s="27"/>
+      <c r="P35" s="27"/>
+      <c r="Q35" s="27"/>
+      <c r="R35" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="S35" s="27"/>
+      <c r="T35" s="27"/>
+      <c r="U35" s="27"/>
+      <c r="V35" s="27"/>
+    </row>
+    <row r="36" spans="1:22" s="29" customFormat="1" ht="27">
+      <c r="A36" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="B36" s="26"/>
+      <c r="C36" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D36" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="E36" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="F36" s="28"/>
+      <c r="G36" s="26"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="26"/>
+      <c r="J36" s="27"/>
+      <c r="K36" s="27"/>
+      <c r="L36" s="27"/>
+      <c r="M36" s="27"/>
+      <c r="N36" s="27"/>
+      <c r="O36" s="27"/>
+      <c r="P36" s="27"/>
+      <c r="Q36" s="27"/>
+      <c r="R36" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="S36" s="27"/>
+      <c r="T36" s="27"/>
+      <c r="U36" s="27"/>
+      <c r="V36" s="27"/>
+    </row>
+    <row r="37" spans="1:22" s="29" customFormat="1" ht="27">
+      <c r="A37" s="36" t="s">
+        <v>121</v>
+      </c>
+      <c r="B37" s="26"/>
+      <c r="C37" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D37" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="E37" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="F37" s="28"/>
+      <c r="G37" s="26"/>
+      <c r="H37" s="26"/>
+      <c r="I37" s="26"/>
+      <c r="J37" s="27"/>
+      <c r="K37" s="27"/>
+      <c r="L37" s="27"/>
+      <c r="M37" s="27"/>
+      <c r="N37" s="27"/>
+      <c r="O37" s="27"/>
+      <c r="P37" s="27"/>
+      <c r="Q37" s="27"/>
+      <c r="R37" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="S37" s="27"/>
+      <c r="T37" s="27"/>
+      <c r="U37" s="27"/>
+      <c r="V37" s="27"/>
+    </row>
+    <row r="38" spans="1:22" s="29" customFormat="1" ht="27">
+      <c r="A38" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="B38" s="26"/>
+      <c r="C38" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D38" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="E38" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="F38" s="28"/>
+      <c r="G38" s="26"/>
+      <c r="H38" s="26"/>
+      <c r="I38" s="26"/>
+      <c r="J38" s="27"/>
+      <c r="K38" s="27"/>
+      <c r="L38" s="27"/>
+      <c r="M38" s="27"/>
+      <c r="N38" s="27"/>
+      <c r="O38" s="27"/>
+      <c r="P38" s="27"/>
+      <c r="Q38" s="27"/>
+      <c r="R38" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="S38" s="27"/>
+      <c r="T38" s="27"/>
+      <c r="U38" s="27"/>
+      <c r="V38" s="27"/>
+    </row>
+    <row r="39" spans="1:22" s="29" customFormat="1" ht="27">
+      <c r="A39" s="36" t="s">
+        <v>123</v>
+      </c>
+      <c r="B39" s="26"/>
+      <c r="C39" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D39" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="E39" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="F39" s="28"/>
+      <c r="G39" s="26"/>
+      <c r="H39" s="26"/>
+      <c r="I39" s="26"/>
+      <c r="J39" s="27"/>
+      <c r="K39" s="27"/>
+      <c r="L39" s="27"/>
+      <c r="M39" s="27"/>
+      <c r="N39" s="27"/>
+      <c r="O39" s="27"/>
+      <c r="P39" s="27"/>
+      <c r="Q39" s="27"/>
+      <c r="R39" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="S39" s="27"/>
+      <c r="T39" s="27"/>
+      <c r="U39" s="27"/>
+      <c r="V39" s="27"/>
+    </row>
+    <row r="40" spans="1:22" s="29" customFormat="1" ht="27">
+      <c r="A40" s="36" t="s">
+        <v>124</v>
+      </c>
+      <c r="B40" s="26"/>
+      <c r="C40" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D40" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="E40" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="F40" s="28"/>
+      <c r="G40" s="26"/>
+      <c r="H40" s="26"/>
+      <c r="I40" s="26"/>
+      <c r="J40" s="27"/>
+      <c r="K40" s="27"/>
+      <c r="L40" s="27"/>
+      <c r="M40" s="27"/>
+      <c r="N40" s="27"/>
+      <c r="O40" s="27"/>
+      <c r="P40" s="27"/>
+      <c r="Q40" s="27"/>
+      <c r="R40" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="S40" s="27"/>
+      <c r="T40" s="27"/>
+      <c r="U40" s="27"/>
+      <c r="V40" s="27"/>
+    </row>
+    <row r="41" spans="1:22">
+      <c r="A41" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="B41" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="C19" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="D19" s="11" t="s">
+      <c r="C41" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D41" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="E19" s="12"/>
-      <c r="F19" s="20" t="str">
+      <c r="E41" s="12"/>
+      <c r="F41" s="20" t="str">
         <f t="shared" si="0"/>
         <v>household.save</v>
       </c>
-      <c r="G19" s="11" t="s">
+      <c r="G41" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="H19" s="11" t="s">
+      <c r="H41" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="I19" s="11"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="12"/>
-      <c r="M19" s="12"/>
-      <c r="N19" s="12"/>
-      <c r="O19" s="12"/>
-      <c r="P19" s="12"/>
-      <c r="Q19" s="12"/>
-      <c r="R19" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="S19" s="12"/>
-      <c r="T19" s="12"/>
-      <c r="U19" s="12"/>
-      <c r="V19" s="12"/>
-    </row>
-    <row r="20" spans="1:22" ht="130.5">
-      <c r="A20" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="B20" s="9" t="s">
+      <c r="I41" s="11"/>
+      <c r="J41" s="12"/>
+      <c r="K41" s="12"/>
+      <c r="L41" s="12"/>
+      <c r="M41" s="12"/>
+      <c r="N41" s="12"/>
+      <c r="O41" s="12"/>
+      <c r="P41" s="12"/>
+      <c r="Q41" s="12"/>
+      <c r="R41" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="S41" s="12"/>
+      <c r="T41" s="12"/>
+      <c r="U41" s="12"/>
+      <c r="V41" s="12"/>
+    </row>
+    <row r="42" spans="1:22" ht="130.5">
+      <c r="A42" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="B42" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="J20" s="24"/>
-      <c r="K20" s="22"/>
-      <c r="R20" s="9" t="b">
+      <c r="C42" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="H42" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="J42" s="24"/>
+      <c r="K42" s="22"/>
+      <c r="R42" s="9" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C21:C1048576 C1:C19">
+  <conditionalFormatting sqref="C43:C1048576 C1:C41">
     <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C21:C1048576 C1:C19">
+  <conditionalFormatting sqref="C43:C1048576 C1:C41">
     <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C20">
+  <conditionalFormatting sqref="C42">
     <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",C20)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FALSE",C42)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",C20)))</formula>
+      <formula>NOT(ISERROR(SEARCH("TRUE",C42)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L20:O20">
+  <conditionalFormatting sqref="L42:O42">
     <cfRule type="expression" dxfId="2" priority="1">
-      <formula>AND($B1048348="Custom",  $B1048348&lt;&gt;"", ROW(L1048348)&lt;&gt;1)</formula>
+      <formula>AND($B1048370="Custom",  $B1048370&lt;&gt;"", ROW(L1048370)&lt;&gt;1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M20:N20">
+  <conditionalFormatting sqref="M42:N42">
     <cfRule type="expression" dxfId="1" priority="5">
-      <formula>AND($B20&lt;&gt;"Select", $B20&lt;&gt;"Checkbox", $B20&lt;&gt;"Radio",  $B20&lt;&gt;"", ROW(M20)&lt;&gt;1)</formula>
+      <formula>AND($B42&lt;&gt;"Select", $B42&lt;&gt;"Checkbox", $B42&lt;&gt;"Radio",  $B42&lt;&gt;"", ROW(M42)&lt;&gt;1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O20">
+  <conditionalFormatting sqref="O42">
     <cfRule type="expression" dxfId="0" priority="2">
-      <formula>AND($B20&lt;&gt;"Range", $B20&lt;&gt;"", ROW(O20)&lt;&gt;1)</formula>
+      <formula>AND($B42&lt;&gt;"Range", $B42&lt;&gt;"", ROW(O42)&lt;&gt;1)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2109,7 +3008,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2124,34 +3023,34 @@
   <sheetData>
     <row r="1" spans="1:6" s="6" customFormat="1">
       <c r="A1" s="16" t="s">
-        <v>105</v>
+        <v>130</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>106</v>
+        <v>131</v>
       </c>
       <c r="C1" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>107</v>
+        <v>132</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>108</v>
+        <v>133</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>109</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="29.25">
       <c r="A2" s="14" t="s">
-        <v>110</v>
+        <v>135</v>
       </c>
       <c r="B2" s="14"/>
       <c r="C2" s="14" t="s">
-        <v>111</v>
+        <v>136</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>112</v>
+        <v>137</v>
       </c>
       <c r="E2" s="14">
         <v>1</v>
@@ -2164,10 +3063,10 @@
       </c>
       <c r="B3" s="14"/>
       <c r="C3" s="14" t="s">
-        <v>111</v>
+        <v>136</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>113</v>
+        <v>138</v>
       </c>
       <c r="E3" s="14">
         <v>2</v>
@@ -2184,7 +3083,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
@@ -2204,25 +3103,25 @@
         <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>114</v>
+        <v>139</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>115</v>
+        <v>140</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>116</v>
+        <v>141</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>118</v>
+        <v>143</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>119</v>
+        <v>144</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>120</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -2230,13 +3129,13 @@
         <v>24</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>121</v>
+        <v>146</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>123</v>
+        <v>148</v>
       </c>
       <c r="E2" s="14" t="b">
         <v>1</v>
@@ -2253,13 +3152,13 @@
         <v>100</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>126</v>
+        <v>151</v>
       </c>
       <c r="E3" s="14" t="b">
         <v>1</v>
@@ -2273,16 +3172,16 @@
     </row>
     <row r="4" spans="1:8" ht="29.25">
       <c r="A4" s="14" t="s">
-        <v>102</v>
+        <v>127</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>127</v>
+        <v>152</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>128</v>
+        <v>153</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>129</v>
+        <v>154</v>
       </c>
       <c r="E4" s="14" t="b">
         <v>0</v>
@@ -2319,10 +3218,10 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="3" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>108</v>
+        <v>133</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>6</v>
@@ -2331,7 +3230,7 @@
         <v>7</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>10</v>
@@ -2339,72 +3238,72 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>132</v>
+        <v>157</v>
       </c>
       <c r="B2" t="s">
-        <v>132</v>
+        <v>157</v>
       </c>
       <c r="C2" t="s">
-        <v>133</v>
+        <v>158</v>
       </c>
       <c r="D2" t="s">
-        <v>134</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>135</v>
+        <v>160</v>
       </c>
       <c r="B3" t="s">
-        <v>135</v>
+        <v>160</v>
       </c>
       <c r="C3" t="s">
-        <v>136</v>
+        <v>161</v>
       </c>
       <c r="D3" t="s">
-        <v>137</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>163</v>
       </c>
       <c r="B4" t="s">
-        <v>138</v>
+        <v>163</v>
       </c>
       <c r="C4" t="s">
-        <v>139</v>
+        <v>164</v>
       </c>
       <c r="D4" t="s">
-        <v>140</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>141</v>
+        <v>166</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>141</v>
+        <v>166</v>
       </c>
       <c r="C5" t="s">
-        <v>142</v>
+        <v>167</v>
       </c>
       <c r="D5" t="s">
-        <v>143</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>144</v>
+        <v>169</v>
       </c>
       <c r="B6" t="s">
-        <v>144</v>
+        <v>169</v>
       </c>
       <c r="C6" t="s">
-        <v>145</v>
+        <v>170</v>
       </c>
       <c r="D6" t="s">
-        <v>146</v>
+        <v>171</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2412,7 +3311,7 @@
         <v>31</v>
       </c>
       <c r="E7" t="s">
-        <v>132</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2420,12 +3319,12 @@
         <v>31</v>
       </c>
       <c r="E8" t="s">
-        <v>135</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>147</v>
+        <v>172</v>
       </c>
       <c r="E9" t="s">
         <v>31</v>
@@ -2433,10 +3332,10 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>147</v>
+        <v>172</v>
       </c>
       <c r="E10" t="s">
-        <v>141</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2444,7 +3343,7 @@
         <v>94</v>
       </c>
       <c r="E11" t="s">
-        <v>132</v>
+        <v>157</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2452,7 +3351,7 @@
         <v>94</v>
       </c>
       <c r="E12" t="s">
-        <v>135</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2460,7 +3359,7 @@
         <v>94</v>
       </c>
       <c r="E13" t="s">
-        <v>144</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -2492,40 +3391,40 @@
   <sheetData>
     <row r="1" spans="1:12" s="5" customFormat="1">
       <c r="A1" s="4" t="s">
-        <v>148</v>
+        <v>173</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>149</v>
+        <v>174</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>150</v>
+        <v>175</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>151</v>
+        <v>176</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>152</v>
+        <v>177</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>153</v>
+        <v>178</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>154</v>
+        <v>179</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>155</v>
+        <v>180</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>156</v>
+        <v>181</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>157</v>
+        <v>182</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>158</v>
+        <v>183</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>159</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -2545,19 +3444,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>160</v>
+        <v>185</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>161</v>
+        <v>186</v>
       </c>
       <c r="D1" t="s">
         <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>162</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BREAKING POINT: Rename preload to customPreload
Add some customPreload to the Demo_Generator.
Add the function countAdults and some tests in the helper.
Add preload for each section, because we need to call the customPreloadBase in each section.
BREAKING POINT: You need to rename each preload to customPreload in each survey.
</commit_message>
<xml_diff>
--- a/example/demo_generator/references/Household_Travel_Generate_Survey.xlsx
+++ b/example/demo_generator/references/Household_Travel_Generate_Survey.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28922"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28926"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="681" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB5A37E8-8767-4056-91CD-F7CE27EF0031}"/>
+  <xr:revisionPtr revIDLastSave="684" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD6D3077-663E-4E58-A164-1387DA22EFF7}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Widgets" sheetId="1" r:id="rId1"/>
@@ -780,7 +780,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -855,16 +855,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -879,19 +870,13 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1301,9 +1286,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="I20" sqref="I20"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="N20" sqref="N20"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -2110,8 +2095,8 @@
       <c r="D18" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="27"/>
-      <c r="F18" s="28" t="str">
+      <c r="E18" s="10"/>
+      <c r="F18" s="7" t="str">
         <f t="shared" si="0"/>
         <v>home.save</v>
       </c>
@@ -2122,779 +2107,779 @@
         <v>98</v>
       </c>
       <c r="I18" s="26"/>
-      <c r="J18" s="27"/>
-      <c r="K18" s="27"/>
-      <c r="L18" s="27"/>
-      <c r="M18" s="27"/>
-      <c r="N18" s="27"/>
-      <c r="O18" s="27"/>
-      <c r="P18" s="27"/>
-      <c r="Q18" s="27"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10"/>
       <c r="R18" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="S18" s="27"/>
-      <c r="T18" s="27"/>
-      <c r="U18" s="27"/>
-      <c r="V18" s="27"/>
+      <c r="S18" s="10"/>
+      <c r="T18" s="10"/>
+      <c r="U18" s="10"/>
+      <c r="V18" s="10"/>
     </row>
     <row r="19" spans="1:22" s="25" customFormat="1">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="C19" s="33" t="b">
-        <v>1</v>
-      </c>
-      <c r="D19" s="34" t="s">
+      <c r="C19" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="E19" s="31"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="30"/>
-      <c r="H19" s="30"/>
-      <c r="I19" s="30"/>
-      <c r="J19" s="31"/>
-      <c r="K19" s="31"/>
-      <c r="L19" s="31"/>
-      <c r="M19" s="31"/>
-      <c r="N19" s="31"/>
-      <c r="O19" s="31"/>
-      <c r="P19" s="31"/>
-      <c r="Q19" s="31"/>
-      <c r="R19" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="S19" s="31"/>
-      <c r="T19" s="31"/>
-      <c r="U19" s="31"/>
-      <c r="V19" s="31"/>
-    </row>
-    <row r="20" spans="1:22" s="29" customFormat="1" ht="144" customHeight="1">
-      <c r="A20" s="37" t="s">
+      <c r="E19" s="28"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="28"/>
+      <c r="M19" s="28"/>
+      <c r="N19" s="28"/>
+      <c r="O19" s="28"/>
+      <c r="P19" s="28"/>
+      <c r="Q19" s="28"/>
+      <c r="R19" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="S19" s="28"/>
+      <c r="T19" s="28"/>
+      <c r="U19" s="28"/>
+      <c r="V19" s="28"/>
+    </row>
+    <row r="20" spans="1:22" ht="144" customHeight="1">
+      <c r="A20" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="D20" s="34" t="s">
+      <c r="C20" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="E20" s="27" t="s">
+      <c r="E20" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="F20" s="28" t="s">
+      <c r="F20" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="G20" s="34" t="s">
+      <c r="G20" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="H20" s="38" t="s">
+      <c r="H20" s="33" t="s">
         <v>104</v>
       </c>
       <c r="I20" s="26"/>
-      <c r="J20" s="27"/>
-      <c r="K20" s="27" t="s">
+      <c r="J20" s="10"/>
+      <c r="K20" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="L20" s="35"/>
-      <c r="M20" s="27"/>
-      <c r="N20" s="27"/>
-      <c r="O20" s="27"/>
-      <c r="P20" s="27"/>
-      <c r="Q20" s="27"/>
-      <c r="R20" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="S20" s="27"/>
-      <c r="T20" s="27"/>
-      <c r="U20" s="27"/>
-      <c r="V20" s="27"/>
-    </row>
-    <row r="21" spans="1:22" s="29" customFormat="1" ht="27">
-      <c r="A21" s="36" t="s">
+      <c r="L20" s="13"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="S20" s="10"/>
+      <c r="T20" s="10"/>
+      <c r="U20" s="10"/>
+      <c r="V20" s="10"/>
+    </row>
+    <row r="21" spans="1:22" ht="27">
+      <c r="A21" s="32" t="s">
         <v>105</v>
       </c>
       <c r="B21" s="26"/>
-      <c r="C21" s="34" t="b">
+      <c r="C21" s="31" t="b">
         <v>0</v>
       </c>
-      <c r="D21" s="34" t="s">
+      <c r="D21" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="E21" s="27" t="s">
+      <c r="E21" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="F21" s="28"/>
+      <c r="F21" s="7"/>
       <c r="G21" s="26"/>
       <c r="H21" s="26"/>
       <c r="I21" s="26"/>
-      <c r="J21" s="27"/>
-      <c r="K21" s="27"/>
-      <c r="L21" s="27"/>
-      <c r="M21" s="27"/>
-      <c r="N21" s="27"/>
-      <c r="O21" s="27"/>
-      <c r="P21" s="27"/>
-      <c r="Q21" s="27"/>
-      <c r="R21" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="S21" s="27"/>
-      <c r="T21" s="27"/>
-      <c r="U21" s="27"/>
-      <c r="V21" s="27"/>
-    </row>
-    <row r="22" spans="1:22" s="29" customFormat="1" ht="27">
-      <c r="A22" s="36" t="s">
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="S21" s="10"/>
+      <c r="T21" s="10"/>
+      <c r="U21" s="10"/>
+      <c r="V21" s="10"/>
+    </row>
+    <row r="22" spans="1:22" ht="27">
+      <c r="A22" s="32" t="s">
         <v>106</v>
       </c>
       <c r="B22" s="26"/>
-      <c r="C22" s="34" t="b">
+      <c r="C22" s="31" t="b">
         <v>0</v>
       </c>
-      <c r="D22" s="34" t="s">
+      <c r="D22" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="E22" s="27" t="s">
+      <c r="E22" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="F22" s="28"/>
+      <c r="F22" s="7"/>
       <c r="G22" s="26"/>
       <c r="H22" s="26"/>
       <c r="I22" s="26"/>
-      <c r="J22" s="27"/>
-      <c r="K22" s="27"/>
-      <c r="L22" s="27"/>
-      <c r="M22" s="27"/>
-      <c r="N22" s="27"/>
-      <c r="O22" s="27"/>
-      <c r="P22" s="27"/>
-      <c r="Q22" s="27"/>
-      <c r="R22" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="S22" s="27"/>
-      <c r="T22" s="27"/>
-      <c r="U22" s="27"/>
-      <c r="V22" s="27"/>
-    </row>
-    <row r="23" spans="1:22" s="29" customFormat="1" ht="27">
-      <c r="A23" s="36" t="s">
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="S22" s="10"/>
+      <c r="T22" s="10"/>
+      <c r="U22" s="10"/>
+      <c r="V22" s="10"/>
+    </row>
+    <row r="23" spans="1:22" ht="27">
+      <c r="A23" s="32" t="s">
         <v>107</v>
       </c>
       <c r="B23" s="26"/>
-      <c r="C23" s="34" t="b">
+      <c r="C23" s="31" t="b">
         <v>0</v>
       </c>
-      <c r="D23" s="34" t="s">
+      <c r="D23" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="E23" s="27" t="s">
+      <c r="E23" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="F23" s="28"/>
+      <c r="F23" s="7"/>
       <c r="G23" s="26"/>
       <c r="H23" s="26"/>
       <c r="I23" s="26"/>
-      <c r="J23" s="27"/>
-      <c r="K23" s="27"/>
-      <c r="L23" s="27"/>
-      <c r="M23" s="27"/>
-      <c r="N23" s="27"/>
-      <c r="O23" s="27"/>
-      <c r="P23" s="27"/>
-      <c r="Q23" s="27"/>
-      <c r="R23" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="S23" s="27"/>
-      <c r="T23" s="27"/>
-      <c r="U23" s="27"/>
-      <c r="V23" s="27"/>
-    </row>
-    <row r="24" spans="1:22" s="29" customFormat="1" ht="27">
-      <c r="A24" s="36" t="s">
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+      <c r="R23" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="S23" s="10"/>
+      <c r="T23" s="10"/>
+      <c r="U23" s="10"/>
+      <c r="V23" s="10"/>
+    </row>
+    <row r="24" spans="1:22" ht="27">
+      <c r="A24" s="32" t="s">
         <v>108</v>
       </c>
       <c r="B24" s="26"/>
-      <c r="C24" s="34" t="b">
+      <c r="C24" s="31" t="b">
         <v>0</v>
       </c>
-      <c r="D24" s="34" t="s">
+      <c r="D24" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="E24" s="27" t="s">
+      <c r="E24" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="F24" s="28"/>
+      <c r="F24" s="7"/>
       <c r="G24" s="26"/>
       <c r="H24" s="26"/>
       <c r="I24" s="26"/>
-      <c r="J24" s="27"/>
-      <c r="K24" s="27"/>
-      <c r="L24" s="27"/>
-      <c r="M24" s="27"/>
-      <c r="N24" s="27"/>
-      <c r="O24" s="27"/>
-      <c r="P24" s="27"/>
-      <c r="Q24" s="27"/>
-      <c r="R24" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="S24" s="27"/>
-      <c r="T24" s="27"/>
-      <c r="U24" s="27"/>
-      <c r="V24" s="27"/>
-    </row>
-    <row r="25" spans="1:22" s="29" customFormat="1" ht="27">
-      <c r="A25" s="36" t="s">
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10"/>
+      <c r="R24" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="S24" s="10"/>
+      <c r="T24" s="10"/>
+      <c r="U24" s="10"/>
+      <c r="V24" s="10"/>
+    </row>
+    <row r="25" spans="1:22" ht="27">
+      <c r="A25" s="32" t="s">
         <v>109</v>
       </c>
       <c r="B25" s="26"/>
-      <c r="C25" s="34" t="b">
+      <c r="C25" s="31" t="b">
         <v>0</v>
       </c>
-      <c r="D25" s="34" t="s">
+      <c r="D25" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="E25" s="27" t="s">
+      <c r="E25" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="F25" s="28"/>
+      <c r="F25" s="7"/>
       <c r="G25" s="26"/>
       <c r="H25" s="26"/>
       <c r="I25" s="26"/>
-      <c r="J25" s="27"/>
-      <c r="K25" s="27"/>
-      <c r="L25" s="27"/>
-      <c r="M25" s="27"/>
-      <c r="N25" s="27"/>
-      <c r="O25" s="27"/>
-      <c r="P25" s="27"/>
-      <c r="Q25" s="27"/>
-      <c r="R25" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="S25" s="27"/>
-      <c r="T25" s="27"/>
-      <c r="U25" s="27"/>
-      <c r="V25" s="27"/>
-    </row>
-    <row r="26" spans="1:22" s="29" customFormat="1" ht="27">
-      <c r="A26" s="36" t="s">
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="10"/>
+      <c r="R25" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="S25" s="10"/>
+      <c r="T25" s="10"/>
+      <c r="U25" s="10"/>
+      <c r="V25" s="10"/>
+    </row>
+    <row r="26" spans="1:22" ht="27">
+      <c r="A26" s="32" t="s">
         <v>110</v>
       </c>
       <c r="B26" s="26"/>
-      <c r="C26" s="34" t="b">
+      <c r="C26" s="31" t="b">
         <v>0</v>
       </c>
-      <c r="D26" s="34" t="s">
+      <c r="D26" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="E26" s="27" t="s">
+      <c r="E26" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="F26" s="28"/>
+      <c r="F26" s="7"/>
       <c r="G26" s="26"/>
       <c r="H26" s="26"/>
       <c r="I26" s="26"/>
-      <c r="J26" s="27"/>
-      <c r="K26" s="27"/>
-      <c r="L26" s="27"/>
-      <c r="M26" s="27"/>
-      <c r="N26" s="27"/>
-      <c r="O26" s="27"/>
-      <c r="P26" s="27"/>
-      <c r="Q26" s="27"/>
-      <c r="R26" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="S26" s="27"/>
-      <c r="T26" s="27"/>
-      <c r="U26" s="27"/>
-      <c r="V26" s="27"/>
-    </row>
-    <row r="27" spans="1:22" s="29" customFormat="1" ht="27">
-      <c r="A27" s="36" t="s">
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="10"/>
+      <c r="R26" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="S26" s="10"/>
+      <c r="T26" s="10"/>
+      <c r="U26" s="10"/>
+      <c r="V26" s="10"/>
+    </row>
+    <row r="27" spans="1:22" ht="27">
+      <c r="A27" s="32" t="s">
         <v>111</v>
       </c>
       <c r="B27" s="26"/>
-      <c r="C27" s="34" t="b">
+      <c r="C27" s="31" t="b">
         <v>0</v>
       </c>
-      <c r="D27" s="34" t="s">
+      <c r="D27" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="E27" s="27" t="s">
+      <c r="E27" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="F27" s="28"/>
+      <c r="F27" s="7"/>
       <c r="G27" s="26"/>
       <c r="H27" s="26"/>
       <c r="I27" s="26"/>
-      <c r="J27" s="27"/>
-      <c r="K27" s="27"/>
-      <c r="L27" s="27"/>
-      <c r="M27" s="27"/>
-      <c r="N27" s="27"/>
-      <c r="O27" s="27"/>
-      <c r="P27" s="27"/>
-      <c r="Q27" s="27"/>
-      <c r="R27" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="S27" s="27"/>
-      <c r="T27" s="27"/>
-      <c r="U27" s="27"/>
-      <c r="V27" s="27"/>
-    </row>
-    <row r="28" spans="1:22" s="29" customFormat="1" ht="27">
-      <c r="A28" s="36" t="s">
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="10"/>
+      <c r="R27" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="S27" s="10"/>
+      <c r="T27" s="10"/>
+      <c r="U27" s="10"/>
+      <c r="V27" s="10"/>
+    </row>
+    <row r="28" spans="1:22" ht="27">
+      <c r="A28" s="32" t="s">
         <v>112</v>
       </c>
       <c r="B28" s="26"/>
-      <c r="C28" s="34" t="b">
+      <c r="C28" s="31" t="b">
         <v>0</v>
       </c>
-      <c r="D28" s="34" t="s">
+      <c r="D28" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="E28" s="27" t="s">
+      <c r="E28" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="F28" s="28"/>
+      <c r="F28" s="7"/>
       <c r="G28" s="26"/>
       <c r="H28" s="26"/>
       <c r="I28" s="26"/>
-      <c r="J28" s="27"/>
-      <c r="K28" s="27"/>
-      <c r="L28" s="27"/>
-      <c r="M28" s="27"/>
-      <c r="N28" s="27"/>
-      <c r="O28" s="27"/>
-      <c r="P28" s="27"/>
-      <c r="Q28" s="27"/>
-      <c r="R28" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="S28" s="27"/>
-      <c r="T28" s="27"/>
-      <c r="U28" s="27"/>
-      <c r="V28" s="27"/>
-    </row>
-    <row r="29" spans="1:22" s="29" customFormat="1" ht="27">
-      <c r="A29" s="36" t="s">
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="10"/>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="10"/>
+      <c r="R28" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="S28" s="10"/>
+      <c r="T28" s="10"/>
+      <c r="U28" s="10"/>
+      <c r="V28" s="10"/>
+    </row>
+    <row r="29" spans="1:22" ht="27">
+      <c r="A29" s="32" t="s">
         <v>113</v>
       </c>
       <c r="B29" s="26"/>
-      <c r="C29" s="34" t="b">
+      <c r="C29" s="31" t="b">
         <v>0</v>
       </c>
-      <c r="D29" s="34" t="s">
+      <c r="D29" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="E29" s="27" t="s">
+      <c r="E29" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="F29" s="28"/>
+      <c r="F29" s="7"/>
       <c r="G29" s="26"/>
       <c r="H29" s="26"/>
       <c r="I29" s="26"/>
-      <c r="J29" s="27"/>
-      <c r="K29" s="27"/>
-      <c r="L29" s="27"/>
-      <c r="M29" s="27"/>
-      <c r="N29" s="27"/>
-      <c r="O29" s="27"/>
-      <c r="P29" s="27"/>
-      <c r="Q29" s="27"/>
-      <c r="R29" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="S29" s="27"/>
-      <c r="T29" s="27"/>
-      <c r="U29" s="27"/>
-      <c r="V29" s="27"/>
-    </row>
-    <row r="30" spans="1:22" s="29" customFormat="1" ht="27">
-      <c r="A30" s="36" t="s">
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="10"/>
+      <c r="N29" s="10"/>
+      <c r="O29" s="10"/>
+      <c r="P29" s="10"/>
+      <c r="Q29" s="10"/>
+      <c r="R29" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="S29" s="10"/>
+      <c r="T29" s="10"/>
+      <c r="U29" s="10"/>
+      <c r="V29" s="10"/>
+    </row>
+    <row r="30" spans="1:22" ht="27">
+      <c r="A30" s="32" t="s">
         <v>114</v>
       </c>
       <c r="B30" s="26"/>
-      <c r="C30" s="34" t="b">
+      <c r="C30" s="31" t="b">
         <v>0</v>
       </c>
-      <c r="D30" s="34" t="s">
+      <c r="D30" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="E30" s="27" t="s">
+      <c r="E30" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="F30" s="28"/>
+      <c r="F30" s="7"/>
       <c r="G30" s="26"/>
       <c r="H30" s="26"/>
       <c r="I30" s="26"/>
-      <c r="J30" s="27"/>
-      <c r="K30" s="27"/>
-      <c r="L30" s="27"/>
-      <c r="M30" s="27"/>
-      <c r="N30" s="27"/>
-      <c r="O30" s="27"/>
-      <c r="P30" s="27"/>
-      <c r="Q30" s="27"/>
-      <c r="R30" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="S30" s="27"/>
-      <c r="T30" s="27"/>
-      <c r="U30" s="27"/>
-      <c r="V30" s="27"/>
-    </row>
-    <row r="31" spans="1:22" s="29" customFormat="1" ht="27">
-      <c r="A31" s="36" t="s">
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
+      <c r="N30" s="10"/>
+      <c r="O30" s="10"/>
+      <c r="P30" s="10"/>
+      <c r="Q30" s="10"/>
+      <c r="R30" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="S30" s="10"/>
+      <c r="T30" s="10"/>
+      <c r="U30" s="10"/>
+      <c r="V30" s="10"/>
+    </row>
+    <row r="31" spans="1:22" ht="27">
+      <c r="A31" s="32" t="s">
         <v>115</v>
       </c>
       <c r="B31" s="26"/>
-      <c r="C31" s="34" t="b">
+      <c r="C31" s="31" t="b">
         <v>0</v>
       </c>
-      <c r="D31" s="34" t="s">
+      <c r="D31" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="E31" s="27" t="s">
+      <c r="E31" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="F31" s="28"/>
+      <c r="F31" s="7"/>
       <c r="G31" s="26"/>
       <c r="H31" s="26"/>
       <c r="I31" s="26"/>
-      <c r="J31" s="27"/>
-      <c r="K31" s="27"/>
-      <c r="L31" s="27"/>
-      <c r="M31" s="27"/>
-      <c r="N31" s="27"/>
-      <c r="O31" s="27"/>
-      <c r="P31" s="27"/>
-      <c r="Q31" s="27"/>
-      <c r="R31" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="S31" s="27"/>
-      <c r="T31" s="27"/>
-      <c r="U31" s="27"/>
-      <c r="V31" s="27"/>
-    </row>
-    <row r="32" spans="1:22" s="29" customFormat="1" ht="27">
-      <c r="A32" s="36" t="s">
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="10"/>
+      <c r="N31" s="10"/>
+      <c r="O31" s="10"/>
+      <c r="P31" s="10"/>
+      <c r="Q31" s="10"/>
+      <c r="R31" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="S31" s="10"/>
+      <c r="T31" s="10"/>
+      <c r="U31" s="10"/>
+      <c r="V31" s="10"/>
+    </row>
+    <row r="32" spans="1:22" ht="27">
+      <c r="A32" s="32" t="s">
         <v>116</v>
       </c>
       <c r="B32" s="26"/>
-      <c r="C32" s="34" t="b">
+      <c r="C32" s="31" t="b">
         <v>0</v>
       </c>
-      <c r="D32" s="34" t="s">
+      <c r="D32" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="E32" s="27" t="s">
+      <c r="E32" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="F32" s="28"/>
+      <c r="F32" s="7"/>
       <c r="G32" s="26"/>
       <c r="H32" s="26"/>
       <c r="I32" s="26"/>
-      <c r="J32" s="27"/>
-      <c r="K32" s="27"/>
-      <c r="L32" s="27"/>
-      <c r="M32" s="27"/>
-      <c r="N32" s="27"/>
-      <c r="O32" s="27"/>
-      <c r="P32" s="27"/>
-      <c r="Q32" s="27"/>
-      <c r="R32" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="S32" s="27"/>
-      <c r="T32" s="27"/>
-      <c r="U32" s="27"/>
-      <c r="V32" s="27"/>
-    </row>
-    <row r="33" spans="1:22" s="29" customFormat="1" ht="27">
-      <c r="A33" s="36" t="s">
+      <c r="J32" s="10"/>
+      <c r="K32" s="10"/>
+      <c r="L32" s="10"/>
+      <c r="M32" s="10"/>
+      <c r="N32" s="10"/>
+      <c r="O32" s="10"/>
+      <c r="P32" s="10"/>
+      <c r="Q32" s="10"/>
+      <c r="R32" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="S32" s="10"/>
+      <c r="T32" s="10"/>
+      <c r="U32" s="10"/>
+      <c r="V32" s="10"/>
+    </row>
+    <row r="33" spans="1:22" ht="27">
+      <c r="A33" s="32" t="s">
         <v>117</v>
       </c>
       <c r="B33" s="26"/>
-      <c r="C33" s="34" t="b">
+      <c r="C33" s="31" t="b">
         <v>0</v>
       </c>
-      <c r="D33" s="34" t="s">
+      <c r="D33" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="E33" s="27" t="s">
+      <c r="E33" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="F33" s="28"/>
+      <c r="F33" s="7"/>
       <c r="G33" s="26"/>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
-      <c r="J33" s="27"/>
-      <c r="K33" s="27"/>
-      <c r="L33" s="27"/>
-      <c r="M33" s="27"/>
-      <c r="N33" s="27"/>
-      <c r="O33" s="27"/>
-      <c r="P33" s="27"/>
-      <c r="Q33" s="27"/>
-      <c r="R33" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="S33" s="27"/>
-      <c r="T33" s="27"/>
-      <c r="U33" s="27"/>
-      <c r="V33" s="27"/>
-    </row>
-    <row r="34" spans="1:22" s="29" customFormat="1" ht="27">
-      <c r="A34" s="36" t="s">
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="10"/>
+      <c r="M33" s="10"/>
+      <c r="N33" s="10"/>
+      <c r="O33" s="10"/>
+      <c r="P33" s="10"/>
+      <c r="Q33" s="10"/>
+      <c r="R33" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="S33" s="10"/>
+      <c r="T33" s="10"/>
+      <c r="U33" s="10"/>
+      <c r="V33" s="10"/>
+    </row>
+    <row r="34" spans="1:22" ht="27">
+      <c r="A34" s="32" t="s">
         <v>118</v>
       </c>
       <c r="B34" s="26"/>
-      <c r="C34" s="34" t="b">
+      <c r="C34" s="31" t="b">
         <v>0</v>
       </c>
-      <c r="D34" s="34" t="s">
+      <c r="D34" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="E34" s="27" t="s">
+      <c r="E34" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="F34" s="28"/>
+      <c r="F34" s="7"/>
       <c r="G34" s="26"/>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
-      <c r="J34" s="27"/>
-      <c r="K34" s="27"/>
-      <c r="L34" s="27"/>
-      <c r="M34" s="27"/>
-      <c r="N34" s="27"/>
-      <c r="O34" s="27"/>
-      <c r="P34" s="27"/>
-      <c r="Q34" s="27"/>
-      <c r="R34" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="S34" s="27"/>
-      <c r="T34" s="27"/>
-      <c r="U34" s="27"/>
-      <c r="V34" s="27"/>
-    </row>
-    <row r="35" spans="1:22" s="29" customFormat="1" ht="27">
-      <c r="A35" s="36" t="s">
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
+      <c r="L34" s="10"/>
+      <c r="M34" s="10"/>
+      <c r="N34" s="10"/>
+      <c r="O34" s="10"/>
+      <c r="P34" s="10"/>
+      <c r="Q34" s="10"/>
+      <c r="R34" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="S34" s="10"/>
+      <c r="T34" s="10"/>
+      <c r="U34" s="10"/>
+      <c r="V34" s="10"/>
+    </row>
+    <row r="35" spans="1:22" ht="27">
+      <c r="A35" s="32" t="s">
         <v>119</v>
       </c>
       <c r="B35" s="26"/>
-      <c r="C35" s="34" t="b">
+      <c r="C35" s="31" t="b">
         <v>0</v>
       </c>
-      <c r="D35" s="34" t="s">
+      <c r="D35" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="E35" s="27" t="s">
+      <c r="E35" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="F35" s="28"/>
+      <c r="F35" s="7"/>
       <c r="G35" s="26"/>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
-      <c r="J35" s="27"/>
-      <c r="K35" s="27"/>
-      <c r="L35" s="27"/>
-      <c r="M35" s="27"/>
-      <c r="N35" s="27"/>
-      <c r="O35" s="27"/>
-      <c r="P35" s="27"/>
-      <c r="Q35" s="27"/>
-      <c r="R35" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="S35" s="27"/>
-      <c r="T35" s="27"/>
-      <c r="U35" s="27"/>
-      <c r="V35" s="27"/>
-    </row>
-    <row r="36" spans="1:22" s="29" customFormat="1" ht="27">
-      <c r="A36" s="36" t="s">
+      <c r="J35" s="10"/>
+      <c r="K35" s="10"/>
+      <c r="L35" s="10"/>
+      <c r="M35" s="10"/>
+      <c r="N35" s="10"/>
+      <c r="O35" s="10"/>
+      <c r="P35" s="10"/>
+      <c r="Q35" s="10"/>
+      <c r="R35" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="S35" s="10"/>
+      <c r="T35" s="10"/>
+      <c r="U35" s="10"/>
+      <c r="V35" s="10"/>
+    </row>
+    <row r="36" spans="1:22" ht="27">
+      <c r="A36" s="32" t="s">
         <v>120</v>
       </c>
       <c r="B36" s="26"/>
-      <c r="C36" s="34" t="b">
+      <c r="C36" s="31" t="b">
         <v>0</v>
       </c>
-      <c r="D36" s="34" t="s">
+      <c r="D36" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="E36" s="27" t="s">
+      <c r="E36" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="F36" s="28"/>
+      <c r="F36" s="7"/>
       <c r="G36" s="26"/>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
-      <c r="J36" s="27"/>
-      <c r="K36" s="27"/>
-      <c r="L36" s="27"/>
-      <c r="M36" s="27"/>
-      <c r="N36" s="27"/>
-      <c r="O36" s="27"/>
-      <c r="P36" s="27"/>
-      <c r="Q36" s="27"/>
-      <c r="R36" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="S36" s="27"/>
-      <c r="T36" s="27"/>
-      <c r="U36" s="27"/>
-      <c r="V36" s="27"/>
-    </row>
-    <row r="37" spans="1:22" s="29" customFormat="1" ht="27">
-      <c r="A37" s="36" t="s">
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
+      <c r="L36" s="10"/>
+      <c r="M36" s="10"/>
+      <c r="N36" s="10"/>
+      <c r="O36" s="10"/>
+      <c r="P36" s="10"/>
+      <c r="Q36" s="10"/>
+      <c r="R36" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="S36" s="10"/>
+      <c r="T36" s="10"/>
+      <c r="U36" s="10"/>
+      <c r="V36" s="10"/>
+    </row>
+    <row r="37" spans="1:22" ht="27">
+      <c r="A37" s="32" t="s">
         <v>121</v>
       </c>
       <c r="B37" s="26"/>
-      <c r="C37" s="34" t="b">
+      <c r="C37" s="31" t="b">
         <v>0</v>
       </c>
-      <c r="D37" s="34" t="s">
+      <c r="D37" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="E37" s="27" t="s">
+      <c r="E37" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="F37" s="28"/>
+      <c r="F37" s="7"/>
       <c r="G37" s="26"/>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
-      <c r="J37" s="27"/>
-      <c r="K37" s="27"/>
-      <c r="L37" s="27"/>
-      <c r="M37" s="27"/>
-      <c r="N37" s="27"/>
-      <c r="O37" s="27"/>
-      <c r="P37" s="27"/>
-      <c r="Q37" s="27"/>
-      <c r="R37" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="S37" s="27"/>
-      <c r="T37" s="27"/>
-      <c r="U37" s="27"/>
-      <c r="V37" s="27"/>
-    </row>
-    <row r="38" spans="1:22" s="29" customFormat="1" ht="27">
-      <c r="A38" s="36" t="s">
+      <c r="J37" s="10"/>
+      <c r="K37" s="10"/>
+      <c r="L37" s="10"/>
+      <c r="M37" s="10"/>
+      <c r="N37" s="10"/>
+      <c r="O37" s="10"/>
+      <c r="P37" s="10"/>
+      <c r="Q37" s="10"/>
+      <c r="R37" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="S37" s="10"/>
+      <c r="T37" s="10"/>
+      <c r="U37" s="10"/>
+      <c r="V37" s="10"/>
+    </row>
+    <row r="38" spans="1:22" ht="27">
+      <c r="A38" s="32" t="s">
         <v>122</v>
       </c>
       <c r="B38" s="26"/>
-      <c r="C38" s="34" t="b">
+      <c r="C38" s="31" t="b">
         <v>0</v>
       </c>
-      <c r="D38" s="34" t="s">
+      <c r="D38" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="E38" s="27" t="s">
+      <c r="E38" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="F38" s="28"/>
+      <c r="F38" s="7"/>
       <c r="G38" s="26"/>
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
-      <c r="J38" s="27"/>
-      <c r="K38" s="27"/>
-      <c r="L38" s="27"/>
-      <c r="M38" s="27"/>
-      <c r="N38" s="27"/>
-      <c r="O38" s="27"/>
-      <c r="P38" s="27"/>
-      <c r="Q38" s="27"/>
-      <c r="R38" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="S38" s="27"/>
-      <c r="T38" s="27"/>
-      <c r="U38" s="27"/>
-      <c r="V38" s="27"/>
-    </row>
-    <row r="39" spans="1:22" s="29" customFormat="1" ht="27">
-      <c r="A39" s="36" t="s">
+      <c r="J38" s="10"/>
+      <c r="K38" s="10"/>
+      <c r="L38" s="10"/>
+      <c r="M38" s="10"/>
+      <c r="N38" s="10"/>
+      <c r="O38" s="10"/>
+      <c r="P38" s="10"/>
+      <c r="Q38" s="10"/>
+      <c r="R38" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="S38" s="10"/>
+      <c r="T38" s="10"/>
+      <c r="U38" s="10"/>
+      <c r="V38" s="10"/>
+    </row>
+    <row r="39" spans="1:22" ht="27">
+      <c r="A39" s="32" t="s">
         <v>123</v>
       </c>
       <c r="B39" s="26"/>
-      <c r="C39" s="34" t="b">
+      <c r="C39" s="31" t="b">
         <v>0</v>
       </c>
-      <c r="D39" s="34" t="s">
+      <c r="D39" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="E39" s="27" t="s">
+      <c r="E39" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="F39" s="28"/>
+      <c r="F39" s="7"/>
       <c r="G39" s="26"/>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
-      <c r="J39" s="27"/>
-      <c r="K39" s="27"/>
-      <c r="L39" s="27"/>
-      <c r="M39" s="27"/>
-      <c r="N39" s="27"/>
-      <c r="O39" s="27"/>
-      <c r="P39" s="27"/>
-      <c r="Q39" s="27"/>
-      <c r="R39" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="S39" s="27"/>
-      <c r="T39" s="27"/>
-      <c r="U39" s="27"/>
-      <c r="V39" s="27"/>
-    </row>
-    <row r="40" spans="1:22" s="29" customFormat="1" ht="27">
-      <c r="A40" s="36" t="s">
+      <c r="J39" s="10"/>
+      <c r="K39" s="10"/>
+      <c r="L39" s="10"/>
+      <c r="M39" s="10"/>
+      <c r="N39" s="10"/>
+      <c r="O39" s="10"/>
+      <c r="P39" s="10"/>
+      <c r="Q39" s="10"/>
+      <c r="R39" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="S39" s="10"/>
+      <c r="T39" s="10"/>
+      <c r="U39" s="10"/>
+      <c r="V39" s="10"/>
+    </row>
+    <row r="40" spans="1:22" ht="27">
+      <c r="A40" s="32" t="s">
         <v>124</v>
       </c>
       <c r="B40" s="26"/>
-      <c r="C40" s="34" t="b">
+      <c r="C40" s="31" t="b">
         <v>0</v>
       </c>
-      <c r="D40" s="34" t="s">
+      <c r="D40" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="E40" s="27" t="s">
+      <c r="E40" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="F40" s="28"/>
+      <c r="F40" s="7"/>
       <c r="G40" s="26"/>
       <c r="H40" s="26"/>
       <c r="I40" s="26"/>
-      <c r="J40" s="27"/>
-      <c r="K40" s="27"/>
-      <c r="L40" s="27"/>
-      <c r="M40" s="27"/>
-      <c r="N40" s="27"/>
-      <c r="O40" s="27"/>
-      <c r="P40" s="27"/>
-      <c r="Q40" s="27"/>
-      <c r="R40" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="S40" s="27"/>
-      <c r="T40" s="27"/>
-      <c r="U40" s="27"/>
-      <c r="V40" s="27"/>
+      <c r="J40" s="10"/>
+      <c r="K40" s="10"/>
+      <c r="L40" s="10"/>
+      <c r="M40" s="10"/>
+      <c r="N40" s="10"/>
+      <c r="O40" s="10"/>
+      <c r="P40" s="10"/>
+      <c r="Q40" s="10"/>
+      <c r="R40" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="S40" s="10"/>
+      <c r="T40" s="10"/>
+      <c r="U40" s="10"/>
+      <c r="V40" s="10"/>
     </row>
     <row r="41" spans="1:22">
       <c r="A41" s="11" t="s">
@@ -3082,8 +3067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{154E0277-C785-47D8-A3E6-B2B8778DC36B}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
@@ -3144,7 +3129,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -3167,7 +3152,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="29.25">
@@ -3190,7 +3175,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add count context for translation with the Generator
We can now add translations for one-person interview.
Fix generate_label tests with different contexts.
</commit_message>
<xml_diff>
--- a/example/demo_generator/references/Household_Travel_Generate_Survey.xlsx
+++ b/example/demo_generator/references/Household_Travel_Generate_Survey.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28928"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="964" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD3B125B-8CC8-42DD-AD5E-7C91AD056CF1}"/>
+  <xr:revisionPtr revIDLastSave="978" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0AF4DD7-5803-4D81-ABD0-4FE84017DD06}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Labels" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Widgets!$A$1:$V$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Widgets!$A$1:$X$1</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="254">
   <si>
     <t>questionName</t>
   </si>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t>label::en</t>
+  </si>
+  <si>
+    <t>label_one::fr</t>
+  </si>
+  <si>
+    <t>label_one::en</t>
   </si>
   <si>
     <t>parameters</t>
@@ -395,6 +401,12 @@
   <si>
     <t>**Age**
 __For babies under the age of 1, write "0"__</t>
+  </si>
+  <si>
+    <t>**Votre âge**</t>
+  </si>
+  <si>
+    <t>**Your age**</t>
   </si>
   <si>
     <t>ageValidation</t>
@@ -1010,7 +1022,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1113,6 +1125,12 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1521,11 +1539,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:V42"/>
+  <dimension ref="A1:X42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="I26" sqref="I26"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="I21" sqref="I21:J21"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -1540,24 +1558,25 @@
     <col min="6" max="6" width="17" style="8" customWidth="1"/>
     <col min="7" max="7" width="31.28515625" style="8" customWidth="1"/>
     <col min="8" max="8" width="31.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.5703125" style="8" customWidth="1"/>
-    <col min="10" max="10" width="22.7109375" style="8" customWidth="1"/>
-    <col min="11" max="11" width="19.7109375" style="8" customWidth="1"/>
-    <col min="12" max="12" width="13.5703125" style="8" customWidth="1"/>
-    <col min="13" max="13" width="13" style="8" customWidth="1"/>
-    <col min="14" max="14" width="13.42578125" style="8" customWidth="1"/>
-    <col min="15" max="15" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.42578125" style="8" customWidth="1"/>
-    <col min="18" max="18" width="14.140625" style="8" customWidth="1"/>
-    <col min="19" max="19" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.42578125" style="8" customWidth="1"/>
-    <col min="21" max="21" width="11.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.5703125" style="8" customWidth="1"/>
-    <col min="23" max="16384" width="9.140625" style="8"/>
+    <col min="9" max="10" width="31.5703125" style="8" customWidth="1"/>
+    <col min="11" max="11" width="20.5703125" style="8" customWidth="1"/>
+    <col min="12" max="12" width="22.7109375" style="8" customWidth="1"/>
+    <col min="13" max="13" width="19.7109375" style="8" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" style="8" customWidth="1"/>
+    <col min="15" max="15" width="13" style="8" customWidth="1"/>
+    <col min="16" max="16" width="13.42578125" style="8" customWidth="1"/>
+    <col min="17" max="17" width="10" style="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.42578125" style="8" customWidth="1"/>
+    <col min="20" max="20" width="14.140625" style="8" customWidth="1"/>
+    <col min="21" max="21" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.42578125" style="8" customWidth="1"/>
+    <col min="23" max="23" width="11.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.5703125" style="8" customWidth="1"/>
+    <col min="25" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="18" customFormat="1" ht="17.25" customHeight="1">
+    <row r="1" spans="1:24" s="18" customFormat="1" ht="17.25" customHeight="1">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -1582,16 +1601,16 @@
       <c r="H1" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="I1" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="25" t="s">
+      <c r="J1" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="24" t="s">
+      <c r="K1" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="24" t="s">
+      <c r="L1" s="25" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="24" t="s">
@@ -1606,10 +1625,10 @@
       <c r="P1" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="23" t="s">
+      <c r="Q1" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="23" t="s">
+      <c r="R1" s="24" t="s">
         <v>17</v>
       </c>
       <c r="S1" s="23" t="s">
@@ -1624,228 +1643,244 @@
       <c r="V1" s="23" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" ht="27" hidden="1">
+      <c r="W1" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" ht="27" hidden="1">
       <c r="A2" s="9" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C2" s="9" t="b">
         <v>1</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="9" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
       <c r="K2" s="9"/>
-      <c r="L2" s="11"/>
+      <c r="L2" s="9"/>
       <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
+      <c r="N2" s="11"/>
       <c r="O2" s="9"/>
       <c r="P2" s="9"/>
       <c r="Q2" s="9"/>
-      <c r="R2" s="9" t="b">
-        <v>1</v>
-      </c>
+      <c r="R2" s="9"/>
       <c r="S2" s="9"/>
-      <c r="T2" s="9"/>
+      <c r="T2" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="U2" s="9"/>
       <c r="V2" s="9"/>
-    </row>
-    <row r="3" spans="1:22" ht="81" hidden="1">
+      <c r="W2" s="9"/>
+      <c r="X2" s="9"/>
+    </row>
+    <row r="3" spans="1:24" ht="81" hidden="1">
       <c r="A3" s="9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C3" s="9" t="b">
         <v>1</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I3" s="9"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="9" t="s">
+        <v>33</v>
+      </c>
       <c r="P3" s="9"/>
       <c r="Q3" s="9"/>
-      <c r="R3" s="9" t="b">
-        <v>1</v>
-      </c>
+      <c r="R3" s="9"/>
       <c r="S3" s="9"/>
-      <c r="T3" s="9"/>
+      <c r="T3" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="U3" s="9"/>
       <c r="V3" s="9"/>
-    </row>
-    <row r="4" spans="1:22" ht="40.5" hidden="1">
+      <c r="W3" s="9"/>
+      <c r="X3" s="9"/>
+    </row>
+    <row r="4" spans="1:24" ht="40.5" hidden="1">
       <c r="A4" s="9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C4" s="9" t="b">
         <v>1</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
-      <c r="K4" s="11"/>
+      <c r="K4" s="9"/>
       <c r="L4" s="9"/>
-      <c r="M4" s="9" t="s">
-        <v>36</v>
-      </c>
+      <c r="M4" s="11"/>
       <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
+      <c r="O4" s="9" t="s">
+        <v>38</v>
+      </c>
       <c r="P4" s="9"/>
       <c r="Q4" s="9"/>
-      <c r="R4" s="9" t="b">
-        <v>1</v>
-      </c>
+      <c r="R4" s="9"/>
       <c r="S4" s="9"/>
-      <c r="T4" s="9"/>
+      <c r="T4" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="U4" s="9"/>
       <c r="V4" s="9"/>
-    </row>
-    <row r="5" spans="1:22" hidden="1">
+      <c r="W4" s="9"/>
+      <c r="X4" s="9"/>
+    </row>
+    <row r="5" spans="1:24" hidden="1">
       <c r="A5" s="9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C5" s="9" t="b">
         <v>1</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="9" t="s">
+        <v>42</v>
+      </c>
       <c r="O5" s="9"/>
       <c r="P5" s="9"/>
       <c r="Q5" s="9"/>
-      <c r="R5" s="9" t="b">
-        <v>1</v>
-      </c>
+      <c r="R5" s="9"/>
       <c r="S5" s="9"/>
-      <c r="T5" s="9"/>
+      <c r="T5" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="U5" s="9"/>
       <c r="V5" s="9"/>
-    </row>
-    <row r="6" spans="1:22" ht="27" hidden="1">
+      <c r="W5" s="9"/>
+      <c r="X5" s="9"/>
+    </row>
+    <row r="6" spans="1:24" ht="27" hidden="1">
       <c r="A6" s="9" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C6" s="9" t="b">
         <v>1</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="9" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I6" s="9"/>
-      <c r="J6" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="K6" s="11"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
       <c r="L6" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
+        <v>46</v>
+      </c>
+      <c r="M6" s="11"/>
+      <c r="N6" s="9" t="s">
+        <v>47</v>
+      </c>
       <c r="O6" s="9"/>
       <c r="P6" s="9"/>
       <c r="Q6" s="9"/>
-      <c r="R6" s="9" t="b">
-        <v>1</v>
-      </c>
+      <c r="R6" s="9"/>
       <c r="S6" s="9"/>
-      <c r="T6" s="9"/>
+      <c r="T6" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="U6" s="9"/>
       <c r="V6" s="9"/>
-    </row>
-    <row r="7" spans="1:22" hidden="1">
+      <c r="W6" s="9"/>
+      <c r="X6" s="9"/>
+    </row>
+    <row r="7" spans="1:24" hidden="1">
       <c r="A7" s="9" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C7" s="9" t="b">
         <v>1</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9" t="str">
@@ -1853,10 +1888,10 @@
         <v>home.address</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
@@ -1867,26 +1902,28 @@
       <c r="O7" s="9"/>
       <c r="P7" s="9"/>
       <c r="Q7" s="9"/>
-      <c r="R7" s="9" t="b">
-        <v>1</v>
-      </c>
+      <c r="R7" s="9"/>
       <c r="S7" s="9"/>
-      <c r="T7" s="9"/>
+      <c r="T7" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="U7" s="9"/>
       <c r="V7" s="9"/>
-    </row>
-    <row r="8" spans="1:22" hidden="1">
+      <c r="W7" s="9"/>
+      <c r="X7" s="9"/>
+    </row>
+    <row r="8" spans="1:24" hidden="1">
       <c r="A8" s="9" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C8" s="9" t="b">
         <v>1</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9" t="str">
@@ -1894,42 +1931,44 @@
         <v>home.city</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
-      <c r="N8" s="9" t="s">
-        <v>52</v>
-      </c>
+      <c r="N8" s="9"/>
       <c r="O8" s="9"/>
-      <c r="P8" s="9"/>
+      <c r="P8" s="9" t="s">
+        <v>54</v>
+      </c>
       <c r="Q8" s="9"/>
-      <c r="R8" s="9" t="b">
-        <v>1</v>
-      </c>
+      <c r="R8" s="9"/>
       <c r="S8" s="9"/>
-      <c r="T8" s="9"/>
+      <c r="T8" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="U8" s="9"/>
       <c r="V8" s="9"/>
-    </row>
-    <row r="9" spans="1:22" ht="40.5" hidden="1">
+      <c r="W8" s="9"/>
+      <c r="X8" s="9"/>
+    </row>
+    <row r="9" spans="1:24" ht="40.5" hidden="1">
       <c r="A9" s="9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C9" s="9" t="b">
         <v>1</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="9" t="str">
@@ -1937,44 +1976,46 @@
         <v>home.region</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
-      <c r="K9" s="9" t="s">
-        <v>55</v>
-      </c>
+      <c r="K9" s="9"/>
       <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
+      <c r="M9" s="9" t="s">
+        <v>57</v>
+      </c>
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
       <c r="P9" s="9"/>
       <c r="Q9" s="9"/>
-      <c r="R9" s="9" t="b">
-        <v>1</v>
-      </c>
+      <c r="R9" s="9"/>
       <c r="S9" s="9"/>
-      <c r="T9" s="9"/>
-      <c r="U9" s="9" t="s">
-        <v>56</v>
-      </c>
+      <c r="T9" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="U9" s="9"/>
       <c r="V9" s="9"/>
-    </row>
-    <row r="10" spans="1:22" ht="40.5" hidden="1">
+      <c r="W9" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="X9" s="9"/>
+    </row>
+    <row r="10" spans="1:24" ht="40.5" hidden="1">
       <c r="A10" s="9" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C10" s="9" t="b">
         <v>1</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="9" t="str">
@@ -1982,44 +2023,46 @@
         <v>home.country</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
-      <c r="K10" s="9" t="s">
-        <v>60</v>
-      </c>
+      <c r="K10" s="9"/>
       <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
+      <c r="M10" s="9" t="s">
+        <v>62</v>
+      </c>
       <c r="N10" s="9"/>
       <c r="O10" s="9"/>
       <c r="P10" s="9"/>
       <c r="Q10" s="9"/>
-      <c r="R10" s="9" t="b">
-        <v>1</v>
-      </c>
+      <c r="R10" s="9"/>
       <c r="S10" s="9"/>
-      <c r="T10" s="9"/>
-      <c r="U10" s="9" t="s">
-        <v>61</v>
-      </c>
+      <c r="T10" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="U10" s="9"/>
       <c r="V10" s="9"/>
-    </row>
-    <row r="11" spans="1:22" ht="27" hidden="1">
+      <c r="W10" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="X10" s="9"/>
+    </row>
+    <row r="11" spans="1:24" ht="27" hidden="1">
       <c r="A11" s="9" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C11" s="9" t="b">
         <v>1</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="9" t="str">
@@ -2027,42 +2070,44 @@
         <v>home.postalCode</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
       <c r="K11" s="9"/>
-      <c r="L11" s="9" t="s">
-        <v>65</v>
-      </c>
+      <c r="L11" s="9"/>
       <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
+      <c r="N11" s="9" t="s">
+        <v>67</v>
+      </c>
       <c r="O11" s="9"/>
       <c r="P11" s="9"/>
       <c r="Q11" s="9"/>
-      <c r="R11" s="9" t="b">
-        <v>1</v>
-      </c>
+      <c r="R11" s="9"/>
       <c r="S11" s="9"/>
-      <c r="T11" s="9"/>
+      <c r="T11" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="U11" s="9"/>
       <c r="V11" s="9"/>
-    </row>
-    <row r="12" spans="1:22" ht="117.75" hidden="1" customHeight="1">
+      <c r="W11" s="9"/>
+      <c r="X11" s="9"/>
+    </row>
+    <row r="12" spans="1:24" ht="117.75" hidden="1" customHeight="1">
       <c r="A12" s="13" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C12" s="9" t="b">
         <v>1</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="9" t="str">
@@ -2070,40 +2115,42 @@
         <v>home.geography</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
-      <c r="K12" s="13"/>
+      <c r="K12" s="9"/>
       <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
+      <c r="M12" s="13"/>
       <c r="N12" s="9"/>
       <c r="O12" s="9"/>
       <c r="P12" s="9"/>
       <c r="Q12" s="9"/>
-      <c r="R12" s="9" t="b">
-        <v>1</v>
-      </c>
+      <c r="R12" s="9"/>
       <c r="S12" s="9"/>
-      <c r="T12" s="9"/>
+      <c r="T12" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="U12" s="9"/>
       <c r="V12" s="9"/>
-    </row>
-    <row r="13" spans="1:22" ht="48" hidden="1" customHeight="1">
+      <c r="W12" s="9"/>
+      <c r="X12" s="9"/>
+    </row>
+    <row r="13" spans="1:24" ht="48" hidden="1" customHeight="1">
       <c r="A13" s="9" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C13" s="9" t="b">
         <v>1</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E13" s="9"/>
       <c r="F13" s="9" t="str">
@@ -2111,46 +2158,48 @@
         <v>household.size</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="I13" s="9" t="s">
-        <v>74</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="I13" s="9"/>
       <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9" t="s">
-        <v>75</v>
-      </c>
+      <c r="K13" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="L13" s="9"/>
       <c r="M13" s="9"/>
       <c r="N13" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
+      <c r="P13" s="9" t="s">
+        <v>78</v>
+      </c>
       <c r="Q13" s="9"/>
-      <c r="R13" s="9" t="b">
-        <v>1</v>
-      </c>
+      <c r="R13" s="9"/>
       <c r="S13" s="9"/>
-      <c r="T13" s="9"/>
+      <c r="T13" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="U13" s="9"/>
       <c r="V13" s="9"/>
-    </row>
-    <row r="14" spans="1:22" ht="56.25" hidden="1" customHeight="1">
+      <c r="W13" s="9"/>
+      <c r="X13" s="9"/>
+    </row>
+    <row r="14" spans="1:24" ht="56.25" hidden="1" customHeight="1">
       <c r="A14" s="9" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C14" s="9" t="b">
         <v>1</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="9" t="str">
@@ -2158,46 +2207,48 @@
         <v>household.carNumber</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="I14" s="9" t="s">
-        <v>80</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="I14" s="9"/>
       <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9" t="s">
-        <v>81</v>
-      </c>
+      <c r="K14" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="L14" s="9"/>
       <c r="M14" s="9"/>
       <c r="N14" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="O14" s="9"/>
-      <c r="P14" s="9"/>
+      <c r="P14" s="9" t="s">
+        <v>84</v>
+      </c>
       <c r="Q14" s="9"/>
-      <c r="R14" s="9" t="b">
-        <v>1</v>
-      </c>
+      <c r="R14" s="9"/>
       <c r="S14" s="9"/>
-      <c r="T14" s="9"/>
+      <c r="T14" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="U14" s="9"/>
       <c r="V14" s="9"/>
-    </row>
-    <row r="15" spans="1:22" ht="76.5" hidden="1" customHeight="1">
+      <c r="W14" s="9"/>
+      <c r="X14" s="9"/>
+    </row>
+    <row r="15" spans="1:24" ht="76.5" hidden="1" customHeight="1">
       <c r="A15" s="9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C15" s="9" t="b">
         <v>1</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E15" s="9"/>
       <c r="F15" s="9" t="str">
@@ -2205,44 +2256,46 @@
         <v>household.bicycleNumber</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="I15" s="9" t="s">
-        <v>80</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="I15" s="9"/>
       <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9" t="s">
-        <v>86</v>
-      </c>
+      <c r="K15" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="L15" s="9"/>
       <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
+      <c r="N15" s="9" t="s">
+        <v>88</v>
+      </c>
       <c r="O15" s="9"/>
       <c r="P15" s="9"/>
       <c r="Q15" s="9"/>
-      <c r="R15" s="9" t="b">
-        <v>1</v>
-      </c>
+      <c r="R15" s="9"/>
       <c r="S15" s="9"/>
-      <c r="T15" s="9"/>
+      <c r="T15" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="U15" s="9"/>
       <c r="V15" s="9"/>
-    </row>
-    <row r="16" spans="1:22" ht="40.5" hidden="1">
+      <c r="W15" s="9"/>
+      <c r="X15" s="9"/>
+    </row>
+    <row r="16" spans="1:24" ht="40.5" hidden="1">
       <c r="A16" s="9" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C16" s="9" t="b">
         <v>1</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E16" s="9"/>
       <c r="F16" s="9" t="str">
@@ -2250,42 +2303,44 @@
         <v>household.electricBicycleNumber</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="I16" s="9" t="s">
-        <v>80</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="I16" s="9"/>
       <c r="J16" s="9"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
+      <c r="K16" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="L16" s="9"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
       <c r="O16" s="9"/>
       <c r="P16" s="9"/>
       <c r="Q16" s="9"/>
-      <c r="R16" s="9" t="b">
-        <v>1</v>
-      </c>
+      <c r="R16" s="9"/>
       <c r="S16" s="9"/>
-      <c r="T16" s="9"/>
+      <c r="T16" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="U16" s="9"/>
       <c r="V16" s="9"/>
-    </row>
-    <row r="17" spans="1:22" ht="76.5" hidden="1" customHeight="1">
+      <c r="W16" s="9"/>
+      <c r="X16" s="9"/>
+    </row>
+    <row r="17" spans="1:24" ht="76.5" hidden="1" customHeight="1">
       <c r="A17" s="9" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C17" s="9" t="b">
         <v>1</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="9" t="str">
@@ -2293,44 +2348,46 @@
         <v>household.atLeastOnePersonWithDisability</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
-      <c r="K17" s="9" t="s">
-        <v>93</v>
-      </c>
+      <c r="K17" s="9"/>
       <c r="L17" s="9"/>
       <c r="M17" s="9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
+      <c r="O17" s="9" t="s">
+        <v>96</v>
+      </c>
       <c r="P17" s="9"/>
       <c r="Q17" s="9"/>
-      <c r="R17" s="9" t="b">
-        <v>1</v>
-      </c>
+      <c r="R17" s="9"/>
       <c r="S17" s="9"/>
-      <c r="T17" s="9"/>
+      <c r="T17" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="U17" s="9"/>
       <c r="V17" s="9"/>
-    </row>
-    <row r="18" spans="1:22" hidden="1">
+      <c r="W17" s="9"/>
+      <c r="X17" s="9"/>
+    </row>
+    <row r="18" spans="1:24" hidden="1">
       <c r="A18" s="22" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C18" s="22" t="b">
         <v>1</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E18" s="9"/>
       <c r="F18" s="7" t="str">
@@ -2338,986 +2395,1036 @@
         <v>home.save</v>
       </c>
       <c r="G18" s="22" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="H18" s="22" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="I18" s="22"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="22"/>
       <c r="L18" s="9"/>
       <c r="M18" s="9"/>
       <c r="N18" s="9"/>
       <c r="O18" s="9"/>
       <c r="P18" s="9"/>
       <c r="Q18" s="9"/>
-      <c r="R18" s="10" t="b">
-        <v>1</v>
-      </c>
+      <c r="R18" s="9"/>
       <c r="S18" s="9"/>
-      <c r="T18" s="9"/>
+      <c r="T18" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="U18" s="9"/>
       <c r="V18" s="9"/>
-    </row>
-    <row r="19" spans="1:22" s="21" customFormat="1">
+      <c r="W18" s="9"/>
+      <c r="X18" s="9"/>
+    </row>
+    <row r="19" spans="1:24" s="21" customFormat="1">
       <c r="A19" s="26" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C19" s="26" t="b">
         <v>1</v>
       </c>
       <c r="D19" s="27" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E19" s="28"/>
       <c r="F19" s="28"/>
       <c r="G19" s="26"/>
       <c r="H19" s="26"/>
       <c r="I19" s="26"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="28"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="26"/>
       <c r="L19" s="28"/>
       <c r="M19" s="28"/>
       <c r="N19" s="28"/>
       <c r="O19" s="28"/>
       <c r="P19" s="28"/>
       <c r="Q19" s="28"/>
-      <c r="R19" s="27" t="b">
-        <v>1</v>
-      </c>
+      <c r="R19" s="28"/>
       <c r="S19" s="28"/>
-      <c r="T19" s="28"/>
+      <c r="T19" s="27" t="b">
+        <v>1</v>
+      </c>
       <c r="U19" s="28"/>
       <c r="V19" s="28"/>
-    </row>
-    <row r="20" spans="1:22" ht="144" customHeight="1">
+      <c r="W19" s="28"/>
+      <c r="X19" s="28"/>
+    </row>
+    <row r="20" spans="1:24" ht="144" customHeight="1">
       <c r="A20" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="B20" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="E20" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="B20" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="D20" s="27" t="s">
-        <v>100</v>
-      </c>
-      <c r="E20" s="29" t="s">
-        <v>99</v>
-      </c>
       <c r="F20" s="29" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G20" s="27" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H20" s="30" t="s">
-        <v>104</v>
-      </c>
-      <c r="I20" s="27"/>
-      <c r="J20" s="29"/>
-      <c r="K20" s="29" t="s">
-        <v>93</v>
-      </c>
-      <c r="L20" s="31"/>
-      <c r="M20" s="29"/>
-      <c r="N20" s="29"/>
+        <v>106</v>
+      </c>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="29"/>
+      <c r="M20" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="N20" s="31"/>
       <c r="O20" s="29"/>
       <c r="P20" s="29"/>
       <c r="Q20" s="29"/>
-      <c r="R20" s="27" t="b">
-        <v>1</v>
-      </c>
+      <c r="R20" s="29"/>
       <c r="S20" s="29"/>
-      <c r="T20" s="29"/>
+      <c r="T20" s="27" t="b">
+        <v>1</v>
+      </c>
       <c r="U20" s="29"/>
       <c r="V20" s="29"/>
-    </row>
-    <row r="21" spans="1:22" ht="37.5">
+      <c r="W20" s="29"/>
+      <c r="X20" s="29"/>
+    </row>
+    <row r="21" spans="1:24" ht="37.5">
       <c r="A21" s="27" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C21" s="27" t="b">
         <v>1</v>
       </c>
       <c r="D21" s="27" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E21" s="29" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F21" s="29" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G21" s="27" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="H21" s="30" t="s">
-        <v>109</v>
-      </c>
-      <c r="I21" s="27"/>
-      <c r="J21" s="29"/>
-      <c r="K21" s="29"/>
-      <c r="L21" s="29" t="s">
-        <v>110</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="I21" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="J21" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="K21" s="27"/>
+      <c r="L21" s="29"/>
       <c r="M21" s="29"/>
-      <c r="N21" s="29"/>
+      <c r="N21" s="29" t="s">
+        <v>114</v>
+      </c>
       <c r="O21" s="29"/>
       <c r="P21" s="29"/>
       <c r="Q21" s="29"/>
-      <c r="R21" s="27" t="b">
-        <v>1</v>
-      </c>
+      <c r="R21" s="29"/>
       <c r="S21" s="29"/>
-      <c r="T21" s="29"/>
+      <c r="T21" s="27" t="b">
+        <v>1</v>
+      </c>
       <c r="U21" s="29"/>
       <c r="V21" s="29"/>
-    </row>
-    <row r="22" spans="1:22" ht="37.5">
+      <c r="W21" s="29"/>
+      <c r="X21" s="29"/>
+    </row>
+    <row r="22" spans="1:24" ht="37.5">
       <c r="A22" s="27" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C22" s="27" t="b">
         <v>1</v>
       </c>
       <c r="D22" s="27" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E22" s="29" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F22" s="29" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="G22" s="27" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="H22" s="27" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="I22" s="27"/>
-      <c r="J22" s="29"/>
-      <c r="K22" s="31"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="27"/>
       <c r="L22" s="29"/>
-      <c r="M22" s="31" t="s">
-        <v>115</v>
-      </c>
+      <c r="M22" s="31"/>
       <c r="N22" s="29"/>
-      <c r="O22" s="29"/>
+      <c r="O22" s="31" t="s">
+        <v>119</v>
+      </c>
       <c r="P22" s="29"/>
       <c r="Q22" s="29"/>
-      <c r="R22" s="27" t="b">
-        <v>1</v>
-      </c>
+      <c r="R22" s="29"/>
       <c r="S22" s="29"/>
-      <c r="T22" s="29"/>
+      <c r="T22" s="27" t="b">
+        <v>1</v>
+      </c>
       <c r="U22" s="29"/>
       <c r="V22" s="29"/>
-    </row>
-    <row r="23" spans="1:22" ht="50.25">
+      <c r="W22" s="29"/>
+      <c r="X22" s="29"/>
+    </row>
+    <row r="23" spans="1:24" ht="50.25">
       <c r="A23" s="27" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C23" s="27" t="b">
         <v>1</v>
       </c>
       <c r="D23" s="27" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E23" s="29" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F23" s="29" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="G23" s="27" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="H23" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="I23" s="27"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="27"/>
+      <c r="L23" s="29"/>
+      <c r="M23" s="31"/>
+      <c r="N23" s="29"/>
+      <c r="O23" s="31" t="s">
         <v>119</v>
       </c>
-      <c r="I23" s="27"/>
-      <c r="J23" s="29"/>
-      <c r="K23" s="31"/>
-      <c r="L23" s="29"/>
-      <c r="M23" s="31" t="s">
-        <v>115</v>
-      </c>
-      <c r="N23" s="29"/>
-      <c r="O23" s="29"/>
       <c r="P23" s="29"/>
       <c r="Q23" s="29"/>
-      <c r="R23" s="27" t="b">
-        <v>1</v>
-      </c>
+      <c r="R23" s="29"/>
       <c r="S23" s="29"/>
-      <c r="T23" s="29"/>
+      <c r="T23" s="27" t="b">
+        <v>1</v>
+      </c>
       <c r="U23" s="29"/>
       <c r="V23" s="29"/>
-    </row>
-    <row r="24" spans="1:22" ht="24.75">
+      <c r="W23" s="29"/>
+      <c r="X23" s="29"/>
+    </row>
+    <row r="24" spans="1:24" ht="24.75">
       <c r="A24" s="27" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B24" s="27" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C24" s="27" t="b">
         <v>1</v>
       </c>
       <c r="D24" s="27" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E24" s="29" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F24" s="29" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="G24" s="32" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="H24" s="32" t="s">
-        <v>123</v>
-      </c>
-      <c r="I24" s="27"/>
-      <c r="J24" s="29"/>
-      <c r="K24" s="31"/>
+        <v>127</v>
+      </c>
+      <c r="I24" s="32"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="27"/>
       <c r="L24" s="29"/>
-      <c r="M24" s="31" t="s">
-        <v>115</v>
-      </c>
+      <c r="M24" s="31"/>
       <c r="N24" s="29"/>
-      <c r="O24" s="29"/>
+      <c r="O24" s="31" t="s">
+        <v>119</v>
+      </c>
       <c r="P24" s="29"/>
       <c r="Q24" s="29"/>
-      <c r="R24" s="27" t="b">
-        <v>1</v>
-      </c>
+      <c r="R24" s="29"/>
       <c r="S24" s="29"/>
-      <c r="T24" s="29"/>
+      <c r="T24" s="27" t="b">
+        <v>1</v>
+      </c>
       <c r="U24" s="29"/>
       <c r="V24" s="29"/>
-    </row>
-    <row r="25" spans="1:22" ht="24.75">
+      <c r="W24" s="29"/>
+      <c r="X24" s="29"/>
+    </row>
+    <row r="25" spans="1:24" ht="24.75">
       <c r="A25" s="27" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C25" s="27" t="b">
         <v>1</v>
       </c>
       <c r="D25" s="27" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E25" s="29" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F25" s="29" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="G25" s="27" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="H25" s="27" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="I25" s="27"/>
-      <c r="J25" s="29"/>
-      <c r="K25" s="31"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="27"/>
       <c r="L25" s="29"/>
-      <c r="M25" s="31" t="s">
-        <v>115</v>
-      </c>
-      <c r="N25" s="31"/>
-      <c r="O25" s="29"/>
-      <c r="P25" s="29"/>
+      <c r="M25" s="31"/>
+      <c r="N25" s="29"/>
+      <c r="O25" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="P25" s="31"/>
       <c r="Q25" s="29"/>
-      <c r="R25" s="27" t="b">
-        <v>1</v>
-      </c>
+      <c r="R25" s="29"/>
       <c r="S25" s="29"/>
-      <c r="T25" s="29"/>
+      <c r="T25" s="27" t="b">
+        <v>1</v>
+      </c>
       <c r="U25" s="29"/>
       <c r="V25" s="29"/>
-    </row>
-    <row r="26" spans="1:22" ht="24.75">
+      <c r="W25" s="29"/>
+      <c r="X25" s="29"/>
+    </row>
+    <row r="26" spans="1:24" ht="24.75">
       <c r="A26" s="27" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B26" s="27" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C26" s="27" t="b">
         <v>1</v>
       </c>
       <c r="D26" s="27" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E26" s="29" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F26" s="33" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="G26" s="27" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="H26" s="27" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="I26" s="27"/>
-      <c r="J26" s="29"/>
-      <c r="K26" s="31"/>
+      <c r="J26" s="27"/>
+      <c r="K26" s="27"/>
       <c r="L26" s="29"/>
-      <c r="M26" s="31" t="s">
-        <v>115</v>
-      </c>
+      <c r="M26" s="31"/>
       <c r="N26" s="29"/>
-      <c r="O26" s="29"/>
+      <c r="O26" s="31" t="s">
+        <v>119</v>
+      </c>
       <c r="P26" s="29"/>
       <c r="Q26" s="29"/>
-      <c r="R26" s="27" t="b">
-        <v>1</v>
-      </c>
+      <c r="R26" s="29"/>
       <c r="S26" s="29"/>
-      <c r="T26" s="29"/>
+      <c r="T26" s="27" t="b">
+        <v>1</v>
+      </c>
       <c r="U26" s="29"/>
       <c r="V26" s="29"/>
-    </row>
-    <row r="27" spans="1:22" ht="62.25" customHeight="1">
+      <c r="W26" s="29"/>
+      <c r="X26" s="29"/>
+    </row>
+    <row r="27" spans="1:24" ht="62.25" customHeight="1">
       <c r="A27" s="27" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="B27" s="27" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C27" s="27" t="b">
         <v>1</v>
       </c>
       <c r="D27" s="27" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E27" s="29" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F27" s="29" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="G27" s="32" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="H27" s="27" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="I27" s="27"/>
-      <c r="J27" s="29"/>
-      <c r="K27" s="31"/>
+      <c r="J27" s="27"/>
+      <c r="K27" s="27"/>
       <c r="L27" s="29"/>
-      <c r="M27" s="31" t="s">
-        <v>115</v>
-      </c>
+      <c r="M27" s="31"/>
       <c r="N27" s="29"/>
-      <c r="O27" s="29"/>
+      <c r="O27" s="31" t="s">
+        <v>119</v>
+      </c>
       <c r="P27" s="29"/>
       <c r="Q27" s="29"/>
-      <c r="R27" s="27" t="b">
-        <v>1</v>
-      </c>
+      <c r="R27" s="29"/>
       <c r="S27" s="29"/>
-      <c r="T27" s="29"/>
+      <c r="T27" s="27" t="b">
+        <v>1</v>
+      </c>
       <c r="U27" s="29"/>
       <c r="V27" s="29"/>
-    </row>
-    <row r="28" spans="1:22" ht="52.5" customHeight="1">
+      <c r="W27" s="29"/>
+      <c r="X27" s="29"/>
+    </row>
+    <row r="28" spans="1:24" ht="52.5" customHeight="1">
       <c r="A28" s="27" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="B28" s="27" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C28" s="27" t="b">
         <v>1</v>
       </c>
       <c r="D28" s="27" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E28" s="29" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F28" s="29" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="G28" s="27" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="H28" s="27" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="I28" s="27"/>
-      <c r="J28" s="29"/>
-      <c r="K28" s="31"/>
+      <c r="J28" s="27"/>
+      <c r="K28" s="27"/>
       <c r="L28" s="29"/>
-      <c r="M28" s="31" t="s">
-        <v>115</v>
-      </c>
+      <c r="M28" s="31"/>
       <c r="N28" s="29"/>
-      <c r="O28" s="29"/>
+      <c r="O28" s="31" t="s">
+        <v>119</v>
+      </c>
       <c r="P28" s="29"/>
       <c r="Q28" s="29"/>
-      <c r="R28" s="27" t="b">
-        <v>1</v>
-      </c>
+      <c r="R28" s="29"/>
       <c r="S28" s="29"/>
-      <c r="T28" s="29"/>
+      <c r="T28" s="27" t="b">
+        <v>1</v>
+      </c>
       <c r="U28" s="29"/>
       <c r="V28" s="29"/>
-    </row>
-    <row r="29" spans="1:22" ht="50.25">
+      <c r="W28" s="29"/>
+      <c r="X28" s="29"/>
+    </row>
+    <row r="29" spans="1:24" ht="50.25">
       <c r="A29" s="27" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B29" s="27" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C29" s="27" t="b">
         <v>1</v>
       </c>
       <c r="D29" s="27" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E29" s="29" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F29" s="29" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="G29" s="27" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="H29" s="27" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="I29" s="27"/>
-      <c r="J29" s="29"/>
-      <c r="K29" s="31"/>
-      <c r="L29" s="31"/>
-      <c r="M29" s="31" t="s">
-        <v>115</v>
-      </c>
-      <c r="N29" s="29"/>
-      <c r="O29" s="29"/>
+      <c r="J29" s="27"/>
+      <c r="K29" s="27"/>
+      <c r="L29" s="29"/>
+      <c r="M29" s="31"/>
+      <c r="N29" s="31"/>
+      <c r="O29" s="31" t="s">
+        <v>119</v>
+      </c>
       <c r="P29" s="29"/>
       <c r="Q29" s="29"/>
-      <c r="R29" s="27" t="b">
-        <v>1</v>
-      </c>
+      <c r="R29" s="29"/>
       <c r="S29" s="29"/>
-      <c r="T29" s="29"/>
+      <c r="T29" s="27" t="b">
+        <v>1</v>
+      </c>
       <c r="U29" s="29"/>
       <c r="V29" s="29"/>
-    </row>
-    <row r="30" spans="1:22" ht="37.5">
+      <c r="W29" s="29"/>
+      <c r="X29" s="29"/>
+    </row>
+    <row r="30" spans="1:24" ht="37.5">
       <c r="A30" s="27" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B30" s="27" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C30" s="27" t="b">
         <v>1</v>
       </c>
       <c r="D30" s="27" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E30" s="29" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F30" s="29" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="G30" s="27" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="H30" s="27" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="I30" s="27"/>
-      <c r="J30" s="29"/>
-      <c r="K30" s="31"/>
+      <c r="J30" s="27"/>
+      <c r="K30" s="27"/>
       <c r="L30" s="29"/>
-      <c r="M30" s="31" t="s">
-        <v>115</v>
-      </c>
+      <c r="M30" s="31"/>
       <c r="N30" s="29"/>
-      <c r="O30" s="29"/>
+      <c r="O30" s="31" t="s">
+        <v>119</v>
+      </c>
       <c r="P30" s="29"/>
       <c r="Q30" s="29"/>
-      <c r="R30" s="27" t="b">
-        <v>1</v>
-      </c>
+      <c r="R30" s="29"/>
       <c r="S30" s="29"/>
-      <c r="T30" s="29"/>
+      <c r="T30" s="27" t="b">
+        <v>1</v>
+      </c>
       <c r="U30" s="29"/>
       <c r="V30" s="29"/>
-    </row>
-    <row r="31" spans="1:22" ht="24.75">
+      <c r="W30" s="29"/>
+      <c r="X30" s="29"/>
+    </row>
+    <row r="31" spans="1:24" ht="24.75">
       <c r="A31" s="27" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B31" s="27" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C31" s="27" t="b">
         <v>1</v>
       </c>
       <c r="D31" s="27" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E31" s="29" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F31" s="29" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="G31" s="27" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="H31" s="27" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="I31" s="27"/>
-      <c r="J31" s="29"/>
-      <c r="K31" s="31"/>
+      <c r="J31" s="27"/>
+      <c r="K31" s="27"/>
       <c r="L31" s="29"/>
-      <c r="M31" s="31" t="s">
-        <v>115</v>
-      </c>
+      <c r="M31" s="31"/>
       <c r="N31" s="29"/>
-      <c r="O31" s="29"/>
+      <c r="O31" s="31" t="s">
+        <v>119</v>
+      </c>
       <c r="P31" s="29"/>
       <c r="Q31" s="29"/>
-      <c r="R31" s="27" t="b">
-        <v>1</v>
-      </c>
+      <c r="R31" s="29"/>
       <c r="S31" s="29"/>
-      <c r="T31" s="29"/>
+      <c r="T31" s="27" t="b">
+        <v>1</v>
+      </c>
       <c r="U31" s="29"/>
       <c r="V31" s="29"/>
-    </row>
-    <row r="32" spans="1:22" ht="24.75">
+      <c r="W31" s="29"/>
+      <c r="X31" s="29"/>
+    </row>
+    <row r="32" spans="1:24" ht="24.75">
       <c r="A32" s="27" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="B32" s="27" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C32" s="27" t="b">
         <v>1</v>
       </c>
       <c r="D32" s="27" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E32" s="29" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F32" s="29" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="G32" s="27" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="H32" s="27" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="I32" s="27"/>
-      <c r="J32" s="29"/>
-      <c r="K32" s="31"/>
+      <c r="J32" s="27"/>
+      <c r="K32" s="27"/>
       <c r="L32" s="29"/>
-      <c r="M32" s="31" t="s">
-        <v>115</v>
-      </c>
+      <c r="M32" s="31"/>
       <c r="N32" s="29"/>
-      <c r="O32" s="29"/>
+      <c r="O32" s="31" t="s">
+        <v>119</v>
+      </c>
       <c r="P32" s="29"/>
       <c r="Q32" s="29"/>
-      <c r="R32" s="27" t="b">
-        <v>1</v>
-      </c>
+      <c r="R32" s="29"/>
       <c r="S32" s="29"/>
-      <c r="T32" s="29"/>
+      <c r="T32" s="27" t="b">
+        <v>1</v>
+      </c>
       <c r="U32" s="29"/>
       <c r="V32" s="29"/>
-    </row>
-    <row r="33" spans="1:22" ht="24.75">
+      <c r="W32" s="29"/>
+      <c r="X32" s="29"/>
+    </row>
+    <row r="33" spans="1:24" ht="24.75">
       <c r="A33" s="27" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="B33" s="27" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C33" s="27" t="b">
         <v>1</v>
       </c>
       <c r="D33" s="27" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E33" s="29" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F33" s="29" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="G33" s="27" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="H33" s="27" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="I33" s="27"/>
-      <c r="J33" s="29"/>
-      <c r="K33" s="31"/>
+      <c r="J33" s="27"/>
+      <c r="K33" s="27"/>
       <c r="L33" s="29"/>
-      <c r="M33" s="29"/>
-      <c r="N33" s="31"/>
+      <c r="M33" s="31"/>
+      <c r="N33" s="29"/>
       <c r="O33" s="29"/>
-      <c r="P33" s="29"/>
+      <c r="P33" s="31"/>
       <c r="Q33" s="29"/>
-      <c r="R33" s="27" t="b">
-        <v>1</v>
-      </c>
+      <c r="R33" s="29"/>
       <c r="S33" s="29"/>
-      <c r="T33" s="29"/>
+      <c r="T33" s="27" t="b">
+        <v>1</v>
+      </c>
       <c r="U33" s="29"/>
       <c r="V33" s="29"/>
-    </row>
-    <row r="34" spans="1:22" ht="24.75">
+      <c r="W33" s="29"/>
+      <c r="X33" s="29"/>
+    </row>
+    <row r="34" spans="1:24" ht="24.75">
       <c r="A34" s="27" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="B34" s="27"/>
       <c r="C34" s="27" t="b">
         <v>0</v>
       </c>
       <c r="D34" s="27" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E34" s="29" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F34" s="29" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="G34" s="32" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="H34" s="32" t="s">
-        <v>163</v>
-      </c>
-      <c r="I34" s="27"/>
-      <c r="J34" s="29"/>
-      <c r="K34" s="31"/>
+        <v>167</v>
+      </c>
+      <c r="I34" s="32"/>
+      <c r="J34" s="32"/>
+      <c r="K34" s="27"/>
       <c r="L34" s="29"/>
-      <c r="M34" s="29"/>
-      <c r="N34" s="31"/>
+      <c r="M34" s="31"/>
+      <c r="N34" s="29"/>
       <c r="O34" s="29"/>
-      <c r="P34" s="29"/>
+      <c r="P34" s="31"/>
       <c r="Q34" s="29"/>
-      <c r="R34" s="27" t="b">
-        <v>1</v>
-      </c>
+      <c r="R34" s="29"/>
       <c r="S34" s="29"/>
-      <c r="T34" s="29"/>
+      <c r="T34" s="27" t="b">
+        <v>1</v>
+      </c>
       <c r="U34" s="29"/>
       <c r="V34" s="29"/>
-    </row>
-    <row r="35" spans="1:22" ht="24.75">
+      <c r="W34" s="29"/>
+      <c r="X34" s="29"/>
+    </row>
+    <row r="35" spans="1:24" ht="24.75">
       <c r="A35" s="27" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="B35" s="27" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C35" s="27" t="b">
         <v>1</v>
       </c>
       <c r="D35" s="27" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E35" s="29" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F35" s="29" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="G35" s="27" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="H35" s="27" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="I35" s="27"/>
-      <c r="J35" s="29"/>
-      <c r="K35" s="31"/>
+      <c r="J35" s="27"/>
+      <c r="K35" s="27"/>
       <c r="L35" s="29"/>
-      <c r="M35" s="29"/>
-      <c r="N35" s="31"/>
+      <c r="M35" s="31"/>
+      <c r="N35" s="29"/>
       <c r="O35" s="29"/>
-      <c r="P35" s="29"/>
+      <c r="P35" s="31"/>
       <c r="Q35" s="29"/>
-      <c r="R35" s="27" t="b">
-        <v>1</v>
-      </c>
+      <c r="R35" s="29"/>
       <c r="S35" s="29"/>
-      <c r="T35" s="29"/>
+      <c r="T35" s="27" t="b">
+        <v>1</v>
+      </c>
       <c r="U35" s="29"/>
       <c r="V35" s="29"/>
-    </row>
-    <row r="36" spans="1:22" ht="24.75">
+      <c r="W35" s="29"/>
+      <c r="X35" s="29"/>
+    </row>
+    <row r="36" spans="1:24" ht="24.75">
       <c r="A36" s="27" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="B36" s="27"/>
       <c r="C36" s="27" t="b">
         <v>0</v>
       </c>
       <c r="D36" s="27" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E36" s="29" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F36" s="29" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="G36" s="32" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="H36" s="32" t="s">
-        <v>163</v>
-      </c>
-      <c r="I36" s="27"/>
-      <c r="J36" s="29"/>
-      <c r="K36" s="31"/>
+        <v>167</v>
+      </c>
+      <c r="I36" s="32"/>
+      <c r="J36" s="32"/>
+      <c r="K36" s="27"/>
       <c r="L36" s="29"/>
-      <c r="M36" s="29"/>
-      <c r="N36" s="31"/>
+      <c r="M36" s="31"/>
+      <c r="N36" s="29"/>
       <c r="O36" s="29"/>
-      <c r="P36" s="29"/>
+      <c r="P36" s="31"/>
       <c r="Q36" s="29"/>
-      <c r="R36" s="27" t="b">
-        <v>1</v>
-      </c>
+      <c r="R36" s="29"/>
       <c r="S36" s="29"/>
-      <c r="T36" s="29"/>
+      <c r="T36" s="27" t="b">
+        <v>1</v>
+      </c>
       <c r="U36" s="29"/>
       <c r="V36" s="29"/>
-    </row>
-    <row r="37" spans="1:22" ht="86.25" customHeight="1">
+      <c r="W36" s="29"/>
+      <c r="X36" s="29"/>
+    </row>
+    <row r="37" spans="1:24" ht="86.25" customHeight="1">
       <c r="A37" s="27" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="B37" s="27" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C37" s="27" t="b">
         <v>1</v>
       </c>
       <c r="D37" s="27" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E37" s="29" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F37" s="29" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="G37" s="27" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="H37" s="27" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="I37" s="27"/>
-      <c r="J37" s="29"/>
-      <c r="K37" s="31"/>
-      <c r="L37" s="31"/>
-      <c r="M37" s="31" t="s">
-        <v>115</v>
-      </c>
-      <c r="N37" s="29"/>
-      <c r="O37" s="29"/>
+      <c r="J37" s="27"/>
+      <c r="K37" s="27"/>
+      <c r="L37" s="29"/>
+      <c r="M37" s="31"/>
+      <c r="N37" s="31"/>
+      <c r="O37" s="31" t="s">
+        <v>119</v>
+      </c>
       <c r="P37" s="29"/>
       <c r="Q37" s="29"/>
-      <c r="R37" s="27" t="b">
-        <v>1</v>
-      </c>
+      <c r="R37" s="29"/>
       <c r="S37" s="29"/>
-      <c r="T37" s="29"/>
+      <c r="T37" s="27" t="b">
+        <v>1</v>
+      </c>
       <c r="U37" s="29"/>
       <c r="V37" s="29"/>
-    </row>
-    <row r="38" spans="1:22" ht="37.5">
+      <c r="W37" s="29"/>
+      <c r="X37" s="29"/>
+    </row>
+    <row r="38" spans="1:24" ht="37.5">
       <c r="A38" s="27" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="B38" s="27" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C38" s="27" t="b">
         <v>1</v>
       </c>
       <c r="D38" s="27" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E38" s="29" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F38" s="29" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="G38" s="27" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="H38" s="27" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="I38" s="27"/>
-      <c r="J38" s="29"/>
-      <c r="K38" s="31"/>
-      <c r="L38" s="31"/>
-      <c r="M38" s="31" t="s">
-        <v>115</v>
-      </c>
-      <c r="N38" s="29"/>
-      <c r="O38" s="29"/>
+      <c r="J38" s="27"/>
+      <c r="K38" s="27"/>
+      <c r="L38" s="29"/>
+      <c r="M38" s="31"/>
+      <c r="N38" s="31"/>
+      <c r="O38" s="31" t="s">
+        <v>119</v>
+      </c>
       <c r="P38" s="29"/>
       <c r="Q38" s="29"/>
-      <c r="R38" s="27" t="b">
-        <v>1</v>
-      </c>
+      <c r="R38" s="29"/>
       <c r="S38" s="29"/>
-      <c r="T38" s="29"/>
+      <c r="T38" s="27" t="b">
+        <v>1</v>
+      </c>
       <c r="U38" s="29"/>
       <c r="V38" s="29"/>
-    </row>
-    <row r="39" spans="1:22" ht="75.75">
+      <c r="W38" s="29"/>
+      <c r="X38" s="29"/>
+    </row>
+    <row r="39" spans="1:24" ht="75.75">
       <c r="A39" s="27" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="B39" s="27" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C39" s="27" t="b">
         <v>1</v>
       </c>
       <c r="D39" s="27" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E39" s="29" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F39" s="29" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="G39" s="27" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="H39" s="27" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="I39" s="27"/>
-      <c r="J39" s="29"/>
-      <c r="K39" s="31"/>
-      <c r="L39" s="31"/>
-      <c r="M39" s="31" t="s">
-        <v>115</v>
-      </c>
-      <c r="N39" s="29"/>
-      <c r="O39" s="29"/>
+      <c r="J39" s="27"/>
+      <c r="K39" s="27"/>
+      <c r="L39" s="29"/>
+      <c r="M39" s="31"/>
+      <c r="N39" s="31"/>
+      <c r="O39" s="31" t="s">
+        <v>119</v>
+      </c>
       <c r="P39" s="29"/>
       <c r="Q39" s="29"/>
-      <c r="R39" s="27" t="b">
-        <v>1</v>
-      </c>
+      <c r="R39" s="29"/>
       <c r="S39" s="29"/>
-      <c r="T39" s="29"/>
+      <c r="T39" s="27" t="b">
+        <v>1</v>
+      </c>
       <c r="U39" s="29"/>
       <c r="V39" s="29"/>
-    </row>
-    <row r="40" spans="1:22" ht="37.5">
+      <c r="W39" s="29"/>
+      <c r="X39" s="29"/>
+    </row>
+    <row r="40" spans="1:24" ht="37.5">
       <c r="A40" s="27" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B40" s="27" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C40" s="27" t="b">
         <v>1</v>
       </c>
       <c r="D40" s="27" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E40" s="29" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F40" s="29" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="G40" s="27" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="H40" s="27" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="I40" s="27"/>
-      <c r="J40" s="29"/>
-      <c r="K40" s="31"/>
-      <c r="L40" s="31"/>
-      <c r="M40" s="31" t="s">
-        <v>115</v>
-      </c>
-      <c r="N40" s="29"/>
-      <c r="O40" s="29"/>
+      <c r="J40" s="27"/>
+      <c r="K40" s="27"/>
+      <c r="L40" s="29"/>
+      <c r="M40" s="31"/>
+      <c r="N40" s="31"/>
+      <c r="O40" s="31" t="s">
+        <v>119</v>
+      </c>
       <c r="P40" s="29"/>
       <c r="Q40" s="29"/>
-      <c r="R40" s="27" t="b">
-        <v>1</v>
-      </c>
+      <c r="R40" s="29"/>
       <c r="S40" s="29"/>
-      <c r="T40" s="29"/>
+      <c r="T40" s="27" t="b">
+        <v>1</v>
+      </c>
       <c r="U40" s="29"/>
       <c r="V40" s="29"/>
-    </row>
-    <row r="41" spans="1:22" s="18" customFormat="1">
+      <c r="W40" s="29"/>
+      <c r="X40" s="29"/>
+    </row>
+    <row r="41" spans="1:24" s="18" customFormat="1">
       <c r="A41" s="34" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="B41" s="34" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C41" s="34" t="b">
         <v>1</v>
       </c>
       <c r="D41" s="34" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E41" s="35"/>
       <c r="F41" s="35" t="str">
@@ -3325,58 +3432,60 @@
         <v>household.save</v>
       </c>
       <c r="G41" s="34" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="H41" s="34" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="I41" s="34"/>
-      <c r="J41" s="35"/>
-      <c r="K41" s="35"/>
+      <c r="J41" s="34"/>
+      <c r="K41" s="34"/>
       <c r="L41" s="35"/>
       <c r="M41" s="35"/>
       <c r="N41" s="35"/>
       <c r="O41" s="35"/>
       <c r="P41" s="35"/>
       <c r="Q41" s="35"/>
-      <c r="R41" s="34" t="b">
-        <v>1</v>
-      </c>
+      <c r="R41" s="35"/>
       <c r="S41" s="35"/>
-      <c r="T41" s="35"/>
+      <c r="T41" s="34" t="b">
+        <v>1</v>
+      </c>
       <c r="U41" s="35"/>
       <c r="V41" s="35"/>
-    </row>
-    <row r="42" spans="1:22" ht="130.5" hidden="1">
+      <c r="W41" s="35"/>
+      <c r="X41" s="35"/>
+    </row>
+    <row r="42" spans="1:24" ht="130.5" hidden="1">
       <c r="A42" s="8" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C42" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="H42" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="J42" s="20"/>
-      <c r="K42" s="19"/>
-      <c r="R42" s="8" t="b">
+        <v>194</v>
+      </c>
+      <c r="L42" s="20"/>
+      <c r="M42" s="19"/>
+      <c r="T42" s="8" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:V42" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <autoFilter ref="A1:X42" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="3">
       <filters>
         <filter val="household"/>
@@ -3401,19 +3510,19 @@
       <formula>NOT(ISERROR(SEARCH("TRUE",C42)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L42:O42">
+  <conditionalFormatting sqref="N42:Q42">
     <cfRule type="expression" dxfId="2" priority="1">
-      <formula>AND($B1048370="Custom",  $B1048370&lt;&gt;"", ROW(L1048370)&lt;&gt;1)</formula>
+      <formula>AND($B1048370="Custom",  $B1048370&lt;&gt;"", ROW(N1048370)&lt;&gt;1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M42:N42">
+  <conditionalFormatting sqref="O42:P42">
     <cfRule type="expression" dxfId="1" priority="5">
-      <formula>AND($B42&lt;&gt;"Select", $B42&lt;&gt;"Checkbox", $B42&lt;&gt;"Radio",  $B42&lt;&gt;"", ROW(M42)&lt;&gt;1)</formula>
+      <formula>AND($B42&lt;&gt;"Select", $B42&lt;&gt;"Checkbox", $B42&lt;&gt;"Radio",  $B42&lt;&gt;"", ROW(O42)&lt;&gt;1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O42">
+  <conditionalFormatting sqref="Q42">
     <cfRule type="expression" dxfId="0" priority="2">
-      <formula>AND($B42&lt;&gt;"Range", $B42&lt;&gt;"", ROW(O42)&lt;&gt;1)</formula>
+      <formula>AND($B42&lt;&gt;"Range", $B42&lt;&gt;"", ROW(Q42)&lt;&gt;1)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3440,34 +3549,34 @@
   <sheetData>
     <row r="1" spans="1:6" s="6" customFormat="1">
       <c r="A1" s="14" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="29.25">
       <c r="A2" s="12" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="E2" s="12">
         <v>1</v>
@@ -3476,14 +3585,14 @@
     </row>
     <row r="3" spans="1:6" ht="29.25">
       <c r="A3" s="12" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="12" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="E3" s="12">
         <v>2</v>
@@ -3500,7 +3609,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
@@ -3520,39 +3629,39 @@
         <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="12" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="E2" s="12" t="b">
         <v>1</v>
@@ -3566,16 +3675,16 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="12" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="E3" s="12" t="b">
         <v>1</v>
@@ -3589,16 +3698,16 @@
     </row>
     <row r="4" spans="1:8" ht="29.25">
       <c r="A4" s="12" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="E4" s="12" t="b">
         <v>0</v>
@@ -3635,10 +3744,10 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="3" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>6</v>
@@ -3647,136 +3756,136 @@
         <v>7</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="B2" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="C2" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="D2" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="B3" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="C3" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="D3" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="B4" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="C4" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="D4" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="C5" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="D5" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="B6" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="C6" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="D6" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E7" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E8" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="E9" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="E10" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E11" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E12" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E13" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -3808,40 +3917,40 @@
   <sheetData>
     <row r="1" spans="1:12" s="5" customFormat="1">
       <c r="A1" s="4" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -3861,19 +3970,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="B1" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="C1" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="D1" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="E1" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add gender context for label translations with the Generator.
Add getActivePersonGender helper function to help with that.
Update the household Excel with this new method.
</commit_message>
<xml_diff>
--- a/example/demo_generator/references/Household_Travel_Generate_Survey.xlsx
+++ b/example/demo_generator/references/Household_Travel_Generate_Survey.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28928"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="978" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0AF4DD7-5803-4D81-ABD0-4FE84017DD06}"/>
+  <xr:revisionPtr revIDLastSave="1011" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{16609EB3-8854-4224-91CB-3373A9034551}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="260">
   <si>
     <t>questionName</t>
   </si>
@@ -403,10 +403,10 @@
 __For babies under the age of 1, write "0"__</t>
   </si>
   <si>
-    <t>**Votre âge**</t>
-  </si>
-  <si>
-    <t>**Your age**</t>
+    <t>Votre **âge**</t>
+  </si>
+  <si>
+    <t>Your **age**</t>
   </si>
   <si>
     <t>ageValidation</t>
@@ -426,9 +426,6 @@
 __Sex assigned at birth or that which appears on legal documents.__</t>
   </si>
   <si>
-    <t>yesNoDontKnow</t>
-  </si>
-  <si>
     <t>personWorkerType</t>
   </si>
   <si>
@@ -443,6 +440,9 @@
 __Including self-employed, artist, on sick leave or parental leave.__</t>
   </si>
   <si>
+    <t>yesNoDontKnow</t>
+  </si>
+  <si>
     <t>personSchoolType</t>
   </si>
   <si>
@@ -461,7 +461,7 @@
     <t>studentType</t>
   </si>
   <si>
-    <t>**Étudiant**</t>
+    <t>**Étudiant{{gender:e}}**</t>
   </si>
   <si>
     <t>**Student**</t>
@@ -486,7 +486,7 @@
   </si>
   <si>
     <t>**Permis de conduire**
-__Inclure les permis d’apprenti{{suffixE}}conduct{{suffixEurRice}} et probatoires, mais ne pas inclure les permis de cyclomoteur/scooter.__</t>
+__Inclure les permis d’apprenti{{gender:e}} conduct{{gender:eur/rice}} et probatoires, mais ne pas inclure les permis de cyclomoteur/scooter.__</t>
   </si>
   <si>
     <t>**Driver's licence**
@@ -603,7 +603,7 @@
     <t>travelToWorkDays</t>
   </si>
   <si>
-    <t>Durant la dernière **semaine**, quand est-ce que {{nickname}} s'est **déplacé{{suffixE}}** pour le **travail** ?
+    <t>Durant la dernière **semaine**, quand est-ce que {{nickname}} s'est **déplacé{{gender:e}}** pour le **travail** ?
 __Pour se rendre au travail ou toute autre raison concernant le travail.__</t>
   </si>
   <si>
@@ -629,7 +629,7 @@
     <t>travelToStudyDays</t>
   </si>
   <si>
-    <t>Durant la **dernière semaine**, est-ce que {{nickname}} s'est **déplacé{{suffixE}}** pour les **études**.
+    <t>Durant la **dernière semaine**, est-ce que {{nickname}} s'est **déplacé{{gender:e}}** pour les **études**.
 __Pour se rendre à l'établissement d'enseignement ou pour toute autre raison concernant les études.__</t>
   </si>
   <si>
@@ -790,6 +790,24 @@
   </si>
   <si>
     <t>I prefer not to answer</t>
+  </si>
+  <si>
+    <t>man</t>
+  </si>
+  <si>
+    <t>Homme</t>
+  </si>
+  <si>
+    <t>Man</t>
+  </si>
+  <si>
+    <t>woman</t>
+  </si>
+  <si>
+    <t>Femme</t>
+  </si>
+  <si>
+    <t>Woman</t>
   </si>
   <si>
     <t>inputRangeName</t>
@@ -1127,10 +1145,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1542,8 +1560,8 @@
   <dimension ref="A1:X42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="I21" sqref="I21:J21"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="H19" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="O22" sqref="O22"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -2526,10 +2544,10 @@
       <c r="H21" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="I21" s="37" t="s">
+      <c r="I21" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="J21" s="37" t="s">
+      <c r="J21" s="30" t="s">
         <v>113</v>
       </c>
       <c r="K21" s="27"/>
@@ -2582,8 +2600,8 @@
       <c r="L22" s="29"/>
       <c r="M22" s="31"/>
       <c r="N22" s="29"/>
-      <c r="O22" s="31" t="s">
-        <v>119</v>
+      <c r="O22" s="37" t="s">
+        <v>116</v>
       </c>
       <c r="P22" s="29"/>
       <c r="Q22" s="29"/>
@@ -2599,7 +2617,7 @@
     </row>
     <row r="23" spans="1:24" ht="50.25">
       <c r="A23" s="27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B23" s="27" t="s">
         <v>30</v>
@@ -2614,13 +2632,13 @@
         <v>101</v>
       </c>
       <c r="F23" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="G23" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="G23" s="27" t="s">
+      <c r="H23" s="27" t="s">
         <v>122</v>
-      </c>
-      <c r="H23" s="27" t="s">
-        <v>123</v>
       </c>
       <c r="I23" s="27"/>
       <c r="J23" s="27"/>
@@ -2629,7 +2647,7 @@
       <c r="M23" s="31"/>
       <c r="N23" s="29"/>
       <c r="O23" s="31" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="P23" s="29"/>
       <c r="Q23" s="29"/>
@@ -2668,14 +2686,14 @@
       <c r="H24" s="32" t="s">
         <v>127</v>
       </c>
-      <c r="I24" s="32"/>
-      <c r="J24" s="32"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="27"/>
       <c r="K24" s="27"/>
       <c r="L24" s="29"/>
       <c r="M24" s="31"/>
       <c r="N24" s="29"/>
       <c r="O24" s="31" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="P24" s="29"/>
       <c r="Q24" s="29"/>
@@ -2721,7 +2739,7 @@
       <c r="M25" s="31"/>
       <c r="N25" s="29"/>
       <c r="O25" s="31" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="P25" s="31"/>
       <c r="Q25" s="29"/>
@@ -2767,7 +2785,7 @@
       <c r="M26" s="31"/>
       <c r="N26" s="29"/>
       <c r="O26" s="31" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="P26" s="29"/>
       <c r="Q26" s="29"/>
@@ -2813,7 +2831,7 @@
       <c r="M27" s="31"/>
       <c r="N27" s="29"/>
       <c r="O27" s="31" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="P27" s="29"/>
       <c r="Q27" s="29"/>
@@ -2859,7 +2877,7 @@
       <c r="M28" s="31"/>
       <c r="N28" s="29"/>
       <c r="O28" s="31" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="P28" s="29"/>
       <c r="Q28" s="29"/>
@@ -2905,7 +2923,7 @@
       <c r="M29" s="31"/>
       <c r="N29" s="31"/>
       <c r="O29" s="31" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="P29" s="29"/>
       <c r="Q29" s="29"/>
@@ -2951,7 +2969,7 @@
       <c r="M30" s="31"/>
       <c r="N30" s="29"/>
       <c r="O30" s="31" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="P30" s="29"/>
       <c r="Q30" s="29"/>
@@ -2997,7 +3015,7 @@
       <c r="M31" s="31"/>
       <c r="N31" s="29"/>
       <c r="O31" s="31" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="P31" s="29"/>
       <c r="Q31" s="29"/>
@@ -3043,7 +3061,7 @@
       <c r="M32" s="31"/>
       <c r="N32" s="29"/>
       <c r="O32" s="31" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="P32" s="29"/>
       <c r="Q32" s="29"/>
@@ -3261,7 +3279,7 @@
       <c r="M37" s="31"/>
       <c r="N37" s="31"/>
       <c r="O37" s="31" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="P37" s="29"/>
       <c r="Q37" s="29"/>
@@ -3307,7 +3325,7 @@
       <c r="M38" s="31"/>
       <c r="N38" s="31"/>
       <c r="O38" s="31" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="P38" s="29"/>
       <c r="Q38" s="29"/>
@@ -3353,7 +3371,7 @@
       <c r="M39" s="31"/>
       <c r="N39" s="31"/>
       <c r="O39" s="31" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="P39" s="29"/>
       <c r="Q39" s="29"/>
@@ -3399,7 +3417,7 @@
       <c r="M40" s="31"/>
       <c r="N40" s="31"/>
       <c r="O40" s="31" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="P40" s="29"/>
       <c r="Q40" s="29"/>
@@ -3726,10 +3744,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B85C046C-24FF-4202-B29D-53FEFBA5C312}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3850,7 +3868,7 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="E9" t="s">
         <v>33</v>
@@ -3858,7 +3876,7 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="E10" t="s">
         <v>231</v>
@@ -3885,6 +3903,42 @@
         <v>96</v>
       </c>
       <c r="E13" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>116</v>
+      </c>
+      <c r="B14" t="s">
+        <v>237</v>
+      </c>
+      <c r="C14" t="s">
+        <v>238</v>
+      </c>
+      <c r="D14" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>116</v>
+      </c>
+      <c r="B15" t="s">
+        <v>240</v>
+      </c>
+      <c r="C15" t="s">
+        <v>241</v>
+      </c>
+      <c r="D15" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>116</v>
+      </c>
+      <c r="E16" t="s">
         <v>234</v>
       </c>
     </row>
@@ -3917,40 +3971,40 @@
   <sheetData>
     <row r="1" spans="1:12" s="5" customFormat="1">
       <c r="A1" s="4" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -3970,19 +4024,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="B1" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="C1" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="D1" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="E1" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add 2 custom widgets map in household
Add custom helpers and geojson that was not possible to migrate to Evolution yet.
</commit_message>
<xml_diff>
--- a/example/demo_generator/references/Household_Travel_Generate_Survey.xlsx
+++ b/example/demo_generator/references/Household_Travel_Generate_Survey.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28928"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="1011" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{16609EB3-8854-4224-91CB-3373A9034551}"/>
+  <xr:revisionPtr revIDLastSave="1018" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62ECE760-9A17-495C-ADE5-20B0A6087FD8}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="260">
   <si>
     <t>questionName</t>
   </si>
@@ -1148,7 +1148,7 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1560,8 +1560,8 @@
   <dimension ref="A1:X42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="H19" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="O22" sqref="O22"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="B19" sqref="B19"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -2441,7 +2441,7 @@
       <c r="A19" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="37" t="s">
         <v>69</v>
       </c>
       <c r="C19" s="26" t="b">
@@ -2600,7 +2600,7 @@
       <c r="L22" s="29"/>
       <c r="M22" s="31"/>
       <c r="N22" s="29"/>
-      <c r="O22" s="37" t="s">
+      <c r="O22" s="29" t="s">
         <v>116</v>
       </c>
       <c r="P22" s="29"/>
@@ -3123,9 +3123,11 @@
       <c r="A34" s="27" t="s">
         <v>165</v>
       </c>
-      <c r="B34" s="27"/>
+      <c r="B34" s="32" t="s">
+        <v>69</v>
+      </c>
       <c r="C34" s="27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D34" s="27" t="s">
         <v>102</v>
@@ -3209,9 +3211,11 @@
       <c r="A36" s="27" t="s">
         <v>172</v>
       </c>
-      <c r="B36" s="27"/>
+      <c r="B36" s="32" t="s">
+        <v>69</v>
+      </c>
       <c r="C36" s="27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D36" s="27" t="s">
         <v>102</v>

</xml_diff>

<commit_message>
Generate labels with other gender
We want to generate labels with 'man', 'woman' and 'other' genders.
Remove getActivePersonId and getActivePersonId helpers functions.
Make a migration for gender values.
Add an adultAge on the config.
BREAKING CHANGE: We don't use 'male' and 'female' gender in survey anymore, because it's is dehumanizing to use 'female' and 'male'
You need to 'yarn migrate' when updating Evolution on a new survey.
</commit_message>
<xml_diff>
--- a/example/demo_generator/references/Household_Travel_Generate_Survey.xlsx
+++ b/example/demo_generator/references/Household_Travel_Generate_Survey.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28928"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="1018" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62ECE760-9A17-495C-ADE5-20B0A6087FD8}"/>
+  <xr:revisionPtr revIDLastSave="1027" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E51C2A9C-F1A6-4CE7-AB37-B37BAB07BA3E}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -461,7 +461,7 @@
     <t>studentType</t>
   </si>
   <si>
-    <t>**Étudiant{{gender:e}}**</t>
+    <t>**Étudiant{{gender:/e/·e}}**</t>
   </si>
   <si>
     <t>**Student**</t>
@@ -486,7 +486,7 @@
   </si>
   <si>
     <t>**Permis de conduire**
-__Inclure les permis d’apprenti{{gender:e}} conduct{{gender:eur/rice}} et probatoires, mais ne pas inclure les permis de cyclomoteur/scooter.__</t>
+__Inclure les permis d’apprenti{{gender:e}} conduct{{gender:eur/rice/eur·rice}} et probatoires, mais ne pas inclure les permis de cyclomoteur/scooter.__</t>
   </si>
   <si>
     <t>**Driver's licence**
@@ -603,7 +603,7 @@
     <t>travelToWorkDays</t>
   </si>
   <si>
-    <t>Durant la dernière **semaine**, quand est-ce que {{nickname}} s'est **déplacé{{gender:e}}** pour le **travail** ?
+    <t>Durant la dernière **semaine**, quand est-ce que {{nickname}} s'est **déplacé{{gender:/e/·e}}** pour le **travail** ?
 __Pour se rendre au travail ou toute autre raison concernant le travail.__</t>
   </si>
   <si>
@@ -629,7 +629,7 @@
     <t>travelToStudyDays</t>
   </si>
   <si>
-    <t>Durant la **dernière semaine**, est-ce que {{nickname}} s'est **déplacé{{gender:e}}** pour les **études**.
+    <t>Durant la **dernière semaine**, est-ce que {{nickname}} s'est **déplacé{{gender:/e/·e}}** pour les **études**.
 __Pour se rendre à l'établissement d'enseignement ou pour toute autre raison concernant les études.__</t>
   </si>
   <si>
@@ -1561,7 +1561,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="B19" sqref="B19"/>
+      <selection pane="bottomRight" activeCell="I23" sqref="I23"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -2818,7 +2818,7 @@
       <c r="F27" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="G27" s="32" t="s">
+      <c r="G27" s="27" t="s">
         <v>138</v>
       </c>
       <c r="H27" s="27" t="s">

</xml_diff>

<commit_message>
Add support for labels sheet names and update survey generation logic.
Fix: #1075
This will help to generate custom labels for everything that are not in the Widgets sheet.
</commit_message>
<xml_diff>
--- a/example/demo_generator/references/Household_Travel_Generate_Survey.xlsx
+++ b/example/demo_generator/references/Household_Travel_Generate_Survey.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Widgets" sheetId="1" state="visible" r:id="rId3"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="385">
   <si>
     <t xml:space="preserve">questionName</t>
   </si>
@@ -1226,28 +1226,29 @@
     <t xml:space="preserve">input_color</t>
   </si>
   <si>
-    <t xml:space="preserve">key</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fr_one</t>
-  </si>
-  <si>
-    <t xml:space="preserve">en</t>
-  </si>
-  <si>
-    <t xml:space="preserve">en_one</t>
+    <t xml:space="preserve">home.test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Test**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mon test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**My test**</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="165" formatCode="General"/>
+    <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
   <fonts count="17">
     <font>
@@ -1467,217 +1468,213 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="52">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2030,15 +2027,15 @@
   </sheetPr>
   <dimension ref="A1:X42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="L23" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="L1" activeCellId="0" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
-      <selection pane="bottomRight" activeCell="P30" activeCellId="0" sqref="P30"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.86"/>
@@ -2049,13 +2046,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="31.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="1" width="31.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="20.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="22.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="22.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="19.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="13.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="13.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="9.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="9.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="14.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="10.29"/>
@@ -2692,7 +2689,7 @@
       <c r="Q13" s="7"/>
       <c r="R13" s="7"/>
       <c r="S13" s="7"/>
-      <c r="T13" s="7" t="b">
+      <c r="T13" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2743,7 +2740,7 @@
       <c r="Q14" s="7"/>
       <c r="R14" s="7"/>
       <c r="S14" s="7"/>
-      <c r="T14" s="7" t="b">
+      <c r="T14" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3314,7 +3311,7 @@
       <c r="J26" s="19"/>
       <c r="K26" s="19"/>
       <c r="L26" s="23"/>
-      <c r="M26" s="27" t="s">
+      <c r="M26" s="23" t="s">
         <v>142</v>
       </c>
       <c r="N26" s="23"/>
@@ -3375,7 +3372,7 @@
       <c r="Q27" s="23"/>
       <c r="R27" s="23"/>
       <c r="S27" s="23"/>
-      <c r="T27" s="19" t="b">
+      <c r="T27" s="21" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3414,7 +3411,7 @@
       <c r="J28" s="19"/>
       <c r="K28" s="19"/>
       <c r="L28" s="23"/>
-      <c r="M28" s="27" t="s">
+      <c r="M28" s="23" t="s">
         <v>152</v>
       </c>
       <c r="N28" s="23"/>
@@ -3425,7 +3422,7 @@
       <c r="Q28" s="23"/>
       <c r="R28" s="23"/>
       <c r="S28" s="23"/>
-      <c r="T28" s="19" t="b">
+      <c r="T28" s="21" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3435,7 +3432,7 @@
       <c r="X28" s="23"/>
     </row>
     <row r="29" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="28" t="s">
+      <c r="A29" s="27" t="s">
         <v>153</v>
       </c>
       <c r="B29" s="19" t="s">
@@ -3464,7 +3461,7 @@
       <c r="J29" s="19"/>
       <c r="K29" s="19"/>
       <c r="L29" s="23"/>
-      <c r="M29" s="27" t="s">
+      <c r="M29" s="23" t="s">
         <v>158</v>
       </c>
       <c r="N29" s="24"/>
@@ -3514,7 +3511,7 @@
       <c r="J30" s="19"/>
       <c r="K30" s="19"/>
       <c r="L30" s="23"/>
-      <c r="M30" s="27" t="s">
+      <c r="M30" s="23" t="s">
         <v>164</v>
       </c>
       <c r="N30" s="23"/>
@@ -3564,7 +3561,7 @@
       <c r="J31" s="19"/>
       <c r="K31" s="19"/>
       <c r="L31" s="23"/>
-      <c r="M31" s="27" t="s">
+      <c r="M31" s="23" t="s">
         <v>169</v>
       </c>
       <c r="N31" s="23"/>
@@ -3614,7 +3611,7 @@
       <c r="J32" s="19"/>
       <c r="K32" s="19"/>
       <c r="L32" s="23"/>
-      <c r="M32" s="27" t="s">
+      <c r="M32" s="23" t="s">
         <v>174</v>
       </c>
       <c r="N32" s="23"/>
@@ -3651,7 +3648,7 @@
       <c r="E33" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="F33" s="27" t="s">
+      <c r="F33" s="23" t="s">
         <v>177</v>
       </c>
       <c r="G33" s="19" t="s">
@@ -3664,12 +3661,12 @@
       <c r="J33" s="19"/>
       <c r="K33" s="19"/>
       <c r="L33" s="23"/>
-      <c r="M33" s="29" t="s">
+      <c r="M33" s="19" t="s">
         <v>180</v>
       </c>
       <c r="N33" s="23"/>
       <c r="O33" s="23"/>
-      <c r="P33" s="27"/>
+      <c r="P33" s="23"/>
       <c r="Q33" s="23"/>
       <c r="R33" s="23"/>
       <c r="S33" s="23"/>
@@ -3686,7 +3683,7 @@
       <c r="A34" s="19" t="s">
         <v>181</v>
       </c>
-      <c r="B34" s="30" t="s">
+      <c r="B34" s="28" t="s">
         <v>69</v>
       </c>
       <c r="C34" s="21" t="b">
@@ -3699,7 +3696,7 @@
       <c r="E34" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="F34" s="27" t="s">
+      <c r="F34" s="23" t="s">
         <v>182</v>
       </c>
       <c r="G34" s="19" t="s">
@@ -3716,12 +3713,12 @@
       </c>
       <c r="K34" s="19"/>
       <c r="L34" s="23"/>
-      <c r="M34" s="29" t="s">
+      <c r="M34" s="19" t="s">
         <v>180</v>
       </c>
       <c r="N34" s="23"/>
       <c r="O34" s="23"/>
-      <c r="P34" s="27"/>
+      <c r="P34" s="23"/>
       <c r="Q34" s="23"/>
       <c r="R34" s="23"/>
       <c r="S34" s="23"/>
@@ -3751,7 +3748,7 @@
       <c r="E35" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="F35" s="27" t="s">
+      <c r="F35" s="23" t="s">
         <v>188</v>
       </c>
       <c r="G35" s="19" t="s">
@@ -3764,12 +3761,12 @@
       <c r="J35" s="19"/>
       <c r="K35" s="19"/>
       <c r="L35" s="23"/>
-      <c r="M35" s="29" t="s">
+      <c r="M35" s="19" t="s">
         <v>191</v>
       </c>
       <c r="N35" s="23"/>
       <c r="O35" s="23"/>
-      <c r="P35" s="27"/>
+      <c r="P35" s="23"/>
       <c r="Q35" s="23"/>
       <c r="R35" s="23"/>
       <c r="S35" s="23"/>
@@ -3786,7 +3783,7 @@
       <c r="A36" s="19" t="s">
         <v>192</v>
       </c>
-      <c r="B36" s="30" t="s">
+      <c r="B36" s="28" t="s">
         <v>69</v>
       </c>
       <c r="C36" s="21" t="b">
@@ -3799,7 +3796,7 @@
       <c r="E36" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="F36" s="27" t="s">
+      <c r="F36" s="23" t="s">
         <v>193</v>
       </c>
       <c r="G36" s="19" t="s">
@@ -3814,13 +3811,13 @@
       <c r="J36" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="K36" s="31"/>
-      <c r="L36" s="32"/>
-      <c r="M36" s="31"/>
-      <c r="N36" s="32"/>
-      <c r="O36" s="32"/>
-      <c r="P36" s="32"/>
-      <c r="Q36" s="33"/>
+      <c r="K36" s="29"/>
+      <c r="L36" s="30"/>
+      <c r="M36" s="29"/>
+      <c r="N36" s="30"/>
+      <c r="O36" s="30"/>
+      <c r="P36" s="30"/>
+      <c r="Q36" s="30"/>
       <c r="R36" s="23"/>
       <c r="S36" s="23"/>
       <c r="T36" s="21" t="b">
@@ -3833,7 +3830,7 @@
       <c r="X36" s="23"/>
     </row>
     <row r="37" customFormat="false" ht="86.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="28" t="s">
+      <c r="A37" s="27" t="s">
         <v>198</v>
       </c>
       <c r="B37" s="19" t="s">
@@ -3864,14 +3861,14 @@
       <c r="L37" s="23"/>
       <c r="M37" s="24"/>
       <c r="N37" s="24"/>
-      <c r="O37" s="34" t="s">
+      <c r="O37" s="31" t="s">
         <v>147</v>
       </c>
       <c r="P37" s="23"/>
       <c r="Q37" s="23"/>
       <c r="R37" s="23"/>
       <c r="S37" s="23"/>
-      <c r="T37" s="19" t="b">
+      <c r="T37" s="21" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3881,7 +3878,7 @@
       <c r="X37" s="23"/>
     </row>
     <row r="38" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="28" t="s">
+      <c r="A38" s="27" t="s">
         <v>202</v>
       </c>
       <c r="B38" s="19" t="s">
@@ -3912,7 +3909,7 @@
       <c r="L38" s="23"/>
       <c r="M38" s="24"/>
       <c r="N38" s="24"/>
-      <c r="O38" s="34" t="s">
+      <c r="O38" s="31" t="s">
         <v>147</v>
       </c>
       <c r="P38" s="23"/>
@@ -3929,7 +3926,7 @@
       <c r="X38" s="23"/>
     </row>
     <row r="39" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="28" t="s">
+      <c r="A39" s="27" t="s">
         <v>206</v>
       </c>
       <c r="B39" s="19" t="s">
@@ -3960,7 +3957,7 @@
       <c r="L39" s="23"/>
       <c r="M39" s="24"/>
       <c r="N39" s="24"/>
-      <c r="O39" s="34" t="s">
+      <c r="O39" s="31" t="s">
         <v>147</v>
       </c>
       <c r="P39" s="23"/>
@@ -3977,7 +3974,7 @@
       <c r="X39" s="23"/>
     </row>
     <row r="40" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="28" t="s">
+      <c r="A40" s="27" t="s">
         <v>210</v>
       </c>
       <c r="B40" s="19" t="s">
@@ -4008,7 +4005,7 @@
       <c r="L40" s="23"/>
       <c r="M40" s="24"/>
       <c r="N40" s="24"/>
-      <c r="O40" s="34" t="s">
+      <c r="O40" s="31" t="s">
         <v>147</v>
       </c>
       <c r="P40" s="23"/>
@@ -4025,49 +4022,49 @@
       <c r="X40" s="23"/>
     </row>
     <row r="41" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="35" t="s">
+      <c r="A41" s="32" t="s">
         <v>214</v>
       </c>
-      <c r="B41" s="35" t="s">
+      <c r="B41" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="C41" s="36" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D41" s="35" t="s">
+      <c r="C41" s="33" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D41" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="E41" s="37"/>
-      <c r="F41" s="37" t="str">
+      <c r="E41" s="34"/>
+      <c r="F41" s="34" t="str">
         <f aca="false">REPLACE(A41, FIND("_", A41), 1, ".")</f>
         <v>household.save</v>
       </c>
-      <c r="G41" s="35" t="s">
+      <c r="G41" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="H41" s="35" t="s">
+      <c r="H41" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="I41" s="35"/>
-      <c r="J41" s="35"/>
-      <c r="K41" s="35"/>
-      <c r="L41" s="37"/>
-      <c r="M41" s="37"/>
-      <c r="N41" s="37"/>
-      <c r="O41" s="37"/>
-      <c r="P41" s="37"/>
-      <c r="Q41" s="37"/>
-      <c r="R41" s="37"/>
-      <c r="S41" s="37"/>
-      <c r="T41" s="36" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U41" s="37"/>
-      <c r="V41" s="37"/>
-      <c r="W41" s="37"/>
-      <c r="X41" s="37"/>
+      <c r="I41" s="32"/>
+      <c r="J41" s="32"/>
+      <c r="K41" s="32"/>
+      <c r="L41" s="34"/>
+      <c r="M41" s="34"/>
+      <c r="N41" s="34"/>
+      <c r="O41" s="34"/>
+      <c r="P41" s="34"/>
+      <c r="Q41" s="34"/>
+      <c r="R41" s="34"/>
+      <c r="S41" s="34"/>
+      <c r="T41" s="33" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U41" s="34"/>
+      <c r="V41" s="34"/>
+      <c r="W41" s="34"/>
+      <c r="X41" s="34"/>
     </row>
     <row r="42" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
@@ -4076,7 +4073,7 @@
       <c r="B42" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C42" s="38" t="b">
+      <c r="C42" s="35" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4092,9 +4089,9 @@
       <c r="H42" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="L42" s="39"/>
-      <c r="M42" s="40"/>
-      <c r="T42" s="38" t="b">
+      <c r="L42" s="36"/>
+      <c r="M42" s="37"/>
+      <c r="T42" s="35" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4154,487 +4151,487 @@
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="41" width="20.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="38" width="27.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="38" width="15.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="38" width="31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="39" width="20.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="38" width="19.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="38" width="12.14"/>
   </cols>
   <sheetData>
-    <row r="1" s="44" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="42" t="s">
+    <row r="1" s="42" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="40" t="s">
         <v>219</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="40" t="s">
         <v>220</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="41" t="s">
         <v>221</v>
       </c>
-      <c r="E1" s="42" t="s">
+      <c r="E1" s="40" t="s">
         <v>222</v>
       </c>
-      <c r="F1" s="42" t="s">
+      <c r="F1" s="40" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="43" t="s">
         <v>224</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45" t="s">
+      <c r="B2" s="43"/>
+      <c r="C2" s="43" t="s">
         <v>225</v>
       </c>
-      <c r="D2" s="46" t="s">
+      <c r="D2" s="44" t="s">
         <v>226</v>
       </c>
-      <c r="E2" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="F2" s="45"/>
+      <c r="E2" s="43" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="43"/>
     </row>
     <row r="3" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45" t="s">
+      <c r="B3" s="43"/>
+      <c r="C3" s="43" t="s">
         <v>225</v>
       </c>
-      <c r="D3" s="46" t="s">
+      <c r="D3" s="44" t="s">
         <v>227</v>
       </c>
-      <c r="E3" s="45" t="n">
+      <c r="E3" s="43" t="n">
         <v>2</v>
       </c>
-      <c r="F3" s="45"/>
+      <c r="F3" s="43"/>
     </row>
     <row r="4" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="43" t="s">
         <v>164</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45" t="s">
+      <c r="B4" s="43"/>
+      <c r="C4" s="43" t="s">
         <v>228</v>
       </c>
-      <c r="D4" s="46" t="s">
+      <c r="D4" s="44" t="s">
         <v>226</v>
       </c>
-      <c r="E4" s="45" t="s">
+      <c r="E4" s="43" t="s">
         <v>229</v>
       </c>
-      <c r="F4" s="45"/>
+      <c r="F4" s="43"/>
     </row>
     <row r="5" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="43" t="s">
         <v>164</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="43" t="s">
         <v>230</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="43" t="s">
         <v>225</v>
       </c>
-      <c r="D5" s="46" t="s">
+      <c r="D5" s="44" t="s">
         <v>226</v>
       </c>
-      <c r="E5" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" s="45"/>
+      <c r="E5" s="43" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="43"/>
     </row>
     <row r="6" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="43" t="s">
         <v>231</v>
       </c>
-      <c r="B6" s="45"/>
-      <c r="C6" s="45" t="s">
+      <c r="B6" s="43"/>
+      <c r="C6" s="43" t="s">
         <v>232</v>
       </c>
-      <c r="D6" s="46" t="s">
+      <c r="D6" s="44" t="s">
         <v>227</v>
       </c>
-      <c r="E6" s="45" t="n">
+      <c r="E6" s="43" t="n">
         <v>3</v>
       </c>
-      <c r="F6" s="45"/>
+      <c r="F6" s="43"/>
     </row>
     <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="43" t="s">
         <v>231</v>
       </c>
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="43" t="s">
         <v>233</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="43" t="s">
         <v>232</v>
       </c>
-      <c r="D7" s="46" t="s">
+      <c r="D7" s="44" t="s">
         <v>234</v>
       </c>
-      <c r="E7" s="45" t="n">
+      <c r="E7" s="43" t="n">
         <v>5</v>
       </c>
-      <c r="F7" s="45"/>
+      <c r="F7" s="43"/>
     </row>
     <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="43" t="s">
         <v>235</v>
       </c>
-      <c r="B8" s="45"/>
-      <c r="C8" s="45" t="s">
+      <c r="B8" s="43"/>
+      <c r="C8" s="43" t="s">
         <v>232</v>
       </c>
-      <c r="D8" s="46" t="s">
+      <c r="D8" s="44" t="s">
         <v>227</v>
       </c>
-      <c r="E8" s="45" t="n">
+      <c r="E8" s="43" t="n">
         <v>4</v>
       </c>
-      <c r="F8" s="45"/>
+      <c r="F8" s="43"/>
     </row>
     <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="43" t="s">
         <v>235</v>
       </c>
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="43" t="s">
         <v>233</v>
       </c>
-      <c r="C9" s="45" t="s">
+      <c r="C9" s="43" t="s">
         <v>232</v>
       </c>
-      <c r="D9" s="46" t="s">
+      <c r="D9" s="44" t="s">
         <v>234</v>
       </c>
-      <c r="E9" s="45" t="n">
+      <c r="E9" s="43" t="n">
         <v>13</v>
       </c>
-      <c r="F9" s="45"/>
+      <c r="F9" s="43"/>
     </row>
     <row r="10" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="43" t="s">
         <v>236</v>
       </c>
-      <c r="B10" s="45"/>
-      <c r="C10" s="45" t="s">
+      <c r="B10" s="43"/>
+      <c r="C10" s="43" t="s">
         <v>232</v>
       </c>
-      <c r="D10" s="46" t="s">
+      <c r="D10" s="44" t="s">
         <v>234</v>
       </c>
-      <c r="E10" s="45" t="n">
+      <c r="E10" s="43" t="n">
         <v>5</v>
       </c>
-      <c r="F10" s="45"/>
+      <c r="F10" s="43"/>
     </row>
     <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="43" t="s">
         <v>119</v>
       </c>
-      <c r="B11" s="45"/>
-      <c r="C11" s="45" t="s">
+      <c r="B11" s="43"/>
+      <c r="C11" s="43" t="s">
         <v>232</v>
       </c>
-      <c r="D11" s="46" t="s">
+      <c r="D11" s="44" t="s">
         <v>227</v>
       </c>
-      <c r="E11" s="45" t="n">
+      <c r="E11" s="43" t="n">
         <v>5</v>
       </c>
-      <c r="F11" s="45"/>
+      <c r="F11" s="43"/>
     </row>
     <row r="12" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="43" t="s">
         <v>158</v>
       </c>
-      <c r="B12" s="45"/>
-      <c r="C12" s="45" t="s">
+      <c r="B12" s="43"/>
+      <c r="C12" s="43" t="s">
         <v>232</v>
       </c>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="44" t="s">
         <v>227</v>
       </c>
-      <c r="E12" s="45" t="n">
+      <c r="E12" s="43" t="n">
         <v>6</v>
       </c>
-      <c r="F12" s="45"/>
+      <c r="F12" s="43"/>
     </row>
     <row r="13" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="43" t="s">
         <v>237</v>
       </c>
-      <c r="B13" s="45"/>
-      <c r="C13" s="45" t="s">
+      <c r="B13" s="43"/>
+      <c r="C13" s="43" t="s">
         <v>232</v>
       </c>
-      <c r="D13" s="46" t="s">
+      <c r="D13" s="44" t="s">
         <v>227</v>
       </c>
-      <c r="E13" s="45" t="n">
+      <c r="E13" s="43" t="n">
         <v>11</v>
       </c>
-      <c r="F13" s="45"/>
+      <c r="F13" s="43"/>
     </row>
     <row r="14" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="45" t="s">
+      <c r="A14" s="43" t="s">
         <v>124</v>
       </c>
-      <c r="B14" s="45"/>
-      <c r="C14" s="45" t="s">
+      <c r="B14" s="43"/>
+      <c r="C14" s="43" t="s">
         <v>232</v>
       </c>
-      <c r="D14" s="46" t="s">
+      <c r="D14" s="44" t="s">
         <v>227</v>
       </c>
-      <c r="E14" s="45" t="n">
+      <c r="E14" s="43" t="n">
         <v>14</v>
       </c>
-      <c r="F14" s="45"/>
+      <c r="F14" s="43"/>
     </row>
     <row r="15" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="45" t="s">
+      <c r="A15" s="43" t="s">
         <v>135</v>
       </c>
-      <c r="B15" s="45"/>
-      <c r="C15" s="45" t="s">
+      <c r="B15" s="43"/>
+      <c r="C15" s="43" t="s">
         <v>232</v>
       </c>
-      <c r="D15" s="46" t="s">
+      <c r="D15" s="44" t="s">
         <v>234</v>
       </c>
-      <c r="E15" s="45" t="n">
+      <c r="E15" s="43" t="n">
         <v>15</v>
       </c>
-      <c r="F15" s="45"/>
+      <c r="F15" s="43"/>
     </row>
     <row r="16" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="45" t="s">
+      <c r="A16" s="43" t="s">
         <v>135</v>
       </c>
-      <c r="B16" s="45"/>
-      <c r="C16" s="45" t="s">
+      <c r="B16" s="43"/>
+      <c r="C16" s="43" t="s">
         <v>232</v>
       </c>
-      <c r="D16" s="46" t="s">
+      <c r="D16" s="44" t="s">
         <v>238</v>
       </c>
-      <c r="E16" s="45" t="s">
+      <c r="E16" s="43" t="s">
         <v>239</v>
       </c>
-      <c r="F16" s="45"/>
+      <c r="F16" s="43"/>
     </row>
     <row r="17" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="45" t="s">
+      <c r="A17" s="43" t="s">
         <v>240</v>
       </c>
-      <c r="B17" s="45"/>
-      <c r="C17" s="45" t="s">
+      <c r="B17" s="43"/>
+      <c r="C17" s="43" t="s">
         <v>232</v>
       </c>
-      <c r="D17" s="46" t="s">
+      <c r="D17" s="44" t="s">
         <v>227</v>
       </c>
-      <c r="E17" s="45" t="n">
+      <c r="E17" s="43" t="n">
         <v>15</v>
       </c>
-      <c r="F17" s="45"/>
+      <c r="F17" s="43"/>
     </row>
     <row r="18" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="45" t="s">
+      <c r="A18" s="43" t="s">
         <v>130</v>
       </c>
-      <c r="B18" s="45"/>
-      <c r="C18" s="45" t="s">
+      <c r="B18" s="43"/>
+      <c r="C18" s="43" t="s">
         <v>232</v>
       </c>
-      <c r="D18" s="46" t="s">
+      <c r="D18" s="44" t="s">
         <v>227</v>
       </c>
-      <c r="E18" s="45" t="n">
+      <c r="E18" s="43" t="n">
         <v>16</v>
       </c>
-      <c r="F18" s="45"/>
+      <c r="F18" s="43"/>
     </row>
     <row r="19" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="45" t="s">
+      <c r="A19" s="43" t="s">
         <v>241</v>
       </c>
-      <c r="B19" s="45"/>
-      <c r="C19" s="45" t="s">
+      <c r="B19" s="43"/>
+      <c r="C19" s="43" t="s">
         <v>232</v>
       </c>
-      <c r="D19" s="46" t="s">
+      <c r="D19" s="44" t="s">
         <v>227</v>
       </c>
-      <c r="E19" s="45" t="n">
+      <c r="E19" s="43" t="n">
         <v>40</v>
       </c>
-      <c r="F19" s="45"/>
+      <c r="F19" s="43"/>
     </row>
     <row r="20" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="45" t="s">
+      <c r="A20" s="43" t="s">
         <v>152</v>
       </c>
-      <c r="B20" s="45"/>
-      <c r="C20" s="45" t="s">
+      <c r="B20" s="43"/>
+      <c r="C20" s="43" t="s">
         <v>242</v>
       </c>
-      <c r="D20" s="46" t="s">
+      <c r="D20" s="44" t="s">
         <v>226</v>
       </c>
-      <c r="E20" s="45" t="s">
+      <c r="E20" s="43" t="s">
         <v>229</v>
       </c>
-      <c r="F20" s="45"/>
+      <c r="F20" s="43"/>
     </row>
     <row r="21" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="38" t="s">
         <v>169</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="D21" s="46" t="s">
+      <c r="D21" s="44" t="s">
         <v>226</v>
       </c>
-      <c r="E21" s="41" t="s">
+      <c r="E21" s="39" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="38" t="s">
         <v>169</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="38" t="s">
         <v>230</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="D22" s="46" t="s">
+      <c r="D22" s="44" t="s">
         <v>226</v>
       </c>
-      <c r="E22" s="41" t="s">
+      <c r="E22" s="39" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="38" t="s">
         <v>169</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="38" t="s">
         <v>230</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="D23" s="46" t="s">
+      <c r="D23" s="44" t="s">
         <v>226</v>
       </c>
-      <c r="E23" s="41" t="s">
+      <c r="E23" s="39" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="C24" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="D24" s="46" t="s">
+      <c r="D24" s="44" t="s">
         <v>226</v>
       </c>
-      <c r="E24" s="41" t="s">
+      <c r="E24" s="39" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="38" t="s">
         <v>230</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="C25" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="D25" s="46" t="s">
+      <c r="D25" s="44" t="s">
         <v>226</v>
       </c>
-      <c r="E25" s="41" t="s">
+      <c r="E25" s="39" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="38" t="s">
         <v>230</v>
       </c>
-      <c r="C26" s="0" t="s">
+      <c r="C26" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="D26" s="46" t="s">
+      <c r="D26" s="44" t="s">
         <v>226</v>
       </c>
-      <c r="E26" s="41" t="s">
+      <c r="E26" s="39" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="38" t="s">
         <v>180</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="C27" s="38" t="s">
         <v>249</v>
       </c>
-      <c r="D27" s="46" t="s">
+      <c r="D27" s="44" t="s">
         <v>226</v>
       </c>
-      <c r="E27" s="0" t="s">
+      <c r="E27" s="38" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="38" t="s">
         <v>180</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="38" t="s">
         <v>230</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="C28" s="38" t="s">
         <v>249</v>
       </c>
-      <c r="D28" s="46" t="s">
+      <c r="D28" s="44" t="s">
         <v>226</v>
       </c>
-      <c r="E28" s="0" t="s">
+      <c r="E28" s="38" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="38" t="s">
         <v>180</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="38" t="s">
         <v>230</v>
       </c>
-      <c r="C29" s="0" t="s">
+      <c r="C29" s="38" t="s">
         <v>249</v>
       </c>
-      <c r="D29" s="46" t="s">
+      <c r="D29" s="44" t="s">
         <v>226</v>
       </c>
-      <c r="E29" s="0" t="s">
+      <c r="E29" s="38" t="s">
         <v>252</v>
       </c>
     </row>
@@ -4660,118 +4657,118 @@
       <selection pane="topLeft" activeCell="L15" activeCellId="0" sqref="L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.71484375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="45" width="10.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="45" width="12.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="45" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="45" width="12.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="45" width="10.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="45" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="45" width="15.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="9" style="45" width="10.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="43" width="10.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="43" width="12.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="43" width="13.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="43" width="12.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="43" width="10.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="43" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="43" width="15.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="9" style="43" width="10.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="46" t="s">
         <v>253</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="45" t="s">
         <v>254</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="45" t="s">
         <v>255</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="45" t="s">
         <v>256</v>
       </c>
-      <c r="F1" s="47" t="s">
+      <c r="F1" s="45" t="s">
         <v>257</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="H1" s="47" t="s">
+      <c r="H1" s="45" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="43" t="s">
         <v>260</v>
       </c>
-      <c r="C2" s="45" t="s">
+      <c r="C2" s="43" t="s">
         <v>261</v>
       </c>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="43" t="s">
         <v>262</v>
       </c>
-      <c r="E2" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F2" s="49" t="b">
+      <c r="E2" s="47" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="47" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G2" s="49" t="b">
+      <c r="G2" s="47" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="43" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="43" t="s">
         <v>263</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="43" t="s">
         <v>264</v>
       </c>
-      <c r="D3" s="45" t="s">
+      <c r="D3" s="43" t="s">
         <v>265</v>
       </c>
-      <c r="E3" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F3" s="49" t="b">
+      <c r="E3" s="47" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F3" s="47" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G3" s="49" t="b">
+      <c r="G3" s="47" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="43" t="s">
         <v>216</v>
       </c>
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="43" t="s">
         <v>266</v>
       </c>
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="43" t="s">
         <v>267</v>
       </c>
-      <c r="D4" s="45" t="s">
+      <c r="D4" s="43" t="s">
         <v>268</v>
       </c>
-      <c r="E4" s="49" t="b">
+      <c r="E4" s="47" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F4" s="49" t="b">
+      <c r="F4" s="47" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G4" s="49" t="b">
+      <c r="G4" s="47" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4798,33 +4795,33 @@
       <selection pane="topLeft" activeCell="A45" activeCellId="0" sqref="A45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="50" width="21.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="50" width="15.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="50" width="23.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="50" width="19.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="50" width="24.29"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="7" style="50" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="48" width="21.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="48" width="15.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="48" width="23.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="48" width="19.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="48" width="24.29"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="7" style="48" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="49" t="s">
         <v>269</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="49" t="s">
         <v>222</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="49" t="s">
         <v>270</v>
       </c>
-      <c r="F1" s="51" t="s">
+      <c r="F1" s="49" t="s">
         <v>12</v>
       </c>
     </row>
@@ -5543,44 +5540,44 @@
       <c r="F48" s="1"/>
     </row>
     <row r="49" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="50" t="s">
+      <c r="A49" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="B49" s="50" t="s">
+      <c r="B49" s="48" t="s">
         <v>250</v>
       </c>
-      <c r="C49" s="50" t="s">
+      <c r="C49" s="48" t="s">
         <v>363</v>
       </c>
-      <c r="D49" s="50" t="s">
+      <c r="D49" s="48" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="50" t="s">
+      <c r="A50" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="B50" s="50" t="s">
+      <c r="B50" s="48" t="s">
         <v>251</v>
       </c>
-      <c r="C50" s="50" t="s">
+      <c r="C50" s="48" t="s">
         <v>364</v>
       </c>
-      <c r="D50" s="50" t="s">
+      <c r="D50" s="48" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="50" t="s">
+      <c r="A51" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="B51" s="50" t="s">
+      <c r="B51" s="48" t="s">
         <v>360</v>
       </c>
-      <c r="C51" s="50" t="s">
+      <c r="C51" s="48" t="s">
         <v>366</v>
       </c>
-      <c r="D51" s="50" t="s">
+      <c r="D51" s="48" t="s">
         <v>367</v>
       </c>
     </row>
@@ -5606,55 +5603,55 @@
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="38" width="18.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="38" width="17.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="38" width="13.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="38" width="12.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="38" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="38" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="38" width="14.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="38" width="11.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="38" width="13.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="38" width="14.43"/>
   </cols>
   <sheetData>
-    <row r="1" s="51" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="52" t="s">
+    <row r="1" s="49" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="50" t="s">
         <v>368</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="50" t="s">
         <v>369</v>
       </c>
-      <c r="C1" s="52" t="s">
+      <c r="C1" s="50" t="s">
         <v>370</v>
       </c>
-      <c r="D1" s="52" t="s">
+      <c r="D1" s="50" t="s">
         <v>371</v>
       </c>
-      <c r="E1" s="52" t="s">
+      <c r="E1" s="50" t="s">
         <v>372</v>
       </c>
-      <c r="F1" s="52" t="s">
+      <c r="F1" s="50" t="s">
         <v>373</v>
       </c>
-      <c r="G1" s="52" t="s">
+      <c r="G1" s="50" t="s">
         <v>374</v>
       </c>
-      <c r="H1" s="52" t="s">
+      <c r="H1" s="50" t="s">
         <v>375</v>
       </c>
-      <c r="I1" s="52" t="s">
+      <c r="I1" s="50" t="s">
         <v>376</v>
       </c>
-      <c r="J1" s="52" t="s">
+      <c r="J1" s="50" t="s">
         <v>377</v>
       </c>
-      <c r="K1" s="52" t="s">
+      <c r="K1" s="50" t="s">
         <v>378</v>
       </c>
-      <c r="L1" s="51" t="s">
+      <c r="L1" s="49" t="s">
         <v>379</v>
       </c>
     </row>
@@ -5674,28 +5671,56 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="0" width="28.55"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="38"/>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="51" t="s">
         <v>380</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="C2" s="51" t="s">
         <v>381</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D2" s="51" t="s">
         <v>382</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E2" s="51" t="s">
         <v>383</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F2" s="51" t="s">
         <v>384</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add support for labels sheet names and fix gender label bug (#1078)
* Add support for labels sheet names and update survey generation logic.

Fix: #1075
This will help to generate custom labels for everything that are not in the Widgets sheet.

* Fix expand_gender to handle space after 'gender' in labels and add corresponding test case.

Fix: #1076

* Refactor label generation to iterate over sheet names, reducing code duplication

* Explain expand_gender function to handle variations in spacing around the colon in gender labels.

* Refactor label generation to support multiple sheet names and improve file deletion logic.

* Refactor function names to follow snake_case convention and add tests for merged_section_translations functionality.
</commit_message>
<xml_diff>
--- a/example/demo_generator/references/Household_Travel_Generate_Survey.xlsx
+++ b/example/demo_generator/references/Household_Travel_Generate_Survey.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Widgets" sheetId="1" state="visible" r:id="rId3"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="385">
   <si>
     <t xml:space="preserve">questionName</t>
   </si>
@@ -1226,28 +1226,29 @@
     <t xml:space="preserve">input_color</t>
   </si>
   <si>
-    <t xml:space="preserve">key</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fr_one</t>
-  </si>
-  <si>
-    <t xml:space="preserve">en</t>
-  </si>
-  <si>
-    <t xml:space="preserve">en_one</t>
+    <t xml:space="preserve">home.test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Test**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mon test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**My test**</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="165" formatCode="General"/>
+    <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
   <fonts count="17">
     <font>
@@ -1467,217 +1468,213 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="52">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2030,15 +2027,15 @@
   </sheetPr>
   <dimension ref="A1:X42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="L23" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="L1" activeCellId="0" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
-      <selection pane="bottomRight" activeCell="P30" activeCellId="0" sqref="P30"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.86"/>
@@ -2049,13 +2046,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="31.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="1" width="31.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="20.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="22.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="22.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="19.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="13.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="13.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="9.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="9.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="14.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="10.29"/>
@@ -2692,7 +2689,7 @@
       <c r="Q13" s="7"/>
       <c r="R13" s="7"/>
       <c r="S13" s="7"/>
-      <c r="T13" s="7" t="b">
+      <c r="T13" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2743,7 +2740,7 @@
       <c r="Q14" s="7"/>
       <c r="R14" s="7"/>
       <c r="S14" s="7"/>
-      <c r="T14" s="7" t="b">
+      <c r="T14" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3314,7 +3311,7 @@
       <c r="J26" s="19"/>
       <c r="K26" s="19"/>
       <c r="L26" s="23"/>
-      <c r="M26" s="27" t="s">
+      <c r="M26" s="23" t="s">
         <v>142</v>
       </c>
       <c r="N26" s="23"/>
@@ -3375,7 +3372,7 @@
       <c r="Q27" s="23"/>
       <c r="R27" s="23"/>
       <c r="S27" s="23"/>
-      <c r="T27" s="19" t="b">
+      <c r="T27" s="21" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3414,7 +3411,7 @@
       <c r="J28" s="19"/>
       <c r="K28" s="19"/>
       <c r="L28" s="23"/>
-      <c r="M28" s="27" t="s">
+      <c r="M28" s="23" t="s">
         <v>152</v>
       </c>
       <c r="N28" s="23"/>
@@ -3425,7 +3422,7 @@
       <c r="Q28" s="23"/>
       <c r="R28" s="23"/>
       <c r="S28" s="23"/>
-      <c r="T28" s="19" t="b">
+      <c r="T28" s="21" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3435,7 +3432,7 @@
       <c r="X28" s="23"/>
     </row>
     <row r="29" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="28" t="s">
+      <c r="A29" s="27" t="s">
         <v>153</v>
       </c>
       <c r="B29" s="19" t="s">
@@ -3464,7 +3461,7 @@
       <c r="J29" s="19"/>
       <c r="K29" s="19"/>
       <c r="L29" s="23"/>
-      <c r="M29" s="27" t="s">
+      <c r="M29" s="23" t="s">
         <v>158</v>
       </c>
       <c r="N29" s="24"/>
@@ -3514,7 +3511,7 @@
       <c r="J30" s="19"/>
       <c r="K30" s="19"/>
       <c r="L30" s="23"/>
-      <c r="M30" s="27" t="s">
+      <c r="M30" s="23" t="s">
         <v>164</v>
       </c>
       <c r="N30" s="23"/>
@@ -3564,7 +3561,7 @@
       <c r="J31" s="19"/>
       <c r="K31" s="19"/>
       <c r="L31" s="23"/>
-      <c r="M31" s="27" t="s">
+      <c r="M31" s="23" t="s">
         <v>169</v>
       </c>
       <c r="N31" s="23"/>
@@ -3614,7 +3611,7 @@
       <c r="J32" s="19"/>
       <c r="K32" s="19"/>
       <c r="L32" s="23"/>
-      <c r="M32" s="27" t="s">
+      <c r="M32" s="23" t="s">
         <v>174</v>
       </c>
       <c r="N32" s="23"/>
@@ -3651,7 +3648,7 @@
       <c r="E33" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="F33" s="27" t="s">
+      <c r="F33" s="23" t="s">
         <v>177</v>
       </c>
       <c r="G33" s="19" t="s">
@@ -3664,12 +3661,12 @@
       <c r="J33" s="19"/>
       <c r="K33" s="19"/>
       <c r="L33" s="23"/>
-      <c r="M33" s="29" t="s">
+      <c r="M33" s="19" t="s">
         <v>180</v>
       </c>
       <c r="N33" s="23"/>
       <c r="O33" s="23"/>
-      <c r="P33" s="27"/>
+      <c r="P33" s="23"/>
       <c r="Q33" s="23"/>
       <c r="R33" s="23"/>
       <c r="S33" s="23"/>
@@ -3686,7 +3683,7 @@
       <c r="A34" s="19" t="s">
         <v>181</v>
       </c>
-      <c r="B34" s="30" t="s">
+      <c r="B34" s="28" t="s">
         <v>69</v>
       </c>
       <c r="C34" s="21" t="b">
@@ -3699,7 +3696,7 @@
       <c r="E34" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="F34" s="27" t="s">
+      <c r="F34" s="23" t="s">
         <v>182</v>
       </c>
       <c r="G34" s="19" t="s">
@@ -3716,12 +3713,12 @@
       </c>
       <c r="K34" s="19"/>
       <c r="L34" s="23"/>
-      <c r="M34" s="29" t="s">
+      <c r="M34" s="19" t="s">
         <v>180</v>
       </c>
       <c r="N34" s="23"/>
       <c r="O34" s="23"/>
-      <c r="P34" s="27"/>
+      <c r="P34" s="23"/>
       <c r="Q34" s="23"/>
       <c r="R34" s="23"/>
       <c r="S34" s="23"/>
@@ -3751,7 +3748,7 @@
       <c r="E35" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="F35" s="27" t="s">
+      <c r="F35" s="23" t="s">
         <v>188</v>
       </c>
       <c r="G35" s="19" t="s">
@@ -3764,12 +3761,12 @@
       <c r="J35" s="19"/>
       <c r="K35" s="19"/>
       <c r="L35" s="23"/>
-      <c r="M35" s="29" t="s">
+      <c r="M35" s="19" t="s">
         <v>191</v>
       </c>
       <c r="N35" s="23"/>
       <c r="O35" s="23"/>
-      <c r="P35" s="27"/>
+      <c r="P35" s="23"/>
       <c r="Q35" s="23"/>
       <c r="R35" s="23"/>
       <c r="S35" s="23"/>
@@ -3786,7 +3783,7 @@
       <c r="A36" s="19" t="s">
         <v>192</v>
       </c>
-      <c r="B36" s="30" t="s">
+      <c r="B36" s="28" t="s">
         <v>69</v>
       </c>
       <c r="C36" s="21" t="b">
@@ -3799,7 +3796,7 @@
       <c r="E36" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="F36" s="27" t="s">
+      <c r="F36" s="23" t="s">
         <v>193</v>
       </c>
       <c r="G36" s="19" t="s">
@@ -3814,13 +3811,13 @@
       <c r="J36" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="K36" s="31"/>
-      <c r="L36" s="32"/>
-      <c r="M36" s="31"/>
-      <c r="N36" s="32"/>
-      <c r="O36" s="32"/>
-      <c r="P36" s="32"/>
-      <c r="Q36" s="33"/>
+      <c r="K36" s="29"/>
+      <c r="L36" s="30"/>
+      <c r="M36" s="29"/>
+      <c r="N36" s="30"/>
+      <c r="O36" s="30"/>
+      <c r="P36" s="30"/>
+      <c r="Q36" s="30"/>
       <c r="R36" s="23"/>
       <c r="S36" s="23"/>
       <c r="T36" s="21" t="b">
@@ -3833,7 +3830,7 @@
       <c r="X36" s="23"/>
     </row>
     <row r="37" customFormat="false" ht="86.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="28" t="s">
+      <c r="A37" s="27" t="s">
         <v>198</v>
       </c>
       <c r="B37" s="19" t="s">
@@ -3864,14 +3861,14 @@
       <c r="L37" s="23"/>
       <c r="M37" s="24"/>
       <c r="N37" s="24"/>
-      <c r="O37" s="34" t="s">
+      <c r="O37" s="31" t="s">
         <v>147</v>
       </c>
       <c r="P37" s="23"/>
       <c r="Q37" s="23"/>
       <c r="R37" s="23"/>
       <c r="S37" s="23"/>
-      <c r="T37" s="19" t="b">
+      <c r="T37" s="21" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3881,7 +3878,7 @@
       <c r="X37" s="23"/>
     </row>
     <row r="38" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="28" t="s">
+      <c r="A38" s="27" t="s">
         <v>202</v>
       </c>
       <c r="B38" s="19" t="s">
@@ -3912,7 +3909,7 @@
       <c r="L38" s="23"/>
       <c r="M38" s="24"/>
       <c r="N38" s="24"/>
-      <c r="O38" s="34" t="s">
+      <c r="O38" s="31" t="s">
         <v>147</v>
       </c>
       <c r="P38" s="23"/>
@@ -3929,7 +3926,7 @@
       <c r="X38" s="23"/>
     </row>
     <row r="39" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="28" t="s">
+      <c r="A39" s="27" t="s">
         <v>206</v>
       </c>
       <c r="B39" s="19" t="s">
@@ -3960,7 +3957,7 @@
       <c r="L39" s="23"/>
       <c r="M39" s="24"/>
       <c r="N39" s="24"/>
-      <c r="O39" s="34" t="s">
+      <c r="O39" s="31" t="s">
         <v>147</v>
       </c>
       <c r="P39" s="23"/>
@@ -3977,7 +3974,7 @@
       <c r="X39" s="23"/>
     </row>
     <row r="40" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="28" t="s">
+      <c r="A40" s="27" t="s">
         <v>210</v>
       </c>
       <c r="B40" s="19" t="s">
@@ -4008,7 +4005,7 @@
       <c r="L40" s="23"/>
       <c r="M40" s="24"/>
       <c r="N40" s="24"/>
-      <c r="O40" s="34" t="s">
+      <c r="O40" s="31" t="s">
         <v>147</v>
       </c>
       <c r="P40" s="23"/>
@@ -4025,49 +4022,49 @@
       <c r="X40" s="23"/>
     </row>
     <row r="41" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="35" t="s">
+      <c r="A41" s="32" t="s">
         <v>214</v>
       </c>
-      <c r="B41" s="35" t="s">
+      <c r="B41" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="C41" s="36" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D41" s="35" t="s">
+      <c r="C41" s="33" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D41" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="E41" s="37"/>
-      <c r="F41" s="37" t="str">
+      <c r="E41" s="34"/>
+      <c r="F41" s="34" t="str">
         <f aca="false">REPLACE(A41, FIND("_", A41), 1, ".")</f>
         <v>household.save</v>
       </c>
-      <c r="G41" s="35" t="s">
+      <c r="G41" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="H41" s="35" t="s">
+      <c r="H41" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="I41" s="35"/>
-      <c r="J41" s="35"/>
-      <c r="K41" s="35"/>
-      <c r="L41" s="37"/>
-      <c r="M41" s="37"/>
-      <c r="N41" s="37"/>
-      <c r="O41" s="37"/>
-      <c r="P41" s="37"/>
-      <c r="Q41" s="37"/>
-      <c r="R41" s="37"/>
-      <c r="S41" s="37"/>
-      <c r="T41" s="36" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U41" s="37"/>
-      <c r="V41" s="37"/>
-      <c r="W41" s="37"/>
-      <c r="X41" s="37"/>
+      <c r="I41" s="32"/>
+      <c r="J41" s="32"/>
+      <c r="K41" s="32"/>
+      <c r="L41" s="34"/>
+      <c r="M41" s="34"/>
+      <c r="N41" s="34"/>
+      <c r="O41" s="34"/>
+      <c r="P41" s="34"/>
+      <c r="Q41" s="34"/>
+      <c r="R41" s="34"/>
+      <c r="S41" s="34"/>
+      <c r="T41" s="33" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U41" s="34"/>
+      <c r="V41" s="34"/>
+      <c r="W41" s="34"/>
+      <c r="X41" s="34"/>
     </row>
     <row r="42" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
@@ -4076,7 +4073,7 @@
       <c r="B42" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C42" s="38" t="b">
+      <c r="C42" s="35" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4092,9 +4089,9 @@
       <c r="H42" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="L42" s="39"/>
-      <c r="M42" s="40"/>
-      <c r="T42" s="38" t="b">
+      <c r="L42" s="36"/>
+      <c r="M42" s="37"/>
+      <c r="T42" s="35" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4154,487 +4151,487 @@
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="41" width="20.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="38" width="27.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="38" width="15.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="38" width="31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="39" width="20.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="38" width="19.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="38" width="12.14"/>
   </cols>
   <sheetData>
-    <row r="1" s="44" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="42" t="s">
+    <row r="1" s="42" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="40" t="s">
         <v>219</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="40" t="s">
         <v>220</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="41" t="s">
         <v>221</v>
       </c>
-      <c r="E1" s="42" t="s">
+      <c r="E1" s="40" t="s">
         <v>222</v>
       </c>
-      <c r="F1" s="42" t="s">
+      <c r="F1" s="40" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="43" t="s">
         <v>224</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45" t="s">
+      <c r="B2" s="43"/>
+      <c r="C2" s="43" t="s">
         <v>225</v>
       </c>
-      <c r="D2" s="46" t="s">
+      <c r="D2" s="44" t="s">
         <v>226</v>
       </c>
-      <c r="E2" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="F2" s="45"/>
+      <c r="E2" s="43" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="43"/>
     </row>
     <row r="3" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45" t="s">
+      <c r="B3" s="43"/>
+      <c r="C3" s="43" t="s">
         <v>225</v>
       </c>
-      <c r="D3" s="46" t="s">
+      <c r="D3" s="44" t="s">
         <v>227</v>
       </c>
-      <c r="E3" s="45" t="n">
+      <c r="E3" s="43" t="n">
         <v>2</v>
       </c>
-      <c r="F3" s="45"/>
+      <c r="F3" s="43"/>
     </row>
     <row r="4" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="43" t="s">
         <v>164</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45" t="s">
+      <c r="B4" s="43"/>
+      <c r="C4" s="43" t="s">
         <v>228</v>
       </c>
-      <c r="D4" s="46" t="s">
+      <c r="D4" s="44" t="s">
         <v>226</v>
       </c>
-      <c r="E4" s="45" t="s">
+      <c r="E4" s="43" t="s">
         <v>229</v>
       </c>
-      <c r="F4" s="45"/>
+      <c r="F4" s="43"/>
     </row>
     <row r="5" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="43" t="s">
         <v>164</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="43" t="s">
         <v>230</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="43" t="s">
         <v>225</v>
       </c>
-      <c r="D5" s="46" t="s">
+      <c r="D5" s="44" t="s">
         <v>226</v>
       </c>
-      <c r="E5" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" s="45"/>
+      <c r="E5" s="43" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="43"/>
     </row>
     <row r="6" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="43" t="s">
         <v>231</v>
       </c>
-      <c r="B6" s="45"/>
-      <c r="C6" s="45" t="s">
+      <c r="B6" s="43"/>
+      <c r="C6" s="43" t="s">
         <v>232</v>
       </c>
-      <c r="D6" s="46" t="s">
+      <c r="D6" s="44" t="s">
         <v>227</v>
       </c>
-      <c r="E6" s="45" t="n">
+      <c r="E6" s="43" t="n">
         <v>3</v>
       </c>
-      <c r="F6" s="45"/>
+      <c r="F6" s="43"/>
     </row>
     <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="43" t="s">
         <v>231</v>
       </c>
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="43" t="s">
         <v>233</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="43" t="s">
         <v>232</v>
       </c>
-      <c r="D7" s="46" t="s">
+      <c r="D7" s="44" t="s">
         <v>234</v>
       </c>
-      <c r="E7" s="45" t="n">
+      <c r="E7" s="43" t="n">
         <v>5</v>
       </c>
-      <c r="F7" s="45"/>
+      <c r="F7" s="43"/>
     </row>
     <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="43" t="s">
         <v>235</v>
       </c>
-      <c r="B8" s="45"/>
-      <c r="C8" s="45" t="s">
+      <c r="B8" s="43"/>
+      <c r="C8" s="43" t="s">
         <v>232</v>
       </c>
-      <c r="D8" s="46" t="s">
+      <c r="D8" s="44" t="s">
         <v>227</v>
       </c>
-      <c r="E8" s="45" t="n">
+      <c r="E8" s="43" t="n">
         <v>4</v>
       </c>
-      <c r="F8" s="45"/>
+      <c r="F8" s="43"/>
     </row>
     <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="43" t="s">
         <v>235</v>
       </c>
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="43" t="s">
         <v>233</v>
       </c>
-      <c r="C9" s="45" t="s">
+      <c r="C9" s="43" t="s">
         <v>232</v>
       </c>
-      <c r="D9" s="46" t="s">
+      <c r="D9" s="44" t="s">
         <v>234</v>
       </c>
-      <c r="E9" s="45" t="n">
+      <c r="E9" s="43" t="n">
         <v>13</v>
       </c>
-      <c r="F9" s="45"/>
+      <c r="F9" s="43"/>
     </row>
     <row r="10" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="43" t="s">
         <v>236</v>
       </c>
-      <c r="B10" s="45"/>
-      <c r="C10" s="45" t="s">
+      <c r="B10" s="43"/>
+      <c r="C10" s="43" t="s">
         <v>232</v>
       </c>
-      <c r="D10" s="46" t="s">
+      <c r="D10" s="44" t="s">
         <v>234</v>
       </c>
-      <c r="E10" s="45" t="n">
+      <c r="E10" s="43" t="n">
         <v>5</v>
       </c>
-      <c r="F10" s="45"/>
+      <c r="F10" s="43"/>
     </row>
     <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="43" t="s">
         <v>119</v>
       </c>
-      <c r="B11" s="45"/>
-      <c r="C11" s="45" t="s">
+      <c r="B11" s="43"/>
+      <c r="C11" s="43" t="s">
         <v>232</v>
       </c>
-      <c r="D11" s="46" t="s">
+      <c r="D11" s="44" t="s">
         <v>227</v>
       </c>
-      <c r="E11" s="45" t="n">
+      <c r="E11" s="43" t="n">
         <v>5</v>
       </c>
-      <c r="F11" s="45"/>
+      <c r="F11" s="43"/>
     </row>
     <row r="12" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="43" t="s">
         <v>158</v>
       </c>
-      <c r="B12" s="45"/>
-      <c r="C12" s="45" t="s">
+      <c r="B12" s="43"/>
+      <c r="C12" s="43" t="s">
         <v>232</v>
       </c>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="44" t="s">
         <v>227</v>
       </c>
-      <c r="E12" s="45" t="n">
+      <c r="E12" s="43" t="n">
         <v>6</v>
       </c>
-      <c r="F12" s="45"/>
+      <c r="F12" s="43"/>
     </row>
     <row r="13" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="43" t="s">
         <v>237</v>
       </c>
-      <c r="B13" s="45"/>
-      <c r="C13" s="45" t="s">
+      <c r="B13" s="43"/>
+      <c r="C13" s="43" t="s">
         <v>232</v>
       </c>
-      <c r="D13" s="46" t="s">
+      <c r="D13" s="44" t="s">
         <v>227</v>
       </c>
-      <c r="E13" s="45" t="n">
+      <c r="E13" s="43" t="n">
         <v>11</v>
       </c>
-      <c r="F13" s="45"/>
+      <c r="F13" s="43"/>
     </row>
     <row r="14" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="45" t="s">
+      <c r="A14" s="43" t="s">
         <v>124</v>
       </c>
-      <c r="B14" s="45"/>
-      <c r="C14" s="45" t="s">
+      <c r="B14" s="43"/>
+      <c r="C14" s="43" t="s">
         <v>232</v>
       </c>
-      <c r="D14" s="46" t="s">
+      <c r="D14" s="44" t="s">
         <v>227</v>
       </c>
-      <c r="E14" s="45" t="n">
+      <c r="E14" s="43" t="n">
         <v>14</v>
       </c>
-      <c r="F14" s="45"/>
+      <c r="F14" s="43"/>
     </row>
     <row r="15" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="45" t="s">
+      <c r="A15" s="43" t="s">
         <v>135</v>
       </c>
-      <c r="B15" s="45"/>
-      <c r="C15" s="45" t="s">
+      <c r="B15" s="43"/>
+      <c r="C15" s="43" t="s">
         <v>232</v>
       </c>
-      <c r="D15" s="46" t="s">
+      <c r="D15" s="44" t="s">
         <v>234</v>
       </c>
-      <c r="E15" s="45" t="n">
+      <c r="E15" s="43" t="n">
         <v>15</v>
       </c>
-      <c r="F15" s="45"/>
+      <c r="F15" s="43"/>
     </row>
     <row r="16" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="45" t="s">
+      <c r="A16" s="43" t="s">
         <v>135</v>
       </c>
-      <c r="B16" s="45"/>
-      <c r="C16" s="45" t="s">
+      <c r="B16" s="43"/>
+      <c r="C16" s="43" t="s">
         <v>232</v>
       </c>
-      <c r="D16" s="46" t="s">
+      <c r="D16" s="44" t="s">
         <v>238</v>
       </c>
-      <c r="E16" s="45" t="s">
+      <c r="E16" s="43" t="s">
         <v>239</v>
       </c>
-      <c r="F16" s="45"/>
+      <c r="F16" s="43"/>
     </row>
     <row r="17" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="45" t="s">
+      <c r="A17" s="43" t="s">
         <v>240</v>
       </c>
-      <c r="B17" s="45"/>
-      <c r="C17" s="45" t="s">
+      <c r="B17" s="43"/>
+      <c r="C17" s="43" t="s">
         <v>232</v>
       </c>
-      <c r="D17" s="46" t="s">
+      <c r="D17" s="44" t="s">
         <v>227</v>
       </c>
-      <c r="E17" s="45" t="n">
+      <c r="E17" s="43" t="n">
         <v>15</v>
       </c>
-      <c r="F17" s="45"/>
+      <c r="F17" s="43"/>
     </row>
     <row r="18" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="45" t="s">
+      <c r="A18" s="43" t="s">
         <v>130</v>
       </c>
-      <c r="B18" s="45"/>
-      <c r="C18" s="45" t="s">
+      <c r="B18" s="43"/>
+      <c r="C18" s="43" t="s">
         <v>232</v>
       </c>
-      <c r="D18" s="46" t="s">
+      <c r="D18" s="44" t="s">
         <v>227</v>
       </c>
-      <c r="E18" s="45" t="n">
+      <c r="E18" s="43" t="n">
         <v>16</v>
       </c>
-      <c r="F18" s="45"/>
+      <c r="F18" s="43"/>
     </row>
     <row r="19" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="45" t="s">
+      <c r="A19" s="43" t="s">
         <v>241</v>
       </c>
-      <c r="B19" s="45"/>
-      <c r="C19" s="45" t="s">
+      <c r="B19" s="43"/>
+      <c r="C19" s="43" t="s">
         <v>232</v>
       </c>
-      <c r="D19" s="46" t="s">
+      <c r="D19" s="44" t="s">
         <v>227</v>
       </c>
-      <c r="E19" s="45" t="n">
+      <c r="E19" s="43" t="n">
         <v>40</v>
       </c>
-      <c r="F19" s="45"/>
+      <c r="F19" s="43"/>
     </row>
     <row r="20" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="45" t="s">
+      <c r="A20" s="43" t="s">
         <v>152</v>
       </c>
-      <c r="B20" s="45"/>
-      <c r="C20" s="45" t="s">
+      <c r="B20" s="43"/>
+      <c r="C20" s="43" t="s">
         <v>242</v>
       </c>
-      <c r="D20" s="46" t="s">
+      <c r="D20" s="44" t="s">
         <v>226</v>
       </c>
-      <c r="E20" s="45" t="s">
+      <c r="E20" s="43" t="s">
         <v>229</v>
       </c>
-      <c r="F20" s="45"/>
+      <c r="F20" s="43"/>
     </row>
     <row r="21" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="38" t="s">
         <v>169</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="D21" s="46" t="s">
+      <c r="D21" s="44" t="s">
         <v>226</v>
       </c>
-      <c r="E21" s="41" t="s">
+      <c r="E21" s="39" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="38" t="s">
         <v>169</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="38" t="s">
         <v>230</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="D22" s="46" t="s">
+      <c r="D22" s="44" t="s">
         <v>226</v>
       </c>
-      <c r="E22" s="41" t="s">
+      <c r="E22" s="39" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="38" t="s">
         <v>169</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="38" t="s">
         <v>230</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="D23" s="46" t="s">
+      <c r="D23" s="44" t="s">
         <v>226</v>
       </c>
-      <c r="E23" s="41" t="s">
+      <c r="E23" s="39" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="C24" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="D24" s="46" t="s">
+      <c r="D24" s="44" t="s">
         <v>226</v>
       </c>
-      <c r="E24" s="41" t="s">
+      <c r="E24" s="39" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="38" t="s">
         <v>230</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="C25" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="D25" s="46" t="s">
+      <c r="D25" s="44" t="s">
         <v>226</v>
       </c>
-      <c r="E25" s="41" t="s">
+      <c r="E25" s="39" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="38" t="s">
         <v>230</v>
       </c>
-      <c r="C26" s="0" t="s">
+      <c r="C26" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="D26" s="46" t="s">
+      <c r="D26" s="44" t="s">
         <v>226</v>
       </c>
-      <c r="E26" s="41" t="s">
+      <c r="E26" s="39" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="38" t="s">
         <v>180</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="C27" s="38" t="s">
         <v>249</v>
       </c>
-      <c r="D27" s="46" t="s">
+      <c r="D27" s="44" t="s">
         <v>226</v>
       </c>
-      <c r="E27" s="0" t="s">
+      <c r="E27" s="38" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="38" t="s">
         <v>180</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="38" t="s">
         <v>230</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="C28" s="38" t="s">
         <v>249</v>
       </c>
-      <c r="D28" s="46" t="s">
+      <c r="D28" s="44" t="s">
         <v>226</v>
       </c>
-      <c r="E28" s="0" t="s">
+      <c r="E28" s="38" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="38" t="s">
         <v>180</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="38" t="s">
         <v>230</v>
       </c>
-      <c r="C29" s="0" t="s">
+      <c r="C29" s="38" t="s">
         <v>249</v>
       </c>
-      <c r="D29" s="46" t="s">
+      <c r="D29" s="44" t="s">
         <v>226</v>
       </c>
-      <c r="E29" s="0" t="s">
+      <c r="E29" s="38" t="s">
         <v>252</v>
       </c>
     </row>
@@ -4660,118 +4657,118 @@
       <selection pane="topLeft" activeCell="L15" activeCellId="0" sqref="L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.71484375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="45" width="10.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="45" width="12.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="45" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="45" width="12.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="45" width="10.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="45" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="45" width="15.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="9" style="45" width="10.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="43" width="10.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="43" width="12.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="43" width="13.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="43" width="12.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="43" width="10.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="43" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="43" width="15.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="9" style="43" width="10.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="46" t="s">
         <v>253</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="45" t="s">
         <v>254</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="45" t="s">
         <v>255</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="45" t="s">
         <v>256</v>
       </c>
-      <c r="F1" s="47" t="s">
+      <c r="F1" s="45" t="s">
         <v>257</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="H1" s="47" t="s">
+      <c r="H1" s="45" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="43" t="s">
         <v>260</v>
       </c>
-      <c r="C2" s="45" t="s">
+      <c r="C2" s="43" t="s">
         <v>261</v>
       </c>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="43" t="s">
         <v>262</v>
       </c>
-      <c r="E2" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F2" s="49" t="b">
+      <c r="E2" s="47" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="47" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G2" s="49" t="b">
+      <c r="G2" s="47" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="43" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="43" t="s">
         <v>263</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="43" t="s">
         <v>264</v>
       </c>
-      <c r="D3" s="45" t="s">
+      <c r="D3" s="43" t="s">
         <v>265</v>
       </c>
-      <c r="E3" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F3" s="49" t="b">
+      <c r="E3" s="47" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F3" s="47" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G3" s="49" t="b">
+      <c r="G3" s="47" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="43" t="s">
         <v>216</v>
       </c>
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="43" t="s">
         <v>266</v>
       </c>
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="43" t="s">
         <v>267</v>
       </c>
-      <c r="D4" s="45" t="s">
+      <c r="D4" s="43" t="s">
         <v>268</v>
       </c>
-      <c r="E4" s="49" t="b">
+      <c r="E4" s="47" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F4" s="49" t="b">
+      <c r="F4" s="47" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G4" s="49" t="b">
+      <c r="G4" s="47" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4798,33 +4795,33 @@
       <selection pane="topLeft" activeCell="A45" activeCellId="0" sqref="A45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="50" width="21.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="50" width="15.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="50" width="23.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="50" width="19.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="50" width="24.29"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="7" style="50" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="48" width="21.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="48" width="15.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="48" width="23.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="48" width="19.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="48" width="24.29"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="7" style="48" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="49" t="s">
         <v>269</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="49" t="s">
         <v>222</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="49" t="s">
         <v>270</v>
       </c>
-      <c r="F1" s="51" t="s">
+      <c r="F1" s="49" t="s">
         <v>12</v>
       </c>
     </row>
@@ -5543,44 +5540,44 @@
       <c r="F48" s="1"/>
     </row>
     <row r="49" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="50" t="s">
+      <c r="A49" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="B49" s="50" t="s">
+      <c r="B49" s="48" t="s">
         <v>250</v>
       </c>
-      <c r="C49" s="50" t="s">
+      <c r="C49" s="48" t="s">
         <v>363</v>
       </c>
-      <c r="D49" s="50" t="s">
+      <c r="D49" s="48" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="50" t="s">
+      <c r="A50" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="B50" s="50" t="s">
+      <c r="B50" s="48" t="s">
         <v>251</v>
       </c>
-      <c r="C50" s="50" t="s">
+      <c r="C50" s="48" t="s">
         <v>364</v>
       </c>
-      <c r="D50" s="50" t="s">
+      <c r="D50" s="48" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="50" t="s">
+      <c r="A51" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="B51" s="50" t="s">
+      <c r="B51" s="48" t="s">
         <v>360</v>
       </c>
-      <c r="C51" s="50" t="s">
+      <c r="C51" s="48" t="s">
         <v>366</v>
       </c>
-      <c r="D51" s="50" t="s">
+      <c r="D51" s="48" t="s">
         <v>367</v>
       </c>
     </row>
@@ -5606,55 +5603,55 @@
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="38" width="18.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="38" width="17.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="38" width="13.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="38" width="12.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="38" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="38" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="38" width="14.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="38" width="11.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="38" width="13.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="38" width="14.43"/>
   </cols>
   <sheetData>
-    <row r="1" s="51" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="52" t="s">
+    <row r="1" s="49" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="50" t="s">
         <v>368</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="50" t="s">
         <v>369</v>
       </c>
-      <c r="C1" s="52" t="s">
+      <c r="C1" s="50" t="s">
         <v>370</v>
       </c>
-      <c r="D1" s="52" t="s">
+      <c r="D1" s="50" t="s">
         <v>371</v>
       </c>
-      <c r="E1" s="52" t="s">
+      <c r="E1" s="50" t="s">
         <v>372</v>
       </c>
-      <c r="F1" s="52" t="s">
+      <c r="F1" s="50" t="s">
         <v>373</v>
       </c>
-      <c r="G1" s="52" t="s">
+      <c r="G1" s="50" t="s">
         <v>374</v>
       </c>
-      <c r="H1" s="52" t="s">
+      <c r="H1" s="50" t="s">
         <v>375</v>
       </c>
-      <c r="I1" s="52" t="s">
+      <c r="I1" s="50" t="s">
         <v>376</v>
       </c>
-      <c r="J1" s="52" t="s">
+      <c r="J1" s="50" t="s">
         <v>377</v>
       </c>
-      <c r="K1" s="52" t="s">
+      <c r="K1" s="50" t="s">
         <v>378</v>
       </c>
-      <c r="L1" s="51" t="s">
+      <c r="L1" s="49" t="s">
         <v>379</v>
       </c>
     </row>
@@ -5674,28 +5671,56 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="0" width="28.55"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="38"/>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="51" t="s">
         <v>380</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="C2" s="51" t="s">
         <v>381</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D2" s="51" t="s">
         <v>382</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E2" s="51" t="s">
         <v>383</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F2" s="51" t="s">
         <v>384</v>
       </c>
     </row>

</xml_diff>